<commit_message>
Update with Test#3 results
</commit_message>
<xml_diff>
--- a/Tablut/TestTablut.xlsx
+++ b/Tablut/TestTablut.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolobartelucci/MyFiles/Projects/Tablut/Tablut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8779CDFC-216A-4C6F-BD78-E741B279586A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0F666A-73B0-2641-8103-745FEAB60C75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
   <si>
     <t>KingEncirclement</t>
   </si>
@@ -80,9 +80,6 @@
     <t>TEST #3</t>
   </si>
   <si>
-    <t xml:space="preserve">RESULT: </t>
-  </si>
-  <si>
     <t>NOTE</t>
   </si>
   <si>
@@ -90,13 +87,19 @@
   </si>
   <si>
     <t>Partita molto lunga visto che il bianco è molto difensivo</t>
+  </si>
+  <si>
+    <t>RESULT: BLACK WIN (BUT WHITE WON ONCE)</t>
+  </si>
+  <si>
+    <t>Situazione strana, ho fatto il test 2 volte e la prima volta ha vinto il bianco, la seocnda il nero. L'unica mossa cambiata è una dalla parte del nero, probabilmente le due mosse pesavano uguali. GG al bianco comunque</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +143,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="7">
@@ -358,6 +366,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -373,23 +418,29 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -397,22 +448,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -425,50 +466,17 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="40% - Colore 1" xfId="1" builtinId="31"/>
-    <cellStyle name="60% - Colore 2" xfId="2" builtinId="36"/>
-    <cellStyle name="60% - Colore 3" xfId="3" builtinId="40"/>
-    <cellStyle name="60% - Colore 4" xfId="4" builtinId="44"/>
-    <cellStyle name="60% - Colore 6" xfId="5" builtinId="52"/>
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
+    <cellStyle name="60% - Accent3" xfId="3" builtinId="40"/>
+    <cellStyle name="60% - Accent4" xfId="4" builtinId="44"/>
+    <cellStyle name="60% - Accent6" xfId="5" builtinId="52"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -484,7 +492,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -786,91 +794,91 @@
       <selection activeCell="G25" sqref="G25:K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:17" ht="21">
+      <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="14"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="13"/>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="24" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="21"/>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="22" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="22" t="s">
+      <c r="E3" s="33"/>
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="29"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="G3" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17">
+      <c r="B4" s="31"/>
+      <c r="C4" s="4">
         <v>0.1</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17">
+      <c r="E4" s="31"/>
+      <c r="F4" s="4">
         <v>0.1</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="32"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="27"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -878,26 +886,26 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:17">
+      <c r="A5" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17">
+      <c r="B5" s="31"/>
+      <c r="C5" s="4">
         <v>0.2</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17">
+      <c r="E5" s="31"/>
+      <c r="F5" s="4">
         <v>0.2</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="32"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="27"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -905,26 +913,26 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:17">
+      <c r="A6" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="3">
         <v>0.4</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="19"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="3">
         <v>0.4</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="32"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="27"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -932,26 +940,26 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:17">
+      <c r="A7" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17">
+      <c r="B7" s="31"/>
+      <c r="C7" s="4">
         <v>0.5</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17">
+      <c r="E7" s="31"/>
+      <c r="F7" s="4">
         <v>1</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="32"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="27"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -959,22 +967,22 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:17">
+      <c r="A8" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17">
+      <c r="B8" s="31"/>
+      <c r="C8" s="4">
         <v>1</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="32"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="27"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -982,22 +990,22 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:17">
+      <c r="A9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="2">
         <v>0</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="32"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="27"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1005,20 +1013,20 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:17" ht="19">
+      <c r="A10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="11"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="16"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1026,7 +1034,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1037,20 +1045,20 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="12" t="s">
+    <row r="12" spans="1:17" ht="21">
+      <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="14"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="13"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -1058,24 +1066,24 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:17">
+      <c r="A13" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="6" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="8"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="21"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -1083,28 +1091,28 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+    <row r="14" spans="1:17">
+      <c r="A14" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22" t="s">
+      <c r="B14" s="33"/>
+      <c r="C14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="22" t="s">
+      <c r="E14" s="33"/>
+      <c r="F14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="29"/>
+      <c r="G14" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="24"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -1112,26 +1120,26 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+    <row r="15" spans="1:17">
+      <c r="A15" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17">
+      <c r="B15" s="31"/>
+      <c r="C15" s="4">
         <v>0.1</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17">
+      <c r="E15" s="31"/>
+      <c r="F15" s="4">
         <v>0.1</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="32"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="27"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1139,26 +1147,26 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+    <row r="16" spans="1:17">
+      <c r="A16" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17">
+      <c r="B16" s="31"/>
+      <c r="C16" s="4">
         <v>0.2</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17">
+      <c r="E16" s="31"/>
+      <c r="F16" s="4">
         <v>0.2</v>
       </c>
-      <c r="G16" s="30"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="32"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="27"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -1166,26 +1174,26 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:17">
+      <c r="A17" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="19"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="3">
         <v>0.5</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="19"/>
+      <c r="E17" s="29"/>
       <c r="F17" s="3">
         <v>0.4</v>
       </c>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="32"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="27"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -1193,26 +1201,26 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+    <row r="18" spans="1:17">
+      <c r="A18" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17">
+      <c r="B18" s="31"/>
+      <c r="C18" s="4">
         <v>0.3</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="17">
+      <c r="E18" s="31"/>
+      <c r="F18" s="4">
         <v>1</v>
       </c>
-      <c r="G18" s="30"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="32"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="27"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1220,22 +1228,22 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+    <row r="19" spans="1:17">
+      <c r="A19" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17">
+      <c r="B19" s="31"/>
+      <c r="C19" s="4">
         <v>1</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="32"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="27"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -1243,22 +1251,22 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:17">
+      <c r="A20" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="2">
         <v>0.7</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="5"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="32"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="27"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -1266,20 +1274,20 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:17" ht="19">
+      <c r="A21" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="11"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="16"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1287,7 +1295,7 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17">
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -1298,20 +1306,20 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A23" s="12" t="s">
+    <row r="23" spans="1:17" ht="21">
+      <c r="A23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="14"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="13"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1319,24 +1327,24 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+    <row r="24" spans="1:17">
+      <c r="A24" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="24" t="s">
+      <c r="B24" s="36"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="26"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="37"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -1344,26 +1352,28 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+    <row r="25" spans="1:17">
+      <c r="A25" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="22" t="s">
+      <c r="B25" s="33"/>
+      <c r="C25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="22" t="s">
+      <c r="E25" s="33"/>
+      <c r="F25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="33"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="35"/>
+      <c r="G25" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="7"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -1371,26 +1381,26 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+    <row r="26" spans="1:17">
+      <c r="A26" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="17">
+      <c r="B26" s="31"/>
+      <c r="C26" s="4">
         <v>0.1</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="17">
+      <c r="E26" s="31"/>
+      <c r="F26" s="4">
         <v>0.1</v>
       </c>
-      <c r="G26" s="36"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="38"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="10"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -1398,26 +1408,26 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+    <row r="27" spans="1:17">
+      <c r="A27" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17">
+      <c r="B27" s="31"/>
+      <c r="C27" s="4">
         <v>0.2</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="16"/>
-      <c r="F27" s="17">
+      <c r="E27" s="31"/>
+      <c r="F27" s="4">
         <v>0.2</v>
       </c>
-      <c r="G27" s="36"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="38"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="10"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
@@ -1425,26 +1435,26 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
+    <row r="28" spans="1:17">
+      <c r="A28" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="19"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="3">
         <v>0.6</v>
       </c>
-      <c r="D28" s="18" t="s">
+      <c r="D28" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E28" s="19"/>
+      <c r="E28" s="29"/>
       <c r="F28" s="3">
         <v>0.4</v>
       </c>
-      <c r="G28" s="36"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="38"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="10"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
@@ -1452,26 +1462,26 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
+    <row r="29" spans="1:17">
+      <c r="A29" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="17">
+      <c r="B29" s="31"/>
+      <c r="C29" s="4">
         <v>0</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="16"/>
-      <c r="F29" s="17">
+      <c r="E29" s="31"/>
+      <c r="F29" s="4">
         <v>1</v>
       </c>
-      <c r="G29" s="36"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="38"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="10"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
@@ -1479,22 +1489,22 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+    <row r="30" spans="1:17">
+      <c r="A30" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="17">
+      <c r="B30" s="31"/>
+      <c r="C30" s="4">
         <v>1.2</v>
       </c>
-      <c r="D30" s="15"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="38"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="10"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
@@ -1502,22 +1512,22 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:17">
+      <c r="A31" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="5"/>
+      <c r="B31" s="18"/>
       <c r="C31" s="2">
         <v>0.4</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="5"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="18"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="38"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="10"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
@@ -1525,20 +1535,20 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="11"/>
+    <row r="32" spans="1:17" ht="19">
+      <c r="A32" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="16"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
@@ -1546,7 +1556,7 @@
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="9:17">
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -1557,7 +1567,7 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="9:17">
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -1568,7 +1578,7 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="9:17">
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -1579,7 +1589,7 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
     </row>
-    <row r="36" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="9:17">
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -1590,7 +1600,7 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="9:17">
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -1601,7 +1611,7 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="9:17">
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -1614,48 +1624,8 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="G25:K31"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A32:K32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="G3:K9"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K20"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="D2:F2"/>
@@ -1672,8 +1642,48 @@
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="G3:K9"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="G25:K31"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A32:K32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K20"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add new tests including a winning one for the White Player after the increase by 0.2 of the PawnDifference Heuristic Element in WhiteHeristic class
</commit_message>
<xml_diff>
--- a/Tablut/TestTablut.xlsx
+++ b/Tablut/TestTablut.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolobartelucci/MyFiles/Projects/Tablut/Tablut/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\Tablut\Tablut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0F666A-73B0-2641-8103-745FEAB60C75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB2087F-41E5-4E77-8FC9-5B45A7C39DBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="26">
   <si>
     <t>KingEncirclement</t>
   </si>
@@ -93,6 +93,24 @@
   </si>
   <si>
     <t>Situazione strana, ho fatto il test 2 volte e la prima volta ha vinto il bianco, la seocnda il nero. L'unica mossa cambiata è una dalla parte del nero, probabilmente le due mosse pesavano uguali. GG al bianco comunque</t>
+  </si>
+  <si>
+    <t>TEST #4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il Black ha vinto in poco tempo tentativo di valutare l'impatto della BlackManhattanD non andato a buon fine, il re si è spostato quasi subito nel quadrate in alto a sx per poi essere mangiato da due neri up &amp; down </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESULT: BLACK WIN </t>
+  </si>
+  <si>
+    <t>TEST #5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESULT: WHITE WIN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il White si è comportato bene per quasi tutta la partita ovviamente è più aggressivo visto l'aumento del PawnsDifference è riuscito a vincere dopo una mezz'ora di gioco          Anche al secondo tentativo si è comportato allo stesso modo   </t>
   </si>
 </sst>
 </file>
@@ -370,6 +388,90 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -385,98 +487,14 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
-    <cellStyle name="60% - Accent3" xfId="3" builtinId="40"/>
-    <cellStyle name="60% - Accent4" xfId="4" builtinId="44"/>
-    <cellStyle name="60% - Accent6" xfId="5" builtinId="52"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Colore 1" xfId="1" builtinId="31"/>
+    <cellStyle name="60% - Colore 2" xfId="2" builtinId="36"/>
+    <cellStyle name="60% - Colore 3" xfId="3" builtinId="40"/>
+    <cellStyle name="60% - Colore 4" xfId="4" builtinId="44"/>
+    <cellStyle name="60% - Colore 6" xfId="5" builtinId="52"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -492,7 +510,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -788,97 +806,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{028B81F1-ACA3-4C72-9A53-A89403C903EE}">
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25:K31"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:K54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="13"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="23"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="35" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="19" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="21"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="12"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="33"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="24"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="26"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="31"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="4">
         <v>0.1</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="4">
         <v>0.1</v>
       </c>
-      <c r="G4" s="25"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="29"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -887,25 +905,25 @@
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="31"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="4">
         <v>0.2</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="17"/>
       <c r="F5" s="4">
         <v>0.2</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="29"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -914,25 +932,25 @@
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="29"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="3">
         <v>0.4</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="29"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="3">
         <v>0.4</v>
       </c>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="29"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -941,25 +959,25 @@
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="31"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="4">
         <v>0.5</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="17"/>
       <c r="F7" s="4">
         <v>1</v>
       </c>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="29"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -968,21 +986,21 @@
       <c r="Q7" s="1"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="31"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="4">
         <v>1</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="31"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="29"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -991,21 +1009,21 @@
       <c r="Q8" s="1"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="18"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="2">
         <v>0</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="18"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="29"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1013,20 +1031,20 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" ht="19">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:17" ht="18.75">
+      <c r="A10" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="16"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="32"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1046,19 +1064,19 @@
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:17" ht="21">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="13"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="23"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -1067,23 +1085,23 @@
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="19" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="19" t="s">
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="21"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="12"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -1092,27 +1110,27 @@
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="33"/>
+      <c r="B14" s="7"/>
       <c r="C14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="33"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="24"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="26"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -1121,25 +1139,25 @@
       <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="31"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="4">
         <v>0.1</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="31"/>
+      <c r="E15" s="17"/>
       <c r="F15" s="4">
         <v>0.1</v>
       </c>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="29"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1148,25 +1166,25 @@
       <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="31"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="4">
         <v>0.2</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="31"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="4">
         <v>0.2</v>
       </c>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="29"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -1175,25 +1193,25 @@
       <c r="Q16" s="1"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="29"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="3">
         <v>0.5</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="29"/>
+      <c r="E17" s="19"/>
       <c r="F17" s="3">
         <v>0.4</v>
       </c>
-      <c r="G17" s="25"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="29"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -1202,25 +1220,25 @@
       <c r="Q17" s="1"/>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="31"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="4">
         <v>0.3</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="31"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="4">
         <v>1</v>
       </c>
-      <c r="G18" s="25"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="29"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1229,21 +1247,21 @@
       <c r="Q18" s="1"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="31"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="4">
         <v>1</v>
       </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="31"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="29"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -1252,21 +1270,21 @@
       <c r="Q19" s="1"/>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="18"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="2">
         <v>0.7</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="18"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="29"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -1274,20 +1292,20 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:17" ht="19">
-      <c r="A21" s="14" t="s">
+    <row r="21" spans="1:17" ht="18.75">
+      <c r="A21" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="16"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="32"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1307,19 +1325,19 @@
       <c r="Q22" s="1"/>
     </row>
     <row r="23" spans="1:17" ht="21">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="13"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="23"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1328,23 +1346,23 @@
       <c r="Q23" s="1"/>
     </row>
     <row r="24" spans="1:17">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="35" t="s">
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="36"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="35" t="s">
+      <c r="E24" s="14"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="37"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="15"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -1353,27 +1371,27 @@
       <c r="Q24" s="1"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="33"/>
+      <c r="B25" s="7"/>
       <c r="C25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="32" t="s">
+      <c r="D25" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="33"/>
+      <c r="E25" s="7"/>
       <c r="F25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="38" t="s">
+      <c r="G25" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="7"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="35"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -1382,25 +1400,25 @@
       <c r="Q25" s="1"/>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="31"/>
+      <c r="B26" s="17"/>
       <c r="C26" s="4">
         <v>0.1</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="D26" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="31"/>
+      <c r="E26" s="17"/>
       <c r="F26" s="4">
         <v>0.1</v>
       </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="10"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="38"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -1409,25 +1427,25 @@
       <c r="Q26" s="1"/>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="31"/>
+      <c r="B27" s="17"/>
       <c r="C27" s="4">
         <v>0.2</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="D27" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="31"/>
+      <c r="E27" s="17"/>
       <c r="F27" s="4">
         <v>0.2</v>
       </c>
-      <c r="G27" s="8"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="10"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="38"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
@@ -1436,25 +1454,25 @@
       <c r="Q27" s="1"/>
     </row>
     <row r="28" spans="1:17">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="29"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="3">
         <v>0.6</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E28" s="29"/>
+      <c r="E28" s="19"/>
       <c r="F28" s="3">
         <v>0.4</v>
       </c>
-      <c r="G28" s="8"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="10"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="38"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
@@ -1463,25 +1481,25 @@
       <c r="Q28" s="1"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="31"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="4">
         <v>0</v>
       </c>
-      <c r="D29" s="30" t="s">
+      <c r="D29" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="31"/>
+      <c r="E29" s="17"/>
       <c r="F29" s="4">
         <v>1</v>
       </c>
-      <c r="G29" s="8"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="10"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="38"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
@@ -1490,21 +1508,21 @@
       <c r="Q29" s="1"/>
     </row>
     <row r="30" spans="1:17">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="31"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="4">
         <v>1.2</v>
       </c>
-      <c r="D30" s="30"/>
-      <c r="E30" s="31"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="17"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="10"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="38"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
@@ -1513,21 +1531,21 @@
       <c r="Q30" s="1"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="18"/>
+      <c r="B31" s="9"/>
       <c r="C31" s="2">
         <v>0.4</v>
       </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="18"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="9"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="10"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="38"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
@@ -1535,20 +1553,20 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="1:17" ht="19">
-      <c r="A32" s="14" t="s">
+    <row r="32" spans="1:17" ht="18.75">
+      <c r="A32" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="16"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="32"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
@@ -1556,7 +1574,7 @@
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="9:17">
+    <row r="33" spans="1:17">
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -1567,10 +1585,20 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="9:17">
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
+    <row r="34" spans="1:17" ht="21">
+      <c r="A34" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="23"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
@@ -1578,10 +1606,24 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="9:17">
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
+    <row r="35" spans="1:17">
+      <c r="A35" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="14"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="14"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="15"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
@@ -1589,10 +1631,28 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
     </row>
-    <row r="36" spans="9:17">
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
+    <row r="36" spans="1:17">
+      <c r="A36" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="F36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="34"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="35"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
@@ -1600,10 +1660,26 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="9:17">
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
+    <row r="37" spans="1:17">
+      <c r="A37" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="17"/>
+      <c r="C37" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="17"/>
+      <c r="F37" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G37" s="36"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="38"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
@@ -1611,10 +1687,26 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="9:17">
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
+    <row r="38" spans="1:17">
+      <c r="A38" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="17"/>
+      <c r="C38" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="17"/>
+      <c r="F38" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G38" s="36"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="38"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
@@ -1622,8 +1714,373 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
     </row>
+    <row r="39" spans="1:17">
+      <c r="A39" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="19"/>
+      <c r="C39" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="19"/>
+      <c r="F39" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G39" s="36"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="38"/>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="A40" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="17"/>
+      <c r="C40" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="17"/>
+      <c r="F40" s="4">
+        <v>1</v>
+      </c>
+      <c r="G40" s="36"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="38"/>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="A41" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="17"/>
+      <c r="C41" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="D41" s="16"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="38"/>
+    </row>
+    <row r="42" spans="1:17">
+      <c r="A42" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="38"/>
+    </row>
+    <row r="43" spans="1:17" ht="18.75">
+      <c r="A43" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="31"/>
+      <c r="K43" s="32"/>
+    </row>
+    <row r="45" spans="1:17" ht="21">
+      <c r="A45" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="23"/>
+    </row>
+    <row r="46" spans="1:17">
+      <c r="A46" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="14"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="14"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="15"/>
+    </row>
+    <row r="47" spans="1:17">
+      <c r="A47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="7"/>
+      <c r="C47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="7"/>
+      <c r="F47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G47" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="H47" s="34"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="34"/>
+      <c r="K47" s="35"/>
+    </row>
+    <row r="48" spans="1:17">
+      <c r="A48" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="17"/>
+      <c r="C48" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" s="17"/>
+      <c r="F48" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G48" s="36"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="37"/>
+      <c r="J48" s="37"/>
+      <c r="K48" s="38"/>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="17"/>
+      <c r="C49" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="17"/>
+      <c r="F49" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G49" s="36"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="38"/>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" s="19"/>
+      <c r="C50" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="19"/>
+      <c r="F50" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G50" s="36"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="37"/>
+      <c r="J50" s="37"/>
+      <c r="K50" s="38"/>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="17"/>
+      <c r="C51" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="17"/>
+      <c r="F51" s="4">
+        <v>1</v>
+      </c>
+      <c r="G51" s="36"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="37"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="38"/>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="17"/>
+      <c r="C52" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="D52" s="16"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="36"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="37"/>
+      <c r="J52" s="37"/>
+      <c r="K52" s="38"/>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="9"/>
+      <c r="C53" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D53" s="8"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="36"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="37"/>
+      <c r="K53" s="38"/>
+    </row>
+    <row r="54" spans="1:11" ht="18.75">
+      <c r="A54" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54" s="31"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="31"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="31"/>
+      <c r="J54" s="31"/>
+      <c r="K54" s="32"/>
+    </row>
   </sheetData>
-  <mergeCells count="60">
+  <mergeCells count="100">
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="A54:K54"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="G46:K46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="G47:K53"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A45:K45"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:K42"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="G25:K31"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A32:K32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K20"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="G3:K9"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:E16"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A13:C13"/>
@@ -1640,50 +2097,6 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="G3:K9"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="G25:K31"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A32:K32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K20"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add test#6, fix wrong black weight values
</commit_message>
<xml_diff>
--- a/Tablut/TestTablut.xlsx
+++ b/Tablut/TestTablut.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\Tablut\Tablut\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolobartelucci/MyFiles/Projects/Tablut/Tablut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB2087F-41E5-4E77-8FC9-5B45A7C39DBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198CCEB6-3F09-0F44-82BB-4EC7BBA14A41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
+    <workbookView xWindow="0" yWindow="580" windowWidth="26660" windowHeight="16740" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="28">
   <si>
     <t>KingEncirclement</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t xml:space="preserve">Il White si è comportato bene per quasi tutta la partita ovviamente è più aggressivo visto l'aumento del PawnsDifference è riuscito a vincere dopo una mezz'ora di gioco          Anche al secondo tentativo si è comportato allo stesso modo   </t>
+  </si>
+  <si>
+    <t>TEST #6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESULT: </t>
   </si>
 </sst>
 </file>
@@ -388,17 +394,77 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -409,39 +475,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -460,41 +493,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="40% - Colore 1" xfId="1" builtinId="31"/>
-    <cellStyle name="60% - Colore 2" xfId="2" builtinId="36"/>
-    <cellStyle name="60% - Colore 3" xfId="3" builtinId="40"/>
-    <cellStyle name="60% - Colore 4" xfId="4" builtinId="44"/>
-    <cellStyle name="60% - Colore 6" xfId="5" builtinId="52"/>
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
+    <cellStyle name="60% - Accent3" xfId="3" builtinId="40"/>
+    <cellStyle name="60% - Accent4" xfId="4" builtinId="44"/>
+    <cellStyle name="60% - Accent6" xfId="5" builtinId="52"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -510,7 +516,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -806,97 +812,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{028B81F1-ACA3-4C72-9A53-A89403C903EE}">
-  <dimension ref="A1:Q54"/>
+  <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:K54"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58:K64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="23"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="29"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="13" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="10" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="12"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="15"/>
       <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="26"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="35"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="4">
         <v>0.1</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="17"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="29"/>
+        <v>0.2</v>
+      </c>
+      <c r="G4" s="36"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="38"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -905,25 +911,25 @@
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="17"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="4">
         <v>0.2</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="17"/>
+      <c r="E5" s="23"/>
       <c r="F5" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="29"/>
+        <v>0.6</v>
+      </c>
+      <c r="G5" s="36"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="38"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -932,25 +938,25 @@
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="3">
         <v>0.4</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="19"/>
+      <c r="E6" s="26"/>
       <c r="F6" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="29"/>
+        <v>1.5</v>
+      </c>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="38"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -959,25 +965,25 @@
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="17"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="4">
         <v>0.5</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="17"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="4">
-        <v>1</v>
-      </c>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="29"/>
+        <v>2</v>
+      </c>
+      <c r="G7" s="36"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="38"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -986,21 +992,21 @@
       <c r="Q7" s="1"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="17"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="4">
         <v>1</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="23"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="29"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="38"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1009,21 +1015,21 @@
       <c r="Q8" s="1"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="9"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="2">
         <v>0</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="29"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="38"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1031,20 +1037,20 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" ht="18.75">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:17" ht="19">
+      <c r="A10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="32"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="10"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1064,19 +1070,19 @@
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:17" ht="21">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="23"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="29"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -1085,23 +1091,23 @@
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="10" t="s">
+      <c r="B13" s="31"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="10" t="s">
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="12"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="32"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -1110,27 +1116,27 @@
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="7"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="15"/>
       <c r="F14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="24" t="s">
+      <c r="G14" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="26"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="35"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -1139,25 +1145,25 @@
       <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="17"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="4">
         <v>0.1</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="17"/>
+      <c r="E15" s="23"/>
       <c r="F15" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="G15" s="27"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="29"/>
+        <v>0.2</v>
+      </c>
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="38"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1166,25 +1172,25 @@
       <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="4">
         <v>0.2</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="17"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="G16" s="27"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="29"/>
+        <v>0.6</v>
+      </c>
+      <c r="G16" s="36"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="38"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -1193,25 +1199,25 @@
       <c r="Q16" s="1"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="19"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="3">
         <v>0.5</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="19"/>
+      <c r="E17" s="26"/>
       <c r="F17" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="G17" s="27"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="29"/>
+        <v>1.5</v>
+      </c>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="38"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -1220,25 +1226,25 @@
       <c r="Q17" s="1"/>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="17"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="4">
         <v>0.3</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="17"/>
+      <c r="E18" s="23"/>
       <c r="F18" s="4">
-        <v>1</v>
-      </c>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="29"/>
+        <v>2</v>
+      </c>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="38"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1247,21 +1253,21 @@
       <c r="Q18" s="1"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="17"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="4">
         <v>1</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="23"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="29"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="38"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -1270,21 +1276,21 @@
       <c r="Q19" s="1"/>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="9"/>
+      <c r="B20" s="7"/>
       <c r="C20" s="2">
         <v>0.7</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="9"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="29"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="38"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -1292,20 +1298,20 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:17" ht="18.75">
-      <c r="A21" s="30" t="s">
+    <row r="21" spans="1:17" ht="19">
+      <c r="A21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="32"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="10"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1325,19 +1331,19 @@
       <c r="Q22" s="1"/>
     </row>
     <row r="23" spans="1:17" ht="21">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="23"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="29"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1346,23 +1352,23 @@
       <c r="Q23" s="1"/>
     </row>
     <row r="24" spans="1:17">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="13" t="s">
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="13" t="s">
+      <c r="E24" s="12"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="15"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="13"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -1371,27 +1377,27 @@
       <c r="Q24" s="1"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="7"/>
+      <c r="B25" s="15"/>
       <c r="C25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="15"/>
       <c r="F25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="33" t="s">
+      <c r="G25" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="35"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="18"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -1400,25 +1406,25 @@
       <c r="Q25" s="1"/>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="17"/>
+      <c r="B26" s="23"/>
       <c r="C26" s="4">
         <v>0.1</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="17"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="G26" s="36"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="38"/>
+        <v>0.2</v>
+      </c>
+      <c r="G26" s="19"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="21"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -1427,25 +1433,25 @@
       <c r="Q26" s="1"/>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="17"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="4">
         <v>0.2</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="17"/>
+      <c r="E27" s="23"/>
       <c r="F27" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="G27" s="36"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="38"/>
+        <v>0.6</v>
+      </c>
+      <c r="G27" s="19"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="21"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
@@ -1454,25 +1460,25 @@
       <c r="Q27" s="1"/>
     </row>
     <row r="28" spans="1:17">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="19"/>
+      <c r="B28" s="26"/>
       <c r="C28" s="3">
         <v>0.6</v>
       </c>
-      <c r="D28" s="18" t="s">
+      <c r="D28" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E28" s="19"/>
+      <c r="E28" s="26"/>
       <c r="F28" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="G28" s="36"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="38"/>
+        <v>1.5</v>
+      </c>
+      <c r="G28" s="19"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="21"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
@@ -1481,25 +1487,25 @@
       <c r="Q28" s="1"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="17"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="4">
         <v>0</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="17"/>
+      <c r="E29" s="23"/>
       <c r="F29" s="4">
-        <v>1</v>
-      </c>
-      <c r="G29" s="36"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="38"/>
+        <v>2</v>
+      </c>
+      <c r="G29" s="19"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="21"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
@@ -1508,21 +1514,21 @@
       <c r="Q29" s="1"/>
     </row>
     <row r="30" spans="1:17">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="17"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="4">
         <v>1.2</v>
       </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="17"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="23"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="38"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="21"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
@@ -1531,21 +1537,21 @@
       <c r="Q30" s="1"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="9"/>
+      <c r="B31" s="7"/>
       <c r="C31" s="2">
         <v>0.4</v>
       </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="9"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="7"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="38"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="21"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
@@ -1553,20 +1559,20 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="1:17" ht="18.75">
-      <c r="A32" s="30" t="s">
+    <row r="32" spans="1:17" ht="19">
+      <c r="A32" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="32"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="10"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
@@ -1586,19 +1592,19 @@
       <c r="Q33" s="1"/>
     </row>
     <row r="34" spans="1:17" ht="21">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="23"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="29"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
@@ -1607,23 +1613,23 @@
       <c r="Q34" s="1"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="13" t="s">
+      <c r="B35" s="12"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="14"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="13" t="s">
+      <c r="E35" s="12"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="15"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="13"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
@@ -1632,27 +1638,27 @@
       <c r="Q35" s="1"/>
     </row>
     <row r="36" spans="1:17">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="7"/>
+      <c r="B36" s="15"/>
       <c r="C36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="7"/>
+      <c r="E36" s="15"/>
       <c r="F36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G36" s="33" t="s">
+      <c r="G36" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H36" s="34"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="35"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="18"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
@@ -1661,25 +1667,25 @@
       <c r="Q36" s="1"/>
     </row>
     <row r="37" spans="1:17">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="17"/>
+      <c r="B37" s="23"/>
       <c r="C37" s="4">
         <v>0.1</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="17"/>
+      <c r="E37" s="23"/>
       <c r="F37" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="G37" s="36"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="37"/>
-      <c r="K37" s="38"/>
+        <v>0.2</v>
+      </c>
+      <c r="G37" s="19"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="21"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
@@ -1688,25 +1694,25 @@
       <c r="Q37" s="1"/>
     </row>
     <row r="38" spans="1:17">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="17"/>
+      <c r="B38" s="23"/>
       <c r="C38" s="4">
         <v>0.2</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D38" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="17"/>
+      <c r="E38" s="23"/>
       <c r="F38" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="G38" s="36"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="37"/>
-      <c r="J38" s="37"/>
-      <c r="K38" s="38"/>
+        <v>0.6</v>
+      </c>
+      <c r="G38" s="19"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="21"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
@@ -1715,288 +1721,580 @@
       <c r="Q38" s="1"/>
     </row>
     <row r="39" spans="1:17">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="19"/>
+      <c r="B39" s="26"/>
       <c r="C39" s="3">
         <v>0.6</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="D39" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E39" s="19"/>
+      <c r="E39" s="26"/>
       <c r="F39" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="G39" s="36"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="38"/>
+        <v>1.5</v>
+      </c>
+      <c r="G39" s="19"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="21"/>
     </row>
     <row r="40" spans="1:17">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="17"/>
+      <c r="B40" s="23"/>
       <c r="C40" s="4">
         <v>0.25</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D40" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="17"/>
+      <c r="E40" s="23"/>
       <c r="F40" s="4">
-        <v>1</v>
-      </c>
-      <c r="G40" s="36"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="38"/>
+        <v>2</v>
+      </c>
+      <c r="G40" s="19"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="21"/>
     </row>
     <row r="41" spans="1:17">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="17"/>
+      <c r="B41" s="23"/>
       <c r="C41" s="4">
         <v>1.2</v>
       </c>
-      <c r="D41" s="16"/>
-      <c r="E41" s="17"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="23"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="37"/>
-      <c r="J41" s="37"/>
-      <c r="K41" s="38"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="21"/>
     </row>
     <row r="42" spans="1:17">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="9"/>
+      <c r="B42" s="7"/>
       <c r="C42" s="2">
         <v>0.4</v>
       </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="9"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="7"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="37"/>
-      <c r="K42" s="38"/>
-    </row>
-    <row r="43" spans="1:17" ht="18.75">
-      <c r="A43" s="30" t="s">
+      <c r="G42" s="19"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="21"/>
+    </row>
+    <row r="43" spans="1:17" ht="19">
+      <c r="A43" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="31"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="32"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="10"/>
     </row>
     <row r="45" spans="1:17" ht="21">
-      <c r="A45" s="21" t="s">
+      <c r="A45" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B45" s="22"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
-      <c r="K45" s="23"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="29"/>
     </row>
     <row r="46" spans="1:17">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="14"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="13" t="s">
+      <c r="B46" s="12"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="14"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="13" t="s">
+      <c r="E46" s="12"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="15"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="13"/>
     </row>
     <row r="47" spans="1:17">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="7"/>
+      <c r="B47" s="15"/>
       <c r="C47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E47" s="7"/>
+      <c r="E47" s="15"/>
       <c r="F47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G47" s="33" t="s">
+      <c r="G47" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H47" s="34"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="34"/>
-      <c r="K47" s="35"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="18"/>
     </row>
     <row r="48" spans="1:17">
-      <c r="A48" s="20" t="s">
+      <c r="A48" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B48" s="17"/>
+      <c r="B48" s="23"/>
       <c r="C48" s="4">
         <v>0.1</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D48" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E48" s="17"/>
+      <c r="E48" s="23"/>
       <c r="F48" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="G48" s="36"/>
-      <c r="H48" s="37"/>
-      <c r="I48" s="37"/>
-      <c r="J48" s="37"/>
-      <c r="K48" s="38"/>
+        <v>0.2</v>
+      </c>
+      <c r="G48" s="19"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="21"/>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="16" t="s">
+      <c r="A49" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B49" s="17"/>
+      <c r="B49" s="23"/>
       <c r="C49" s="4">
         <v>0.2</v>
       </c>
-      <c r="D49" s="16" t="s">
+      <c r="D49" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="17"/>
+      <c r="E49" s="23"/>
       <c r="F49" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="G49" s="36"/>
-      <c r="H49" s="37"/>
-      <c r="I49" s="37"/>
-      <c r="J49" s="37"/>
-      <c r="K49" s="38"/>
+        <v>0.6</v>
+      </c>
+      <c r="G49" s="19"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="21"/>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="18" t="s">
+      <c r="A50" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="19"/>
+      <c r="B50" s="26"/>
       <c r="C50" s="3">
         <v>0.6</v>
       </c>
-      <c r="D50" s="18" t="s">
+      <c r="D50" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E50" s="19"/>
+      <c r="E50" s="26"/>
       <c r="F50" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="G50" s="36"/>
-      <c r="H50" s="37"/>
-      <c r="I50" s="37"/>
-      <c r="J50" s="37"/>
-      <c r="K50" s="38"/>
+        <v>1.5</v>
+      </c>
+      <c r="G50" s="19"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="21"/>
     </row>
     <row r="51" spans="1:11">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="17"/>
+      <c r="B51" s="23"/>
       <c r="C51" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="D51" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="17"/>
+      <c r="E51" s="23"/>
       <c r="F51" s="4">
-        <v>1</v>
-      </c>
-      <c r="G51" s="36"/>
-      <c r="H51" s="37"/>
-      <c r="I51" s="37"/>
-      <c r="J51" s="37"/>
-      <c r="K51" s="38"/>
+        <v>2</v>
+      </c>
+      <c r="G51" s="19"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="21"/>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="16" t="s">
+      <c r="A52" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B52" s="17"/>
+      <c r="B52" s="23"/>
       <c r="C52" s="4">
         <v>1.4</v>
       </c>
-      <c r="D52" s="16"/>
-      <c r="E52" s="17"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="23"/>
       <c r="F52" s="4"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="37"/>
-      <c r="I52" s="37"/>
-      <c r="J52" s="37"/>
-      <c r="K52" s="38"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="21"/>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="9"/>
+      <c r="B53" s="7"/>
       <c r="C53" s="2">
         <v>0.4</v>
       </c>
-      <c r="D53" s="8"/>
-      <c r="E53" s="9"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="7"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="37"/>
-      <c r="I53" s="37"/>
-      <c r="J53" s="37"/>
-      <c r="K53" s="38"/>
-    </row>
-    <row r="54" spans="1:11" ht="18.75">
-      <c r="A54" s="30" t="s">
+      <c r="G53" s="19"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="20"/>
+      <c r="K53" s="21"/>
+    </row>
+    <row r="54" spans="1:11" ht="19">
+      <c r="A54" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B54" s="31"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="31"/>
-      <c r="H54" s="31"/>
-      <c r="I54" s="31"/>
-      <c r="J54" s="31"/>
-      <c r="K54" s="32"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="10"/>
+    </row>
+    <row r="56" spans="1:11" ht="21">
+      <c r="A56" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="28"/>
+      <c r="I56" s="28"/>
+      <c r="J56" s="28"/>
+      <c r="K56" s="29"/>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" s="12"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E57" s="12"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="13"/>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="15"/>
+      <c r="C58" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" s="15"/>
+      <c r="F58" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G58" s="16"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17"/>
+      <c r="K58" s="18"/>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="23"/>
+      <c r="C59" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D59" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E59" s="23"/>
+      <c r="F59" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G59" s="19"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="21"/>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" s="23"/>
+      <c r="C60" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D60" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="23"/>
+      <c r="F60" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="G60" s="19"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
+      <c r="J60" s="20"/>
+      <c r="K60" s="21"/>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" s="26"/>
+      <c r="C61" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="D61" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="26"/>
+      <c r="F61" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="G61" s="19"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
+      <c r="J61" s="20"/>
+      <c r="K61" s="21"/>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62" s="23"/>
+      <c r="C62" s="4">
+        <v>0</v>
+      </c>
+      <c r="D62" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="23"/>
+      <c r="F62" s="4">
+        <v>2</v>
+      </c>
+      <c r="G62" s="19"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="20"/>
+      <c r="K62" s="21"/>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="23"/>
+      <c r="C63" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D63" s="24"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="20"/>
+      <c r="I63" s="20"/>
+      <c r="J63" s="20"/>
+      <c r="K63" s="21"/>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" s="7"/>
+      <c r="C64" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D64" s="6"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="20"/>
+      <c r="I64" s="20"/>
+      <c r="J64" s="20"/>
+      <c r="K64" s="21"/>
+    </row>
+    <row r="65" spans="1:11" ht="19">
+      <c r="A65" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="100">
+  <mergeCells count="120">
+    <mergeCell ref="A56:K56"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="G57:K57"/>
+    <mergeCell ref="G58:K64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A65:K65"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="G3:K9"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="G25:K31"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="A21:K21"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="A32:K32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K20"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:K42"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A45:K45"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="A54:K54"/>
@@ -2013,90 +2311,6 @@
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="D50:E50"/>
     <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A45:K45"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="G36:K42"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="G25:K31"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A32:K32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K20"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="G3:K9"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add test#7 and test#6 results
</commit_message>
<xml_diff>
--- a/Tablut/TestTablut.xlsx
+++ b/Tablut/TestTablut.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolobartelucci/MyFiles/Projects/Tablut/Tablut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198CCEB6-3F09-0F44-82BB-4EC7BBA14A41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0089212F-7DDA-7449-A90A-78F55F6CE519}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="580" windowWidth="26660" windowHeight="16740" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16800" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="32">
   <si>
     <t>KingEncirclement</t>
   </si>
@@ -116,14 +116,26 @@
     <t>TEST #6</t>
   </si>
   <si>
-    <t xml:space="preserve">RESULT: </t>
+    <t>La parita finisce in pareggio. Dopo che il bianco inizia ad oscillare come in figura dopo che il nero sposta tutti i neri sulla riga e colonna del re a un certo punto il bianco si sblocca spostando il re a destra. Il re oscilla a destra e sinistra poiché bloccato dal nero -&gt; DRAW</t>
+  </si>
+  <si>
+    <t>RESULT: DRAW</t>
+  </si>
+  <si>
+    <t>TEST #7</t>
+  </si>
+  <si>
+    <t>RESULT: IN CORSOO</t>
+  </si>
+  <si>
+    <t>DA QUI SOTTO IN AVANTI I TEST SONO FATTI DOPO IL FIX INFINITY DEL BIANCO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,8 +185,15 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +230,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -385,7 +410,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="4" applyBorder="1"/>
@@ -394,6 +419,48 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -409,39 +476,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -457,15 +491,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -492,6 +517,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -513,6 +542,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>2134</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ABB1A42-52E7-1043-A85F-5C2E94774359}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8064500" y="11087100"/>
+          <a:ext cx="2032000" cy="2059534"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -812,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{028B81F1-ACA3-4C72-9A53-A89403C903EE}">
-  <dimension ref="A1:Q65"/>
+  <dimension ref="A1:Q77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58:K64"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -827,19 +905,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="29"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="11" t="s">
@@ -861,17 +939,17 @@
       <c r="K2" s="32"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="15"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
@@ -884,17 +962,17 @@
       <c r="K3" s="35"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="23"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="4">
         <v>0.1</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="4">
         <v>0.2</v>
       </c>
@@ -911,17 +989,17 @@
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="23"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="4">
         <v>0.2</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="26"/>
       <c r="F5" s="4">
         <v>0.6</v>
       </c>
@@ -938,17 +1016,17 @@
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="26"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="3">
         <v>0.4</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="26"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="3">
         <v>1.5</v>
       </c>
@@ -965,17 +1043,17 @@
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="4">
         <v>0.5</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="26"/>
       <c r="F7" s="4">
         <v>2</v>
       </c>
@@ -992,15 +1070,15 @@
       <c r="Q7" s="1"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="23"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="4">
         <v>1</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="23"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="26"/>
       <c r="F8" s="4"/>
       <c r="G8" s="36"/>
       <c r="H8" s="37"/>
@@ -1015,15 +1093,15 @@
       <c r="Q8" s="1"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="2">
         <v>0</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="2"/>
       <c r="G9" s="36"/>
       <c r="H9" s="37"/>
@@ -1038,19 +1116,19 @@
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" ht="19">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="10"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1070,19 +1148,19 @@
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:17" ht="21">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="29"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="8"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -1116,17 +1194,17 @@
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="15"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="15"/>
+      <c r="E14" s="10"/>
       <c r="F14" s="5" t="s">
         <v>5</v>
       </c>
@@ -1145,17 +1223,17 @@
       <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="23"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="4">
         <v>0.1</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="23"/>
+      <c r="E15" s="26"/>
       <c r="F15" s="4">
         <v>0.2</v>
       </c>
@@ -1172,17 +1250,17 @@
       <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="23"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="4">
         <v>0.2</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="23"/>
+      <c r="E16" s="26"/>
       <c r="F16" s="4">
         <v>0.6</v>
       </c>
@@ -1199,17 +1277,17 @@
       <c r="Q16" s="1"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="26"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="3">
         <v>0.5</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="26"/>
+      <c r="E17" s="29"/>
       <c r="F17" s="3">
         <v>1.5</v>
       </c>
@@ -1226,17 +1304,17 @@
       <c r="Q17" s="1"/>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="23"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="4">
         <v>0.3</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="23"/>
+      <c r="E18" s="26"/>
       <c r="F18" s="4">
         <v>2</v>
       </c>
@@ -1253,15 +1331,15 @@
       <c r="Q18" s="1"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="4">
         <v>1</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="23"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="26"/>
       <c r="F19" s="4"/>
       <c r="G19" s="36"/>
       <c r="H19" s="37"/>
@@ -1276,15 +1354,15 @@
       <c r="Q19" s="1"/>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="7"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="2">
         <v>0.7</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
       <c r="F20" s="2"/>
       <c r="G20" s="36"/>
       <c r="H20" s="37"/>
@@ -1299,19 +1377,19 @@
       <c r="Q20" s="1"/>
     </row>
     <row r="21" spans="1:17" ht="19">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="10"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="24"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1331,19 +1409,19 @@
       <c r="Q22" s="1"/>
     </row>
     <row r="23" spans="1:17" ht="21">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="29"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="8"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1377,27 +1455,27 @@
       <c r="Q24" s="1"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="15"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="15"/>
+      <c r="E25" s="10"/>
       <c r="F25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="16" t="s">
+      <c r="G25" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="18"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="16"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -1406,25 +1484,25 @@
       <c r="Q25" s="1"/>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="23"/>
+      <c r="B26" s="26"/>
       <c r="C26" s="4">
         <v>0.1</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="23"/>
+      <c r="E26" s="26"/>
       <c r="F26" s="4">
         <v>0.2</v>
       </c>
-      <c r="G26" s="19"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="21"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="19"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -1433,25 +1511,25 @@
       <c r="Q26" s="1"/>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="23"/>
+      <c r="B27" s="26"/>
       <c r="C27" s="4">
         <v>0.2</v>
       </c>
-      <c r="D27" s="24" t="s">
+      <c r="D27" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="23"/>
+      <c r="E27" s="26"/>
       <c r="F27" s="4">
         <v>0.6</v>
       </c>
-      <c r="G27" s="19"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="21"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="19"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
@@ -1460,25 +1538,25 @@
       <c r="Q27" s="1"/>
     </row>
     <row r="28" spans="1:17">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="26"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="3">
         <v>0.6</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="D28" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E28" s="26"/>
+      <c r="E28" s="29"/>
       <c r="F28" s="3">
         <v>1.5</v>
       </c>
-      <c r="G28" s="19"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="21"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="19"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
@@ -1487,25 +1565,25 @@
       <c r="Q28" s="1"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="23"/>
+      <c r="B29" s="26"/>
       <c r="C29" s="4">
         <v>0</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="D29" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="23"/>
+      <c r="E29" s="26"/>
       <c r="F29" s="4">
         <v>2</v>
       </c>
-      <c r="G29" s="19"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="21"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="19"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
@@ -1514,21 +1592,21 @@
       <c r="Q29" s="1"/>
     </row>
     <row r="30" spans="1:17">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="23"/>
+      <c r="B30" s="26"/>
       <c r="C30" s="4">
         <v>1.2</v>
       </c>
-      <c r="D30" s="24"/>
-      <c r="E30" s="23"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="26"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="21"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="19"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
@@ -1537,21 +1615,21 @@
       <c r="Q30" s="1"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="7"/>
+      <c r="B31" s="21"/>
       <c r="C31" s="2">
         <v>0.4</v>
       </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="7"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="21"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="21"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="19"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
@@ -1560,19 +1638,19 @@
       <c r="Q31" s="1"/>
     </row>
     <row r="32" spans="1:17" ht="19">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="10"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="24"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
@@ -1592,19 +1670,19 @@
       <c r="Q33" s="1"/>
     </row>
     <row r="34" spans="1:17" ht="21">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="29"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="8"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
@@ -1638,27 +1716,27 @@
       <c r="Q35" s="1"/>
     </row>
     <row r="36" spans="1:17">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="15"/>
+      <c r="B36" s="10"/>
       <c r="C36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="15"/>
+      <c r="E36" s="10"/>
       <c r="F36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G36" s="16" t="s">
+      <c r="G36" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="18"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="16"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
@@ -1667,25 +1745,25 @@
       <c r="Q36" s="1"/>
     </row>
     <row r="37" spans="1:17">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="23"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="4">
         <v>0.1</v>
       </c>
-      <c r="D37" s="24" t="s">
+      <c r="D37" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="23"/>
+      <c r="E37" s="26"/>
       <c r="F37" s="4">
         <v>0.2</v>
       </c>
-      <c r="G37" s="19"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="21"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="19"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
@@ -1694,25 +1772,25 @@
       <c r="Q37" s="1"/>
     </row>
     <row r="38" spans="1:17">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="23"/>
+      <c r="B38" s="26"/>
       <c r="C38" s="4">
         <v>0.2</v>
       </c>
-      <c r="D38" s="24" t="s">
+      <c r="D38" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="23"/>
+      <c r="E38" s="26"/>
       <c r="F38" s="4">
         <v>0.6</v>
       </c>
-      <c r="G38" s="19"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="21"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="19"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
@@ -1721,110 +1799,110 @@
       <c r="Q38" s="1"/>
     </row>
     <row r="39" spans="1:17">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="26"/>
+      <c r="B39" s="29"/>
       <c r="C39" s="3">
         <v>0.6</v>
       </c>
-      <c r="D39" s="25" t="s">
+      <c r="D39" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E39" s="26"/>
+      <c r="E39" s="29"/>
       <c r="F39" s="3">
         <v>1.5</v>
       </c>
-      <c r="G39" s="19"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="21"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="19"/>
     </row>
     <row r="40" spans="1:17">
-      <c r="A40" s="24" t="s">
+      <c r="A40" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="23"/>
+      <c r="B40" s="26"/>
       <c r="C40" s="4">
         <v>0.25</v>
       </c>
-      <c r="D40" s="24" t="s">
+      <c r="D40" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="23"/>
+      <c r="E40" s="26"/>
       <c r="F40" s="4">
         <v>2</v>
       </c>
-      <c r="G40" s="19"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="21"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="19"/>
     </row>
     <row r="41" spans="1:17">
-      <c r="A41" s="24" t="s">
+      <c r="A41" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="23"/>
+      <c r="B41" s="26"/>
       <c r="C41" s="4">
         <v>1.2</v>
       </c>
-      <c r="D41" s="24"/>
-      <c r="E41" s="23"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="26"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="21"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="19"/>
     </row>
     <row r="42" spans="1:17">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="7"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="2">
         <v>0.4</v>
       </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="7"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="21"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="21"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="19"/>
     </row>
     <row r="43" spans="1:17" ht="19">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="10"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="24"/>
     </row>
     <row r="45" spans="1:17" ht="21">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="28"/>
-      <c r="K45" s="29"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="8"/>
     </row>
     <row r="46" spans="1:17">
       <c r="A46" s="11" t="s">
@@ -1846,399 +1924,628 @@
       <c r="K46" s="13"/>
     </row>
     <row r="47" spans="1:17">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="15"/>
+      <c r="B47" s="10"/>
       <c r="C47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="14" t="s">
+      <c r="D47" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E47" s="15"/>
+      <c r="E47" s="10"/>
       <c r="F47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G47" s="16" t="s">
+      <c r="G47" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="17"/>
-      <c r="K47" s="18"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="16"/>
     </row>
     <row r="48" spans="1:17">
-      <c r="A48" s="22" t="s">
+      <c r="A48" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B48" s="23"/>
+      <c r="B48" s="26"/>
       <c r="C48" s="4">
         <v>0.1</v>
       </c>
-      <c r="D48" s="24" t="s">
+      <c r="D48" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E48" s="23"/>
+      <c r="E48" s="26"/>
       <c r="F48" s="4">
         <v>0.2</v>
       </c>
-      <c r="G48" s="19"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-      <c r="J48" s="20"/>
-      <c r="K48" s="21"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="19"/>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B49" s="23"/>
+      <c r="B49" s="26"/>
       <c r="C49" s="4">
         <v>0.2</v>
       </c>
-      <c r="D49" s="24" t="s">
+      <c r="D49" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="23"/>
+      <c r="E49" s="26"/>
       <c r="F49" s="4">
         <v>0.6</v>
       </c>
-      <c r="G49" s="19"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="20"/>
-      <c r="J49" s="20"/>
-      <c r="K49" s="21"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="19"/>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="25" t="s">
+      <c r="A50" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="26"/>
+      <c r="B50" s="29"/>
       <c r="C50" s="3">
         <v>0.6</v>
       </c>
-      <c r="D50" s="25" t="s">
+      <c r="D50" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E50" s="26"/>
+      <c r="E50" s="29"/>
       <c r="F50" s="3">
         <v>1.5</v>
       </c>
-      <c r="G50" s="19"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="21"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="19"/>
     </row>
     <row r="51" spans="1:11">
-      <c r="A51" s="24" t="s">
+      <c r="A51" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="23"/>
+      <c r="B51" s="26"/>
       <c r="C51" s="4">
         <v>0</v>
       </c>
-      <c r="D51" s="24" t="s">
+      <c r="D51" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="23"/>
+      <c r="E51" s="26"/>
       <c r="F51" s="4">
         <v>2</v>
       </c>
-      <c r="G51" s="19"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="21"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="19"/>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="24" t="s">
+      <c r="A52" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B52" s="23"/>
+      <c r="B52" s="26"/>
       <c r="C52" s="4">
         <v>1.4</v>
       </c>
-      <c r="D52" s="24"/>
-      <c r="E52" s="23"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="26"/>
       <c r="F52" s="4"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-      <c r="K52" s="21"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="19"/>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="7"/>
+      <c r="B53" s="21"/>
       <c r="C53" s="2">
         <v>0.4</v>
       </c>
-      <c r="D53" s="6"/>
-      <c r="E53" s="7"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="21"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="20"/>
-      <c r="J53" s="20"/>
-      <c r="K53" s="21"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="19"/>
     </row>
     <row r="54" spans="1:11" ht="19">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
-      <c r="K54" s="10"/>
-    </row>
-    <row r="56" spans="1:11" ht="21">
-      <c r="A56" s="27" t="s">
+      <c r="B54" s="23"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="23"/>
+      <c r="G54" s="23"/>
+      <c r="H54" s="23"/>
+      <c r="I54" s="23"/>
+      <c r="J54" s="23"/>
+      <c r="K54" s="24"/>
+    </row>
+    <row r="55" spans="1:11" ht="19">
+      <c r="A55" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="39"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="39"/>
+      <c r="J55" s="39"/>
+      <c r="K55" s="40"/>
+    </row>
+    <row r="57" spans="1:11" ht="21">
+      <c r="A57" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B56" s="28"/>
-      <c r="C56" s="28"/>
-      <c r="D56" s="28"/>
-      <c r="E56" s="28"/>
-      <c r="F56" s="28"/>
-      <c r="G56" s="28"/>
-      <c r="H56" s="28"/>
-      <c r="I56" s="28"/>
-      <c r="J56" s="28"/>
-      <c r="K56" s="29"/>
-    </row>
-    <row r="57" spans="1:11">
-      <c r="A57" s="11" t="s">
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="8"/>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B57" s="12"/>
-      <c r="C57" s="13"/>
-      <c r="D57" s="11" t="s">
+      <c r="B58" s="12"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="12"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="11" t="s">
+      <c r="E58" s="12"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="12"/>
-      <c r="K57" s="13"/>
-    </row>
-    <row r="58" spans="1:11">
-      <c r="A58" s="14" t="s">
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="13"/>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B58" s="15"/>
-      <c r="C58" s="5" t="s">
+      <c r="B59" s="10"/>
+      <c r="C59" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="14" t="s">
+      <c r="D59" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E58" s="15"/>
-      <c r="F58" s="5" t="s">
+      <c r="E59" s="10"/>
+      <c r="F59" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G58" s="16"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="17"/>
-      <c r="J58" s="17"/>
-      <c r="K58" s="18"/>
-    </row>
-    <row r="59" spans="1:11">
-      <c r="A59" s="22" t="s">
+      <c r="G59" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="15"/>
+      <c r="K59" s="16"/>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B59" s="23"/>
-      <c r="C59" s="4">
+      <c r="B60" s="26"/>
+      <c r="C60" s="4">
         <v>0.1</v>
       </c>
-      <c r="D59" s="24" t="s">
+      <c r="D60" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E59" s="23"/>
-      <c r="F59" s="4">
+      <c r="E60" s="26"/>
+      <c r="F60" s="4">
         <v>0.2</v>
       </c>
-      <c r="G59" s="19"/>
-      <c r="H59" s="20"/>
-      <c r="I59" s="20"/>
-      <c r="J59" s="20"/>
-      <c r="K59" s="21"/>
-    </row>
-    <row r="60" spans="1:11">
-      <c r="A60" s="24" t="s">
+      <c r="G60" s="17"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+      <c r="J60" s="18"/>
+      <c r="K60" s="19"/>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B60" s="23"/>
-      <c r="C60" s="4">
+      <c r="B61" s="26"/>
+      <c r="C61" s="4">
         <v>0.2</v>
       </c>
-      <c r="D60" s="24" t="s">
+      <c r="D61" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E60" s="23"/>
-      <c r="F60" s="4">
+      <c r="E61" s="26"/>
+      <c r="F61" s="4">
         <v>0.6</v>
       </c>
-      <c r="G60" s="19"/>
-      <c r="H60" s="20"/>
-      <c r="I60" s="20"/>
-      <c r="J60" s="20"/>
-      <c r="K60" s="21"/>
-    </row>
-    <row r="61" spans="1:11">
-      <c r="A61" s="25" t="s">
+      <c r="G61" s="17"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="19"/>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="26"/>
-      <c r="C61" s="3">
+      <c r="B62" s="29"/>
+      <c r="C62" s="3">
         <v>0.7</v>
       </c>
-      <c r="D61" s="25" t="s">
+      <c r="D62" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E61" s="26"/>
-      <c r="F61" s="3">
+      <c r="E62" s="29"/>
+      <c r="F62" s="3">
         <v>1.5</v>
       </c>
-      <c r="G61" s="19"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="20"/>
-      <c r="J61" s="20"/>
-      <c r="K61" s="21"/>
-    </row>
-    <row r="62" spans="1:11">
-      <c r="A62" s="24" t="s">
+      <c r="G62" s="17"/>
+      <c r="H62" s="18"/>
+      <c r="I62" s="18"/>
+      <c r="J62" s="18"/>
+      <c r="K62" s="19"/>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B62" s="23"/>
-      <c r="C62" s="4">
+      <c r="B63" s="26"/>
+      <c r="C63" s="4">
         <v>0</v>
       </c>
-      <c r="D62" s="24" t="s">
+      <c r="D63" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E62" s="23"/>
-      <c r="F62" s="4">
+      <c r="E63" s="26"/>
+      <c r="F63" s="4">
         <v>2</v>
       </c>
-      <c r="G62" s="19"/>
-      <c r="H62" s="20"/>
-      <c r="I62" s="20"/>
-      <c r="J62" s="20"/>
-      <c r="K62" s="21"/>
-    </row>
-    <row r="63" spans="1:11">
-      <c r="A63" s="24" t="s">
+      <c r="G63" s="17"/>
+      <c r="H63" s="18"/>
+      <c r="I63" s="18"/>
+      <c r="J63" s="18"/>
+      <c r="K63" s="19"/>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="4">
+      <c r="B64" s="26"/>
+      <c r="C64" s="4">
         <v>1.5</v>
       </c>
-      <c r="D63" s="24"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="19"/>
-      <c r="H63" s="20"/>
-      <c r="I63" s="20"/>
-      <c r="J63" s="20"/>
-      <c r="K63" s="21"/>
-    </row>
-    <row r="64" spans="1:11">
-      <c r="A64" s="6" t="s">
+      <c r="D64" s="27"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="18"/>
+      <c r="J64" s="18"/>
+      <c r="K64" s="19"/>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B64" s="7"/>
-      <c r="C64" s="2">
+      <c r="B65" s="21"/>
+      <c r="C65" s="2">
         <v>0.4</v>
       </c>
-      <c r="D64" s="6"/>
-      <c r="E64" s="7"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="19"/>
-      <c r="H64" s="20"/>
-      <c r="I64" s="20"/>
-      <c r="J64" s="20"/>
-      <c r="K64" s="21"/>
-    </row>
-    <row r="65" spans="1:11" ht="19">
-      <c r="A65" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B65" s="9"/>
-      <c r="C65" s="9"/>
-      <c r="D65" s="9"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
-      <c r="I65" s="9"/>
-      <c r="J65" s="9"/>
-      <c r="K65" s="10"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="17"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18"/>
+      <c r="K65" s="19"/>
+    </row>
+    <row r="66" spans="1:11" ht="19">
+      <c r="A66" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66" s="23"/>
+      <c r="C66" s="23"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="23"/>
+      <c r="G66" s="23"/>
+      <c r="H66" s="23"/>
+      <c r="I66" s="23"/>
+      <c r="J66" s="23"/>
+      <c r="K66" s="24"/>
+    </row>
+    <row r="68" spans="1:11" ht="21">
+      <c r="A68" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="7"/>
+      <c r="K68" s="8"/>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69" s="12"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E69" s="12"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="12"/>
+      <c r="K69" s="13"/>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" s="10"/>
+      <c r="C70" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" s="10"/>
+      <c r="F70" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G70" s="14"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+      <c r="J70" s="15"/>
+      <c r="K70" s="16"/>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" s="26"/>
+      <c r="C71" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D71" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E71" s="26"/>
+      <c r="F71" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G71" s="17"/>
+      <c r="H71" s="18"/>
+      <c r="I71" s="18"/>
+      <c r="J71" s="18"/>
+      <c r="K71" s="19"/>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="26"/>
+      <c r="C72" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D72" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" s="26"/>
+      <c r="F72" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="G72" s="17"/>
+      <c r="H72" s="18"/>
+      <c r="I72" s="18"/>
+      <c r="J72" s="18"/>
+      <c r="K72" s="19"/>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="29"/>
+      <c r="C73" s="3">
+        <v>1</v>
+      </c>
+      <c r="D73" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="29"/>
+      <c r="F73" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="G73" s="17"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="18"/>
+      <c r="J73" s="18"/>
+      <c r="K73" s="19"/>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" s="26"/>
+      <c r="C74" s="4">
+        <v>0</v>
+      </c>
+      <c r="D74" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E74" s="26"/>
+      <c r="F74" s="4">
+        <v>2</v>
+      </c>
+      <c r="G74" s="17"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="18"/>
+      <c r="J74" s="18"/>
+      <c r="K74" s="19"/>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" s="26"/>
+      <c r="C75" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D75" s="27"/>
+      <c r="E75" s="26"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="17"/>
+      <c r="H75" s="18"/>
+      <c r="I75" s="18"/>
+      <c r="J75" s="18"/>
+      <c r="K75" s="19"/>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" s="21"/>
+      <c r="C76" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D76" s="20"/>
+      <c r="E76" s="21"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="17"/>
+      <c r="H76" s="18"/>
+      <c r="I76" s="18"/>
+      <c r="J76" s="18"/>
+      <c r="K76" s="19"/>
+    </row>
+    <row r="77" spans="1:11" ht="19">
+      <c r="A77" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B77" s="23"/>
+      <c r="C77" s="23"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="23"/>
+      <c r="F77" s="23"/>
+      <c r="G77" s="23"/>
+      <c r="H77" s="23"/>
+      <c r="I77" s="23"/>
+      <c r="J77" s="23"/>
+      <c r="K77" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="120">
-    <mergeCell ref="A56:K56"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="G57:K57"/>
-    <mergeCell ref="G58:K64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="A65:K65"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:E16"/>
+  <mergeCells count="140">
+    <mergeCell ref="A77:K77"/>
+    <mergeCell ref="A68:K68"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="G69:K69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="G70:K76"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="A54:K54"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="G46:K46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="G47:K53"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A45:K45"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:K42"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A32:K32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K20"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:E17"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="G3:K9"/>
@@ -2259,60 +2566,57 @@
     <mergeCell ref="A12:K12"/>
     <mergeCell ref="A21:K21"/>
     <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A32:K32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K20"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="G36:K42"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A45:K45"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="A54:K54"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="G46:K46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="G47:K53"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="G58:K58"/>
+    <mergeCell ref="G59:K65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="A66:K66"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A65:B65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add test#7 and #8
</commit_message>
<xml_diff>
--- a/Tablut/TestTablut.xlsx
+++ b/Tablut/TestTablut.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolobartelucci/MyFiles/Projects/Tablut/Tablut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0089212F-7DDA-7449-A90A-78F55F6CE519}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32599D1-A4D6-DD45-9744-984715A7F2D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16800" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16780" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="34">
   <si>
     <t>KingEncirclement</t>
   </si>
@@ -110,9 +110,6 @@
     <t xml:space="preserve">RESULT: WHITE WIN </t>
   </si>
   <si>
-    <t xml:space="preserve">Il White si è comportato bene per quasi tutta la partita ovviamente è più aggressivo visto l'aumento del PawnsDifference è riuscito a vincere dopo una mezz'ora di gioco          Anche al secondo tentativo si è comportato allo stesso modo   </t>
-  </si>
-  <si>
     <t>TEST #6</t>
   </si>
   <si>
@@ -125,10 +122,19 @@
     <t>TEST #7</t>
   </si>
   <si>
-    <t>RESULT: IN CORSOO</t>
-  </si>
-  <si>
     <t>DA QUI SOTTO IN AVANTI I TEST SONO FATTI DOPO IL FIX INFINITY DEL BIANCO</t>
+  </si>
+  <si>
+    <t>TEST #8 = 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il White si è comportato bene per quasi tutta la partita ovviamente è più aggressivo visto l'aumento del PawnsDifference è riuscito a vincere dopo una mezz'ora di gioco. Anche al secondo tentativo si è comportato allo stesso modo   </t>
+  </si>
+  <si>
+    <t>RESULT: WHITEWIN</t>
+  </si>
+  <si>
+    <t>Riprovo i pesi del whitewin precedente</t>
   </si>
 </sst>
 </file>
@@ -419,108 +425,108 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -890,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{028B81F1-ACA3-4C72-9A53-A89403C903EE}">
-  <dimension ref="A1:Q77"/>
+  <dimension ref="A1:Q88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="75" workbookViewId="0">
-      <selection activeCell="N52" sqref="N52"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N80" sqref="N80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -905,61 +911,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="8"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="11" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="30" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="32"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="34"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="18"/>
       <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="35"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="37"/>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="25" t="s">
@@ -976,11 +982,11 @@
       <c r="F4" s="4">
         <v>0.2</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="40"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -1003,11 +1009,11 @@
       <c r="F5" s="4">
         <v>0.6</v>
       </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="40"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -1030,11 +1036,11 @@
       <c r="F6" s="3">
         <v>1.5</v>
       </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="40"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -1057,11 +1063,11 @@
       <c r="F7" s="4">
         <v>2</v>
       </c>
-      <c r="G7" s="36"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="40"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -1080,11 +1086,11 @@
       <c r="D8" s="27"/>
       <c r="E8" s="26"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="40"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1093,21 +1099,21 @@
       <c r="Q8" s="1"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="21"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="2">
         <v>0</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="31"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="40"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1116,19 +1122,19 @@
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" ht="19">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="24"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="10"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1148,19 +1154,19 @@
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:17" ht="21">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="8"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="13"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -1169,23 +1175,23 @@
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="30" t="s">
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="30" t="s">
+      <c r="E13" s="33"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="32"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="34"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -1194,27 +1200,27 @@
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="10"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="18"/>
       <c r="F14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="35"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="37"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -1237,11 +1243,11 @@
       <c r="F15" s="4">
         <v>0.2</v>
       </c>
-      <c r="G15" s="36"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="40"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1264,11 +1270,11 @@
       <c r="F16" s="4">
         <v>0.6</v>
       </c>
-      <c r="G16" s="36"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="40"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -1291,11 +1297,11 @@
       <c r="F17" s="3">
         <v>1.5</v>
       </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="40"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -1318,11 +1324,11 @@
       <c r="F18" s="4">
         <v>2</v>
       </c>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="40"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1341,11 +1347,11 @@
       <c r="D19" s="27"/>
       <c r="E19" s="26"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="40"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -1354,21 +1360,21 @@
       <c r="Q19" s="1"/>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="21"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="2">
         <v>0.7</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="31"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="40"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -1377,19 +1383,19 @@
       <c r="Q20" s="1"/>
     </row>
     <row r="21" spans="1:17" ht="19">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="24"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="10"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1409,19 +1415,19 @@
       <c r="Q22" s="1"/>
     </row>
     <row r="23" spans="1:17" ht="21">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="8"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="13"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1430,23 +1436,23 @@
       <c r="Q23" s="1"/>
     </row>
     <row r="24" spans="1:17">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="11" t="s">
+      <c r="B24" s="15"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="11" t="s">
+      <c r="E24" s="15"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="13"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="16"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -1455,27 +1461,27 @@
       <c r="Q24" s="1"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="10"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="10"/>
+      <c r="E25" s="18"/>
       <c r="F25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="16"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="21"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -1498,11 +1504,11 @@
       <c r="F26" s="4">
         <v>0.2</v>
       </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="19"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="24"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -1525,11 +1531,11 @@
       <c r="F27" s="4">
         <v>0.6</v>
       </c>
-      <c r="G27" s="17"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="19"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="24"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
@@ -1552,11 +1558,11 @@
       <c r="F28" s="3">
         <v>1.5</v>
       </c>
-      <c r="G28" s="17"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="19"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="24"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
@@ -1579,11 +1585,11 @@
       <c r="F29" s="4">
         <v>2</v>
       </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="19"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="24"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
@@ -1602,11 +1608,11 @@
       <c r="D30" s="27"/>
       <c r="E30" s="26"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="19"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="24"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
@@ -1615,21 +1621,21 @@
       <c r="Q30" s="1"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="21"/>
+      <c r="B31" s="31"/>
       <c r="C31" s="2">
         <v>0.4</v>
       </c>
-      <c r="D31" s="20"/>
-      <c r="E31" s="21"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="31"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="19"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="24"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
@@ -1638,19 +1644,19 @@
       <c r="Q31" s="1"/>
     </row>
     <row r="32" spans="1:17" ht="19">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="24"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="10"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
@@ -1670,19 +1676,19 @@
       <c r="Q33" s="1"/>
     </row>
     <row r="34" spans="1:17" ht="21">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="8"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="13"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
@@ -1691,23 +1697,23 @@
       <c r="Q34" s="1"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="11" t="s">
+      <c r="B35" s="15"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="12"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="11" t="s">
+      <c r="E35" s="15"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="13"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="16"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
@@ -1716,27 +1722,27 @@
       <c r="Q35" s="1"/>
     </row>
     <row r="36" spans="1:17">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="10"/>
+      <c r="B36" s="18"/>
       <c r="C36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="10"/>
+      <c r="E36" s="18"/>
       <c r="F36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G36" s="14" t="s">
+      <c r="G36" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="16"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="21"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
@@ -1759,11 +1765,11 @@
       <c r="F37" s="4">
         <v>0.2</v>
       </c>
-      <c r="G37" s="17"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
-      <c r="K37" s="19"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="24"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
@@ -1786,11 +1792,11 @@
       <c r="F38" s="4">
         <v>0.6</v>
       </c>
-      <c r="G38" s="17"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="19"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="24"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
@@ -1813,11 +1819,11 @@
       <c r="F39" s="3">
         <v>1.5</v>
       </c>
-      <c r="G39" s="17"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="19"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="24"/>
     </row>
     <row r="40" spans="1:17">
       <c r="A40" s="27" t="s">
@@ -1834,11 +1840,11 @@
       <c r="F40" s="4">
         <v>2</v>
       </c>
-      <c r="G40" s="17"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
-      <c r="K40" s="19"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="24"/>
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="27" t="s">
@@ -1851,100 +1857,100 @@
       <c r="D41" s="27"/>
       <c r="E41" s="26"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="19"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="24"/>
     </row>
     <row r="42" spans="1:17">
-      <c r="A42" s="20" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="31"/>
       <c r="C42" s="2">
         <v>0.4</v>
       </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="21"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="31"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="19"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="24"/>
     </row>
     <row r="43" spans="1:17" ht="19">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="23"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
-      <c r="K43" s="24"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="10"/>
     </row>
     <row r="45" spans="1:17" ht="21">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="8"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="13"/>
     </row>
     <row r="46" spans="1:17">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="12"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="11" t="s">
+      <c r="B46" s="15"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="12"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="11" t="s">
+      <c r="E46" s="15"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="12"/>
-      <c r="K46" s="13"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="16"/>
     </row>
     <row r="47" spans="1:17">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="10"/>
+      <c r="B47" s="18"/>
       <c r="C47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="9" t="s">
+      <c r="D47" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E47" s="10"/>
+      <c r="E47" s="18"/>
       <c r="F47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G47" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="16"/>
+      <c r="G47" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="21"/>
     </row>
     <row r="48" spans="1:17">
       <c r="A48" s="25" t="s">
@@ -1961,11 +1967,11 @@
       <c r="F48" s="4">
         <v>0.2</v>
       </c>
-      <c r="G48" s="17"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
-      <c r="K48" s="19"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="23"/>
+      <c r="K48" s="24"/>
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="27" t="s">
@@ -1982,11 +1988,11 @@
       <c r="F49" s="4">
         <v>0.6</v>
       </c>
-      <c r="G49" s="17"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="19"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="24"/>
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="28" t="s">
@@ -2003,11 +2009,11 @@
       <c r="F50" s="3">
         <v>1.5</v>
       </c>
-      <c r="G50" s="17"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="19"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="23"/>
+      <c r="J50" s="23"/>
+      <c r="K50" s="24"/>
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="27" t="s">
@@ -2024,11 +2030,11 @@
       <c r="F51" s="4">
         <v>2</v>
       </c>
-      <c r="G51" s="17"/>
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="18"/>
-      <c r="K51" s="19"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="23"/>
+      <c r="I51" s="23"/>
+      <c r="J51" s="23"/>
+      <c r="K51" s="24"/>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="27" t="s">
@@ -2041,115 +2047,115 @@
       <c r="D52" s="27"/>
       <c r="E52" s="26"/>
       <c r="F52" s="4"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="18"/>
-      <c r="K52" s="19"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="23"/>
+      <c r="I52" s="23"/>
+      <c r="J52" s="23"/>
+      <c r="K52" s="24"/>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="20" t="s">
+      <c r="A53" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="21"/>
+      <c r="B53" s="31"/>
       <c r="C53" s="2">
         <v>0.4</v>
       </c>
-      <c r="D53" s="20"/>
-      <c r="E53" s="21"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="31"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="19"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="23"/>
+      <c r="J53" s="23"/>
+      <c r="K53" s="24"/>
     </row>
     <row r="54" spans="1:11" ht="19">
-      <c r="A54" s="22" t="s">
+      <c r="A54" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B54" s="23"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="23"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="23"/>
-      <c r="G54" s="23"/>
-      <c r="H54" s="23"/>
-      <c r="I54" s="23"/>
-      <c r="J54" s="23"/>
-      <c r="K54" s="24"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="10"/>
     </row>
     <row r="55" spans="1:11" ht="19">
-      <c r="A55" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="B55" s="39"/>
-      <c r="C55" s="39"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="39"/>
-      <c r="G55" s="39"/>
-      <c r="H55" s="39"/>
-      <c r="I55" s="39"/>
-      <c r="J55" s="39"/>
-      <c r="K55" s="40"/>
+      <c r="A55" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="7"/>
     </row>
     <row r="57" spans="1:11" ht="21">
-      <c r="A57" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="8"/>
+      <c r="A57" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="13"/>
     </row>
     <row r="58" spans="1:11">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B58" s="12"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="11" t="s">
+      <c r="B58" s="15"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E58" s="12"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="11" t="s">
+      <c r="E58" s="15"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H58" s="12"/>
-      <c r="I58" s="12"/>
-      <c r="J58" s="12"/>
-      <c r="K58" s="13"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="16"/>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="10"/>
+      <c r="B59" s="18"/>
       <c r="C59" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D59" s="9" t="s">
+      <c r="D59" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E59" s="10"/>
+      <c r="E59" s="18"/>
       <c r="F59" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G59" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15"/>
-      <c r="J59" s="15"/>
-      <c r="K59" s="16"/>
+      <c r="G59" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="21"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="25" t="s">
@@ -2166,11 +2172,11 @@
       <c r="F60" s="4">
         <v>0.2</v>
       </c>
-      <c r="G60" s="17"/>
-      <c r="H60" s="18"/>
-      <c r="I60" s="18"/>
-      <c r="J60" s="18"/>
-      <c r="K60" s="19"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="23"/>
+      <c r="I60" s="23"/>
+      <c r="J60" s="23"/>
+      <c r="K60" s="24"/>
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="27" t="s">
@@ -2187,11 +2193,11 @@
       <c r="F61" s="4">
         <v>0.6</v>
       </c>
-      <c r="G61" s="17"/>
-      <c r="H61" s="18"/>
-      <c r="I61" s="18"/>
-      <c r="J61" s="18"/>
-      <c r="K61" s="19"/>
+      <c r="G61" s="22"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="23"/>
+      <c r="J61" s="23"/>
+      <c r="K61" s="24"/>
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="28" t="s">
@@ -2208,11 +2214,11 @@
       <c r="F62" s="3">
         <v>1.5</v>
       </c>
-      <c r="G62" s="17"/>
-      <c r="H62" s="18"/>
-      <c r="I62" s="18"/>
-      <c r="J62" s="18"/>
-      <c r="K62" s="19"/>
+      <c r="G62" s="22"/>
+      <c r="H62" s="23"/>
+      <c r="I62" s="23"/>
+      <c r="J62" s="23"/>
+      <c r="K62" s="24"/>
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="27" t="s">
@@ -2229,11 +2235,11 @@
       <c r="F63" s="4">
         <v>2</v>
       </c>
-      <c r="G63" s="17"/>
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
-      <c r="J63" s="18"/>
-      <c r="K63" s="19"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="23"/>
+      <c r="I63" s="23"/>
+      <c r="J63" s="23"/>
+      <c r="K63" s="24"/>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="27" t="s">
@@ -2246,98 +2252,98 @@
       <c r="D64" s="27"/>
       <c r="E64" s="26"/>
       <c r="F64" s="4"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="18"/>
-      <c r="I64" s="18"/>
-      <c r="J64" s="18"/>
-      <c r="K64" s="19"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="23"/>
+      <c r="I64" s="23"/>
+      <c r="J64" s="23"/>
+      <c r="K64" s="24"/>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="20" t="s">
+      <c r="A65" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B65" s="21"/>
+      <c r="B65" s="31"/>
       <c r="C65" s="2">
         <v>0.4</v>
       </c>
-      <c r="D65" s="20"/>
-      <c r="E65" s="21"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="31"/>
       <c r="F65" s="2"/>
-      <c r="G65" s="17"/>
-      <c r="H65" s="18"/>
-      <c r="I65" s="18"/>
-      <c r="J65" s="18"/>
-      <c r="K65" s="19"/>
+      <c r="G65" s="22"/>
+      <c r="H65" s="23"/>
+      <c r="I65" s="23"/>
+      <c r="J65" s="23"/>
+      <c r="K65" s="24"/>
     </row>
     <row r="66" spans="1:11" ht="19">
-      <c r="A66" s="22" t="s">
+      <c r="A66" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="10"/>
+    </row>
+    <row r="68" spans="1:11" ht="21">
+      <c r="A68" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B66" s="23"/>
-      <c r="C66" s="23"/>
-      <c r="D66" s="23"/>
-      <c r="E66" s="23"/>
-      <c r="F66" s="23"/>
-      <c r="G66" s="23"/>
-      <c r="H66" s="23"/>
-      <c r="I66" s="23"/>
-      <c r="J66" s="23"/>
-      <c r="K66" s="24"/>
-    </row>
-    <row r="68" spans="1:11" ht="21">
-      <c r="A68" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
-      <c r="E68" s="7"/>
-      <c r="F68" s="7"/>
-      <c r="G68" s="7"/>
-      <c r="H68" s="7"/>
-      <c r="I68" s="7"/>
-      <c r="J68" s="7"/>
-      <c r="K68" s="8"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="12"/>
+      <c r="K68" s="13"/>
     </row>
     <row r="69" spans="1:11">
-      <c r="A69" s="11" t="s">
+      <c r="A69" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B69" s="12"/>
-      <c r="C69" s="13"/>
-      <c r="D69" s="11" t="s">
+      <c r="B69" s="15"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E69" s="12"/>
-      <c r="F69" s="13"/>
-      <c r="G69" s="11" t="s">
+      <c r="E69" s="15"/>
+      <c r="F69" s="16"/>
+      <c r="G69" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H69" s="12"/>
-      <c r="I69" s="12"/>
-      <c r="J69" s="12"/>
-      <c r="K69" s="13"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+      <c r="J69" s="15"/>
+      <c r="K69" s="16"/>
     </row>
     <row r="70" spans="1:11">
-      <c r="A70" s="9" t="s">
+      <c r="A70" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B70" s="10"/>
+      <c r="B70" s="18"/>
       <c r="C70" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D70" s="9" t="s">
+      <c r="D70" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="10"/>
+      <c r="E70" s="18"/>
       <c r="F70" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G70" s="14"/>
-      <c r="H70" s="15"/>
-      <c r="I70" s="15"/>
-      <c r="J70" s="15"/>
-      <c r="K70" s="16"/>
+      <c r="G70" s="19"/>
+      <c r="H70" s="20"/>
+      <c r="I70" s="20"/>
+      <c r="J70" s="20"/>
+      <c r="K70" s="21"/>
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="25" t="s">
@@ -2354,11 +2360,11 @@
       <c r="F71" s="4">
         <v>0.2</v>
       </c>
-      <c r="G71" s="17"/>
-      <c r="H71" s="18"/>
-      <c r="I71" s="18"/>
-      <c r="J71" s="18"/>
-      <c r="K71" s="19"/>
+      <c r="G71" s="22"/>
+      <c r="H71" s="23"/>
+      <c r="I71" s="23"/>
+      <c r="J71" s="23"/>
+      <c r="K71" s="24"/>
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="27" t="s">
@@ -2375,11 +2381,11 @@
       <c r="F72" s="4">
         <v>0.6</v>
       </c>
-      <c r="G72" s="17"/>
-      <c r="H72" s="18"/>
-      <c r="I72" s="18"/>
-      <c r="J72" s="18"/>
-      <c r="K72" s="19"/>
+      <c r="G72" s="22"/>
+      <c r="H72" s="23"/>
+      <c r="I72" s="23"/>
+      <c r="J72" s="23"/>
+      <c r="K72" s="24"/>
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="28" t="s">
@@ -2396,11 +2402,11 @@
       <c r="F73" s="3">
         <v>1.5</v>
       </c>
-      <c r="G73" s="17"/>
-      <c r="H73" s="18"/>
-      <c r="I73" s="18"/>
-      <c r="J73" s="18"/>
-      <c r="K73" s="19"/>
+      <c r="G73" s="22"/>
+      <c r="H73" s="23"/>
+      <c r="I73" s="23"/>
+      <c r="J73" s="23"/>
+      <c r="K73" s="24"/>
     </row>
     <row r="74" spans="1:11">
       <c r="A74" s="27" t="s">
@@ -2417,11 +2423,11 @@
       <c r="F74" s="4">
         <v>2</v>
       </c>
-      <c r="G74" s="17"/>
-      <c r="H74" s="18"/>
-      <c r="I74" s="18"/>
-      <c r="J74" s="18"/>
-      <c r="K74" s="19"/>
+      <c r="G74" s="22"/>
+      <c r="H74" s="23"/>
+      <c r="I74" s="23"/>
+      <c r="J74" s="23"/>
+      <c r="K74" s="24"/>
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="27" t="s">
@@ -2434,46 +2440,236 @@
       <c r="D75" s="27"/>
       <c r="E75" s="26"/>
       <c r="F75" s="4"/>
-      <c r="G75" s="17"/>
-      <c r="H75" s="18"/>
-      <c r="I75" s="18"/>
-      <c r="J75" s="18"/>
-      <c r="K75" s="19"/>
+      <c r="G75" s="22"/>
+      <c r="H75" s="23"/>
+      <c r="I75" s="23"/>
+      <c r="J75" s="23"/>
+      <c r="K75" s="24"/>
     </row>
     <row r="76" spans="1:11">
-      <c r="A76" s="20" t="s">
+      <c r="A76" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B76" s="21"/>
+      <c r="B76" s="31"/>
       <c r="C76" s="2">
         <v>0.5</v>
       </c>
-      <c r="D76" s="20"/>
-      <c r="E76" s="21"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="31"/>
       <c r="F76" s="2"/>
-      <c r="G76" s="17"/>
-      <c r="H76" s="18"/>
-      <c r="I76" s="18"/>
-      <c r="J76" s="18"/>
-      <c r="K76" s="19"/>
+      <c r="G76" s="22"/>
+      <c r="H76" s="23"/>
+      <c r="I76" s="23"/>
+      <c r="J76" s="23"/>
+      <c r="K76" s="24"/>
     </row>
     <row r="77" spans="1:11" ht="19">
-      <c r="A77" s="22" t="s">
+      <c r="A77" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77" s="9"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="9"/>
+      <c r="J77" s="9"/>
+      <c r="K77" s="10"/>
+    </row>
+    <row r="79" spans="1:11" ht="21">
+      <c r="A79" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B77" s="23"/>
-      <c r="C77" s="23"/>
-      <c r="D77" s="23"/>
-      <c r="E77" s="23"/>
-      <c r="F77" s="23"/>
-      <c r="G77" s="23"/>
-      <c r="H77" s="23"/>
-      <c r="I77" s="23"/>
-      <c r="J77" s="23"/>
-      <c r="K77" s="24"/>
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="12"/>
+      <c r="K79" s="13"/>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B80" s="15"/>
+      <c r="C80" s="16"/>
+      <c r="D80" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E80" s="15"/>
+      <c r="F80" s="16"/>
+      <c r="G80" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H80" s="15"/>
+      <c r="I80" s="15"/>
+      <c r="J80" s="15"/>
+      <c r="K80" s="16"/>
+    </row>
+    <row r="81" spans="1:11">
+      <c r="A81" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" s="18"/>
+      <c r="C81" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E81" s="18"/>
+      <c r="F81" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G81" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H81" s="20"/>
+      <c r="I81" s="20"/>
+      <c r="J81" s="20"/>
+      <c r="K81" s="21"/>
+    </row>
+    <row r="82" spans="1:11">
+      <c r="A82" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="26"/>
+      <c r="C82" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D82" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E82" s="26"/>
+      <c r="F82" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G82" s="22"/>
+      <c r="H82" s="23"/>
+      <c r="I82" s="23"/>
+      <c r="J82" s="23"/>
+      <c r="K82" s="24"/>
+    </row>
+    <row r="83" spans="1:11">
+      <c r="A83" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B83" s="26"/>
+      <c r="C83" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D83" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="26"/>
+      <c r="F83" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="G83" s="22"/>
+      <c r="H83" s="23"/>
+      <c r="I83" s="23"/>
+      <c r="J83" s="23"/>
+      <c r="K83" s="24"/>
+    </row>
+    <row r="84" spans="1:11">
+      <c r="A84" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B84" s="29"/>
+      <c r="C84" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D84" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="29"/>
+      <c r="F84" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="G84" s="22"/>
+      <c r="H84" s="23"/>
+      <c r="I84" s="23"/>
+      <c r="J84" s="23"/>
+      <c r="K84" s="24"/>
+    </row>
+    <row r="85" spans="1:11">
+      <c r="A85" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" s="26"/>
+      <c r="C85" s="4">
+        <v>0</v>
+      </c>
+      <c r="D85" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E85" s="26"/>
+      <c r="F85" s="4">
+        <v>2</v>
+      </c>
+      <c r="G85" s="22"/>
+      <c r="H85" s="23"/>
+      <c r="I85" s="23"/>
+      <c r="J85" s="23"/>
+      <c r="K85" s="24"/>
+    </row>
+    <row r="86" spans="1:11">
+      <c r="A86" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B86" s="26"/>
+      <c r="C86" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="D86" s="27"/>
+      <c r="E86" s="26"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="22"/>
+      <c r="H86" s="23"/>
+      <c r="I86" s="23"/>
+      <c r="J86" s="23"/>
+      <c r="K86" s="24"/>
+    </row>
+    <row r="87" spans="1:11">
+      <c r="A87" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B87" s="31"/>
+      <c r="C87" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D87" s="30"/>
+      <c r="E87" s="31"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="22"/>
+      <c r="H87" s="23"/>
+      <c r="I87" s="23"/>
+      <c r="J87" s="23"/>
+      <c r="K87" s="24"/>
+    </row>
+    <row r="88" spans="1:11" ht="19">
+      <c r="A88" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B88" s="9"/>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+      <c r="H88" s="9"/>
+      <c r="I88" s="9"/>
+      <c r="J88" s="9"/>
+      <c r="K88" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="140">
+  <mergeCells count="160">
     <mergeCell ref="A77:K77"/>
     <mergeCell ref="A68:K68"/>
     <mergeCell ref="A69:C69"/>
@@ -2546,6 +2742,12 @@
     <mergeCell ref="G24:K24"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:E16"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="G3:K9"/>
@@ -2570,12 +2772,6 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:E16"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A13:C13"/>
@@ -2614,6 +2810,26 @@
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="D64:E64"/>
     <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A88:K88"/>
+    <mergeCell ref="A79:K79"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="G80:K80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="G81:K87"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:E87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Test9 and Test10 to the TestTablut.xlsx file
</commit_message>
<xml_diff>
--- a/Tablut/TestTablut.xlsx
+++ b/Tablut/TestTablut.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolobartelucci/MyFiles/Projects/Tablut/Tablut/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\Tablut\Tablut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32599D1-A4D6-DD45-9744-984715A7F2D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604FF609-82E7-4442-A843-DBC29B287E3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16780" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="38">
   <si>
     <t>KingEncirclement</t>
   </si>
@@ -135,13 +135,67 @@
   </si>
   <si>
     <t>Riprovo i pesi del whitewin precedente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST #9 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Comportamento pressochè identico al test 6 dopo un buon inizio del bianco che per i primi 15 minuti ha mangiato 5/6 pedine avversarie situazione di stallo in alto a destra come in figura che ha portato la partita a terminare in pareggio nello stesso modo dopo 45 minuti di gioco.   Il lieve aumento di PawnsDiff e WhiteMan non è ancora sufficiente a sbloccare il gioco.  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST #10 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Comportamento ancora analogo ai test 6 e 9 con la differenza che avendo aumentato la PawnDifference ulteriormente il bianco è più aggressivo ad inizio partita ma nonostante questo la partita e terminata in Draw dopo un ora con le stesse dinamiche dei pareggi citati.     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">     </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +251,30 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -416,7 +494,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="4" applyBorder="1"/>
@@ -528,14 +606,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
-    <cellStyle name="60% - Accent3" xfId="3" builtinId="40"/>
-    <cellStyle name="60% - Accent4" xfId="4" builtinId="44"/>
-    <cellStyle name="60% - Accent6" xfId="5" builtinId="52"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Colore 1" xfId="1" builtinId="31"/>
+    <cellStyle name="60% - Colore 2" xfId="2" builtinId="36"/>
+    <cellStyle name="60% - Colore 3" xfId="3" builtinId="40"/>
+    <cellStyle name="60% - Colore 4" xfId="4" builtinId="44"/>
+    <cellStyle name="60% - Colore 6" xfId="5" builtinId="52"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -600,7 +684,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -896,18 +980,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{028B81F1-ACA3-4C72-9A53-A89403C903EE}">
-  <dimension ref="A1:Q88"/>
+  <dimension ref="A1:Q112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="75" workbookViewId="0">
-      <selection activeCell="N80" sqref="N80"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="75" workbookViewId="0">
+      <selection activeCell="O108" sqref="O108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21">
@@ -1121,7 +1205,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" ht="19">
+    <row r="10" spans="1:17" ht="18.75">
       <c r="A10" s="8" t="s">
         <v>10</v>
       </c>
@@ -1382,7 +1466,7 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="1:17" ht="19">
+    <row r="21" spans="1:17" ht="18.75">
       <c r="A21" s="8" t="s">
         <v>10</v>
       </c>
@@ -1643,7 +1727,7 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="1:17" ht="19">
+    <row r="32" spans="1:17" ht="18.75">
       <c r="A32" s="8" t="s">
         <v>18</v>
       </c>
@@ -1880,7 +1964,7 @@
       <c r="J42" s="23"/>
       <c r="K42" s="24"/>
     </row>
-    <row r="43" spans="1:17" ht="19">
+    <row r="43" spans="1:17" ht="18.75">
       <c r="A43" s="8" t="s">
         <v>22</v>
       </c>
@@ -2070,7 +2154,7 @@
       <c r="J53" s="23"/>
       <c r="K53" s="24"/>
     </row>
-    <row r="54" spans="1:11" ht="19">
+    <row r="54" spans="1:11" ht="18.75">
       <c r="A54" s="8" t="s">
         <v>24</v>
       </c>
@@ -2085,7 +2169,7 @@
       <c r="J54" s="9"/>
       <c r="K54" s="10"/>
     </row>
-    <row r="55" spans="1:11" ht="19">
+    <row r="55" spans="1:11" ht="18.75">
       <c r="A55" s="6" t="s">
         <v>29</v>
       </c>
@@ -2275,7 +2359,7 @@
       <c r="J65" s="23"/>
       <c r="K65" s="24"/>
     </row>
-    <row r="66" spans="1:11" ht="19">
+    <row r="66" spans="1:11" ht="18.75">
       <c r="A66" s="8" t="s">
         <v>27</v>
       </c>
@@ -2463,7 +2547,7 @@
       <c r="J76" s="23"/>
       <c r="K76" s="24"/>
     </row>
-    <row r="77" spans="1:11" ht="19">
+    <row r="77" spans="1:11" ht="18.75">
       <c r="A77" s="8" t="s">
         <v>10</v>
       </c>
@@ -2653,7 +2737,7 @@
       <c r="J87" s="23"/>
       <c r="K87" s="24"/>
     </row>
-    <row r="88" spans="1:11" ht="19">
+    <row r="88" spans="1:11" ht="18.75">
       <c r="A88" s="8" t="s">
         <v>32</v>
       </c>
@@ -2668,86 +2752,486 @@
       <c r="J88" s="9"/>
       <c r="K88" s="10"/>
     </row>
+    <row r="90" spans="1:11" ht="21">
+      <c r="A90" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B90" s="12"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="12"/>
+      <c r="G90" s="12"/>
+      <c r="H90" s="12"/>
+      <c r="I90" s="12"/>
+      <c r="J90" s="12"/>
+      <c r="K90" s="13"/>
+    </row>
+    <row r="91" spans="1:11">
+      <c r="A91" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B91" s="15"/>
+      <c r="C91" s="16"/>
+      <c r="D91" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E91" s="15"/>
+      <c r="F91" s="16"/>
+      <c r="G91" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H91" s="15"/>
+      <c r="I91" s="15"/>
+      <c r="J91" s="15"/>
+      <c r="K91" s="16"/>
+    </row>
+    <row r="92" spans="1:11">
+      <c r="A92" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B92" s="18"/>
+      <c r="C92" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E92" s="18"/>
+      <c r="F92" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G92" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="H92" s="20"/>
+      <c r="I92" s="20"/>
+      <c r="J92" s="20"/>
+      <c r="K92" s="21"/>
+    </row>
+    <row r="93" spans="1:11">
+      <c r="A93" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" s="26"/>
+      <c r="C93" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D93" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E93" s="26"/>
+      <c r="F93" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G93" s="22"/>
+      <c r="H93" s="23"/>
+      <c r="I93" s="23"/>
+      <c r="J93" s="23"/>
+      <c r="K93" s="24"/>
+    </row>
+    <row r="94" spans="1:11">
+      <c r="A94" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B94" s="26"/>
+      <c r="C94" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D94" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E94" s="26"/>
+      <c r="F94" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="G94" s="22"/>
+      <c r="H94" s="23"/>
+      <c r="I94" s="23"/>
+      <c r="J94" s="23"/>
+      <c r="K94" s="24"/>
+    </row>
+    <row r="95" spans="1:11">
+      <c r="A95" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B95" s="29"/>
+      <c r="C95" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="D95" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" s="29"/>
+      <c r="F95" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="G95" s="22"/>
+      <c r="H95" s="23"/>
+      <c r="I95" s="23"/>
+      <c r="J95" s="23"/>
+      <c r="K95" s="24"/>
+    </row>
+    <row r="96" spans="1:11">
+      <c r="A96" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B96" s="26"/>
+      <c r="C96" s="4">
+        <v>0</v>
+      </c>
+      <c r="D96" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E96" s="26"/>
+      <c r="F96" s="4">
+        <v>2</v>
+      </c>
+      <c r="G96" s="22"/>
+      <c r="H96" s="23"/>
+      <c r="I96" s="23"/>
+      <c r="J96" s="23"/>
+      <c r="K96" s="24"/>
+    </row>
+    <row r="97" spans="1:11">
+      <c r="A97" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B97" s="26"/>
+      <c r="C97" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="D97" s="27"/>
+      <c r="E97" s="26"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="22"/>
+      <c r="H97" s="23"/>
+      <c r="I97" s="23"/>
+      <c r="J97" s="23"/>
+      <c r="K97" s="24"/>
+    </row>
+    <row r="98" spans="1:11">
+      <c r="A98" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B98" s="31"/>
+      <c r="C98" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D98" s="30"/>
+      <c r="E98" s="31"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="22"/>
+      <c r="H98" s="23"/>
+      <c r="I98" s="23"/>
+      <c r="J98" s="23"/>
+      <c r="K98" s="24"/>
+    </row>
+    <row r="99" spans="1:11" ht="18.75">
+      <c r="A99" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B99" s="9"/>
+      <c r="C99" s="9"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
+      <c r="G99" s="9"/>
+      <c r="H99" s="9"/>
+      <c r="I99" s="9"/>
+      <c r="J99" s="9"/>
+      <c r="K99" s="10"/>
+    </row>
+    <row r="103" spans="1:11" ht="21">
+      <c r="A103" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B103" s="12"/>
+      <c r="C103" s="12"/>
+      <c r="D103" s="12"/>
+      <c r="E103" s="12"/>
+      <c r="F103" s="12"/>
+      <c r="G103" s="12"/>
+      <c r="H103" s="12"/>
+      <c r="I103" s="12"/>
+      <c r="J103" s="12"/>
+      <c r="K103" s="13"/>
+    </row>
+    <row r="104" spans="1:11">
+      <c r="A104" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B104" s="15"/>
+      <c r="C104" s="16"/>
+      <c r="D104" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E104" s="15"/>
+      <c r="F104" s="16"/>
+      <c r="G104" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H104" s="15"/>
+      <c r="I104" s="15"/>
+      <c r="J104" s="15"/>
+      <c r="K104" s="16"/>
+    </row>
+    <row r="105" spans="1:11">
+      <c r="A105" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B105" s="18"/>
+      <c r="C105" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D105" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E105" s="18"/>
+      <c r="F105" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G105" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="H105" s="20"/>
+      <c r="I105" s="20"/>
+      <c r="J105" s="20"/>
+      <c r="K105" s="21"/>
+    </row>
+    <row r="106" spans="1:11">
+      <c r="A106" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B106" s="26"/>
+      <c r="C106" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D106" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E106" s="26"/>
+      <c r="F106" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G106" s="22"/>
+      <c r="H106" s="23"/>
+      <c r="I106" s="23"/>
+      <c r="J106" s="23"/>
+      <c r="K106" s="24"/>
+    </row>
+    <row r="107" spans="1:11">
+      <c r="A107" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B107" s="26"/>
+      <c r="C107" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D107" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E107" s="26"/>
+      <c r="F107" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="G107" s="22"/>
+      <c r="H107" s="23"/>
+      <c r="I107" s="23"/>
+      <c r="J107" s="23"/>
+      <c r="K107" s="24"/>
+    </row>
+    <row r="108" spans="1:11">
+      <c r="A108" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108" s="29"/>
+      <c r="C108" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D108" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="E108" s="29"/>
+      <c r="F108" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="G108" s="22"/>
+      <c r="H108" s="23"/>
+      <c r="I108" s="23"/>
+      <c r="J108" s="23"/>
+      <c r="K108" s="24"/>
+    </row>
+    <row r="109" spans="1:11">
+      <c r="A109" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B109" s="26"/>
+      <c r="C109" s="4">
+        <v>0</v>
+      </c>
+      <c r="D109" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E109" s="26"/>
+      <c r="F109" s="4">
+        <v>2</v>
+      </c>
+      <c r="G109" s="22"/>
+      <c r="H109" s="23"/>
+      <c r="I109" s="23"/>
+      <c r="J109" s="23"/>
+      <c r="K109" s="24"/>
+    </row>
+    <row r="110" spans="1:11">
+      <c r="A110" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B110" s="26"/>
+      <c r="C110" s="4">
+        <v>2</v>
+      </c>
+      <c r="D110" s="27"/>
+      <c r="E110" s="26"/>
+      <c r="F110" s="4"/>
+      <c r="G110" s="22"/>
+      <c r="H110" s="23"/>
+      <c r="I110" s="23"/>
+      <c r="J110" s="23"/>
+      <c r="K110" s="24"/>
+    </row>
+    <row r="111" spans="1:11">
+      <c r="A111" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B111" s="31"/>
+      <c r="C111" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D111" s="30"/>
+      <c r="E111" s="31"/>
+      <c r="F111" s="2"/>
+      <c r="G111" s="22"/>
+      <c r="H111" s="23"/>
+      <c r="I111" s="23"/>
+      <c r="J111" s="23"/>
+      <c r="K111" s="24"/>
+    </row>
+    <row r="112" spans="1:11" ht="18.75">
+      <c r="A112" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B112" s="9"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="9"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="9"/>
+      <c r="G112" s="9"/>
+      <c r="H112" s="9"/>
+      <c r="I112" s="9"/>
+      <c r="J112" s="9"/>
+      <c r="K112" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="160">
-    <mergeCell ref="A77:K77"/>
-    <mergeCell ref="A68:K68"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="G69:K69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="G70:K76"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="A54:K54"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="G46:K46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="G47:K53"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A45:K45"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="G36:K42"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A32:K32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K20"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:E16"/>
+  <mergeCells count="200">
+    <mergeCell ref="A112:K112"/>
+    <mergeCell ref="A103:K103"/>
+    <mergeCell ref="A104:C104"/>
+    <mergeCell ref="D104:F104"/>
+    <mergeCell ref="G104:K104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="G105:K111"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="A99:K99"/>
+    <mergeCell ref="A90:K90"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="G91:K91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="G92:K98"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="A88:K88"/>
+    <mergeCell ref="A79:K79"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="G80:K80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="G81:K87"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="G58:K58"/>
+    <mergeCell ref="G59:K65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="A66:K66"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="G3:K9"/>
@@ -2772,67 +3256,87 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A57:K57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="G58:K58"/>
-    <mergeCell ref="G59:K65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="A66:K66"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A88:K88"/>
-    <mergeCell ref="A79:K79"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="G80:K80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="G81:K87"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="A32:K32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K20"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A45:K45"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:K42"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A54:K54"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="G46:K46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="G47:K53"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="A77:K77"/>
+    <mergeCell ref="A68:K68"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="G69:K69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="G70:K76"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:E76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update with a new test
</commit_message>
<xml_diff>
--- a/Tablut/TestTablut.xlsx
+++ b/Tablut/TestTablut.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\Tablut\Tablut\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milo\Desktop\Tablut\Tablut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604FF609-82E7-4442-A843-DBC29B287E3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A268FF2A-E05C-4AB8-B784-864BC89C3B08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
+    <workbookView xWindow="5220" yWindow="690" windowWidth="21600" windowHeight="11385" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="41">
   <si>
     <t>KingEncirclement</t>
   </si>
@@ -190,12 +190,21 @@
       <t xml:space="preserve">     </t>
     </r>
   </si>
+  <si>
+    <t>RESULT: WHITE WIN</t>
+  </si>
+  <si>
+    <t>Visto che i miei risultati sono diversi dai vostri li ho separati così non bisogna cercarli in mezzo ai vostri</t>
+  </si>
+  <si>
+    <t>Partita durata un'ora e mezza, il bianco si è mosso bene ed è riuscito a vincere. I pesi sono quelli indicati ma è stata modificata la funzione getWhiteLineScore. I nuovi pesi per lo score sono  citadels -1, throne -1, black -1, escapes +1 e white0  (max=2, min= -24)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,6 +284,14 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -494,7 +511,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="4" applyBorder="1"/>
@@ -540,45 +557,51 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -606,12 +629,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Colore 1" xfId="1" builtinId="31"/>
@@ -980,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{028B81F1-ACA3-4C72-9A53-A89403C903EE}">
-  <dimension ref="A1:Q112"/>
+  <dimension ref="A1:AA112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="75" workbookViewId="0">
-      <selection activeCell="O108" sqref="O108"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -994,7 +1024,7 @@
     <col min="5" max="5" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="21">
+    <row r="1" spans="1:27" ht="21">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -1008,8 +1038,21 @@
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
       <c r="K1" s="13"/>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="Q1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="13"/>
+    </row>
+    <row r="2" spans="1:27">
       <c r="A2" s="14" t="s">
         <v>11</v>
       </c>
@@ -1020,15 +1063,32 @@
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="16"/>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="34"/>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="36"/>
+      <c r="Q2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="15"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="U2" s="15"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="36"/>
+    </row>
+    <row r="3" spans="1:27" ht="15" customHeight="1">
       <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
@@ -1043,15 +1103,41 @@
       <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="37"/>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="39"/>
+      <c r="N3" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="43"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" s="18"/>
+      <c r="S3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="U3" s="18"/>
+      <c r="V3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W3" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="39"/>
+    </row>
+    <row r="4" spans="1:27">
       <c r="A4" s="25" t="s">
         <v>0</v>
       </c>
@@ -1066,19 +1152,37 @@
       <c r="F4" s="4">
         <v>0.2</v>
       </c>
-      <c r="G4" s="38"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="42"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" s="26"/>
+      <c r="S4" s="4">
+        <v>0</v>
+      </c>
+      <c r="T4" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="U4" s="26"/>
+      <c r="V4" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W4" s="40"/>
+      <c r="X4" s="41"/>
+      <c r="Y4" s="41"/>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="42"/>
+    </row>
+    <row r="5" spans="1:27">
       <c r="A5" s="27" t="s">
         <v>1</v>
       </c>
@@ -1093,19 +1197,37 @@
       <c r="F5" s="4">
         <v>0.6</v>
       </c>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="42"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" s="26"/>
+      <c r="S5" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="T5" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="U5" s="26"/>
+      <c r="V5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="W5" s="40"/>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="41"/>
+      <c r="Z5" s="41"/>
+      <c r="AA5" s="42"/>
+    </row>
+    <row r="6" spans="1:27">
       <c r="A6" s="28" t="s">
         <v>2</v>
       </c>
@@ -1120,19 +1242,37 @@
       <c r="F6" s="3">
         <v>1.5</v>
       </c>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="42"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="44"/>
+      <c r="Q6" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="R6" s="29"/>
+      <c r="S6" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="T6" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" s="29"/>
+      <c r="V6" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="W6" s="40"/>
+      <c r="X6" s="41"/>
+      <c r="Y6" s="41"/>
+      <c r="Z6" s="41"/>
+      <c r="AA6" s="42"/>
+    </row>
+    <row r="7" spans="1:27">
       <c r="A7" s="27" t="s">
         <v>3</v>
       </c>
@@ -1147,19 +1287,37 @@
       <c r="F7" s="4">
         <v>2</v>
       </c>
-      <c r="G7" s="38"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="42"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="N7" s="45"/>
+      <c r="O7" s="45"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="R7" s="26"/>
+      <c r="S7" s="4">
+        <v>0</v>
+      </c>
+      <c r="T7" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="U7" s="26"/>
+      <c r="V7" s="4">
+        <v>2</v>
+      </c>
+      <c r="W7" s="40"/>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="41"/>
+      <c r="Z7" s="41"/>
+      <c r="AA7" s="42"/>
+    </row>
+    <row r="8" spans="1:27">
       <c r="A8" s="27" t="s">
         <v>4</v>
       </c>
@@ -1170,19 +1328,33 @@
       <c r="D8" s="27"/>
       <c r="E8" s="26"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="42"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="Q8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="R8" s="26"/>
+      <c r="S8" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="T8" s="27"/>
+      <c r="U8" s="26"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="40"/>
+      <c r="X8" s="41"/>
+      <c r="Y8" s="41"/>
+      <c r="Z8" s="41"/>
+      <c r="AA8" s="42"/>
+    </row>
+    <row r="9" spans="1:27">
       <c r="A9" s="30" t="s">
         <v>7</v>
       </c>
@@ -1193,19 +1365,33 @@
       <c r="D9" s="30"/>
       <c r="E9" s="31"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="42"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:17" ht="18.75">
+      <c r="Q9" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="R9" s="31"/>
+      <c r="S9" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T9" s="30"/>
+      <c r="U9" s="31"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="40"/>
+      <c r="X9" s="41"/>
+      <c r="Y9" s="41"/>
+      <c r="Z9" s="41"/>
+      <c r="AA9" s="42"/>
+    </row>
+    <row r="10" spans="1:27" ht="18.75">
       <c r="A10" s="8" t="s">
         <v>10</v>
       </c>
@@ -1224,9 +1410,21 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="Q10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="10"/>
+    </row>
+    <row r="11" spans="1:27">
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1237,7 +1435,7 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="1:17" ht="21">
+    <row r="12" spans="1:27" ht="21">
       <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
@@ -1258,24 +1456,24 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="32" t="s">
+    <row r="13" spans="1:27">
+      <c r="A13" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="32" t="s">
+      <c r="B13" s="35"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="33"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="32" t="s">
+      <c r="E13" s="35"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="34"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="36"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -1283,7 +1481,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:27">
       <c r="A14" s="17" t="s">
         <v>6</v>
       </c>
@@ -1298,21 +1496,22 @@
       <c r="F14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="35" t="s">
+      <c r="G14" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="37"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="V14" s="47"/>
+    </row>
+    <row r="15" spans="1:27">
       <c r="A15" s="25" t="s">
         <v>0</v>
       </c>
@@ -1327,11 +1526,11 @@
       <c r="F15" s="4">
         <v>0.2</v>
       </c>
-      <c r="G15" s="38"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="42"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1339,7 +1538,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:27">
       <c r="A16" s="27" t="s">
         <v>1</v>
       </c>
@@ -1354,11 +1553,11 @@
       <c r="F16" s="4">
         <v>0.6</v>
       </c>
-      <c r="G16" s="38"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="42"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -1381,11 +1580,11 @@
       <c r="F17" s="3">
         <v>1.5</v>
       </c>
-      <c r="G17" s="38"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="42"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -1408,11 +1607,11 @@
       <c r="F18" s="4">
         <v>2</v>
       </c>
-      <c r="G18" s="38"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="42"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1431,11 +1630,11 @@
       <c r="D19" s="27"/>
       <c r="E19" s="26"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="42"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -1454,11 +1653,11 @@
       <c r="D20" s="30"/>
       <c r="E20" s="31"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="42"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -1559,7 +1758,7 @@
       <c r="F25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="33" t="s">
         <v>19</v>
       </c>
       <c r="H25" s="20"/>
@@ -1820,7 +2019,7 @@
       <c r="F36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G36" s="19" t="s">
+      <c r="G36" s="33" t="s">
         <v>21</v>
       </c>
       <c r="H36" s="20"/>
@@ -2028,7 +2227,7 @@
       <c r="F47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G47" s="19" t="s">
+      <c r="G47" s="33" t="s">
         <v>31</v>
       </c>
       <c r="H47" s="20"/>
@@ -2233,7 +2432,7 @@
       <c r="F59" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G59" s="19" t="s">
+      <c r="G59" s="33" t="s">
         <v>26</v>
       </c>
       <c r="H59" s="20"/>
@@ -2423,7 +2622,7 @@
       <c r="F70" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G70" s="19"/>
+      <c r="G70" s="33"/>
       <c r="H70" s="20"/>
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
@@ -2611,7 +2810,7 @@
       <c r="F81" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G81" s="19" t="s">
+      <c r="G81" s="33" t="s">
         <v>33</v>
       </c>
       <c r="H81" s="20"/>
@@ -2801,7 +3000,7 @@
       <c r="F92" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G92" s="41" t="s">
+      <c r="G92" s="32" t="s">
         <v>35</v>
       </c>
       <c r="H92" s="20"/>
@@ -2991,7 +3190,7 @@
       <c r="F105" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G105" s="42" t="s">
+      <c r="G105" s="19" t="s">
         <v>37</v>
       </c>
       <c r="H105" s="20"/>
@@ -3133,105 +3332,106 @@
       <c r="K112" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="200">
-    <mergeCell ref="A112:K112"/>
-    <mergeCell ref="A103:K103"/>
-    <mergeCell ref="A104:C104"/>
-    <mergeCell ref="D104:F104"/>
-    <mergeCell ref="G104:K104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="G105:K111"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="A99:K99"/>
-    <mergeCell ref="A90:K90"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="G91:K91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="G92:K98"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="A88:K88"/>
-    <mergeCell ref="A79:K79"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="G80:K80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="G81:K87"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="A57:K57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="G58:K58"/>
-    <mergeCell ref="G59:K65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="A66:K66"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
+  <mergeCells count="221">
+    <mergeCell ref="Q10:AA10"/>
+    <mergeCell ref="N3:P6"/>
+    <mergeCell ref="Q1:AA1"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="W2:AA2"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="W3:AA9"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="A77:K77"/>
+    <mergeCell ref="A68:K68"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="G69:K69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="G70:K76"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="A54:K54"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="G46:K46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="G47:K53"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A45:K45"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:K42"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A32:K32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K20"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:E16"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="G3:K9"/>
@@ -3256,84 +3456,104 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A32:K32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K20"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A45:K45"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="G36:K42"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A54:K54"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="G46:K46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="G47:K53"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="A77:K77"/>
-    <mergeCell ref="A68:K68"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="G69:K69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="G70:K76"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="G58:K58"/>
+    <mergeCell ref="G59:K65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="A66:K66"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A88:K88"/>
+    <mergeCell ref="A79:K79"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="G80:K80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="G81:K87"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="A99:K99"/>
+    <mergeCell ref="A90:K90"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="G91:K91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="G92:K98"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="A112:K112"/>
+    <mergeCell ref="A103:K103"/>
+    <mergeCell ref="A104:C104"/>
+    <mergeCell ref="D104:F104"/>
+    <mergeCell ref="G104:K104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="G105:K111"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D111:E111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update with some tests
</commit_message>
<xml_diff>
--- a/Tablut/TestTablut.xlsx
+++ b/Tablut/TestTablut.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milo\Desktop\Tablut\Tablut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED563FE-21AC-4966-B47A-DC885B9368A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70526ABD-F471-413F-8C39-E450316AA003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="690" windowWidth="21600" windowHeight="11385" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
+    <workbookView xWindow="4590" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="44">
   <si>
     <t>KingEncirclement</t>
   </si>
@@ -200,7 +200,13 @@
     <t>Partita durata un'ora e mezza, il bianco si è mosso bene ed è riuscito a vincere. I pesi sono quelli indicati ma è stata modificata la funzione getWhiteLineScore. I nuovi pesi per lo score sono  citadels -1, throne -1, black -1, escapes +1 e white0  (max=2, min= -24)</t>
   </si>
   <si>
-    <t>Il bianco ha impiegato anche meno tempo a vincere, quindi i pesi variati del nero lo hanno peggiorato.</t>
+    <t>Il tempo impiegato dal bianco per vincere è pressocchè lo stesso.</t>
+  </si>
+  <si>
+    <t>Variazione del test 1 ma con la kingPositioning del balck variata: citadels +1, throne +1, black 0, white -1, escapes -1, empty 0</t>
+  </si>
+  <si>
+    <t>La partita è durata quasi 40 minuti, cioè meno del solito</t>
   </si>
 </sst>
 </file>
@@ -506,7 +512,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="4" applyBorder="1"/>
@@ -543,6 +549,60 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -552,24 +612,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -585,13 +630,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
@@ -1007,7 +1046,7 @@
   <dimension ref="A1:AA112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12:AA12"/>
+      <selection activeCell="W47" sqref="W47:AA53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1047,245 +1086,245 @@
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="16" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19" t="s">
+      <c r="E2" s="35"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="21"/>
-      <c r="Q2" s="16" t="s">
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="18"/>
+      <c r="Q2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="17"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="16" t="s">
+      <c r="R2" s="35"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="17"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="19" t="s">
+      <c r="U2" s="35"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="21"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="18"/>
     </row>
     <row r="3" spans="1:27" ht="15" customHeight="1">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="23"/>
+      <c r="E3" s="37"/>
       <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="26"/>
-      <c r="N3" s="45" t="s">
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="39"/>
+      <c r="N3" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="O3" s="45"/>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="22" t="s">
+      <c r="O3" s="56"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="23"/>
+      <c r="R3" s="37"/>
       <c r="S3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="T3" s="22" t="s">
+      <c r="T3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="U3" s="23"/>
+      <c r="U3" s="37"/>
       <c r="V3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="W3" s="24" t="s">
+      <c r="W3" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="26"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="39"/>
     </row>
     <row r="4" spans="1:27">
       <c r="A4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="31"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="4">
         <v>0.1</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="43"/>
       <c r="F4" s="4">
         <v>0.2</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="29"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="42"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="46"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="57"/>
       <c r="Q4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="R4" s="31"/>
+      <c r="R4" s="43"/>
       <c r="S4" s="4">
         <v>0</v>
       </c>
       <c r="T4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="31"/>
+      <c r="U4" s="43"/>
       <c r="V4" s="4">
         <v>0.2</v>
       </c>
-      <c r="W4" s="27"/>
-      <c r="X4" s="28"/>
-      <c r="Y4" s="28"/>
-      <c r="Z4" s="28"/>
-      <c r="AA4" s="29"/>
+      <c r="W4" s="40"/>
+      <c r="X4" s="41"/>
+      <c r="Y4" s="41"/>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="42"/>
     </row>
     <row r="5" spans="1:27">
       <c r="A5" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="31"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="4">
         <v>0.2</v>
       </c>
       <c r="D5" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="43"/>
       <c r="F5" s="4">
         <v>0.6</v>
       </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="29"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="42"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="46"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="56"/>
+      <c r="P5" s="57"/>
       <c r="Q5" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="R5" s="31"/>
+      <c r="R5" s="43"/>
       <c r="S5" s="4">
         <v>0.2</v>
       </c>
       <c r="T5" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="U5" s="31"/>
+      <c r="U5" s="43"/>
       <c r="V5" s="4">
         <v>0.6</v>
       </c>
-      <c r="W5" s="27"/>
-      <c r="X5" s="28"/>
-      <c r="Y5" s="28"/>
-      <c r="Z5" s="28"/>
-      <c r="AA5" s="29"/>
+      <c r="W5" s="40"/>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="41"/>
+      <c r="Z5" s="41"/>
+      <c r="AA5" s="42"/>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="34"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="3">
         <v>0.4</v>
       </c>
-      <c r="D6" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="34"/>
+      <c r="D6" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="45"/>
       <c r="F6" s="3">
         <v>1.5</v>
       </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="29"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="42"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="33" t="s">
+      <c r="N6" s="56"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="R6" s="34"/>
+      <c r="R6" s="45"/>
       <c r="S6" s="3">
         <v>0.6</v>
       </c>
-      <c r="T6" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="U6" s="34"/>
+      <c r="T6" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" s="45"/>
       <c r="V6" s="3">
         <v>1.5</v>
       </c>
-      <c r="W6" s="27"/>
-      <c r="X6" s="28"/>
-      <c r="Y6" s="28"/>
-      <c r="Z6" s="28"/>
-      <c r="AA6" s="29"/>
+      <c r="W6" s="40"/>
+      <c r="X6" s="41"/>
+      <c r="Y6" s="41"/>
+      <c r="Z6" s="41"/>
+      <c r="AA6" s="42"/>
     </row>
     <row r="7" spans="1:27">
       <c r="A7" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="31"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="4">
         <v>0.5</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="43"/>
       <c r="F7" s="4">
         <v>2</v>
       </c>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="29"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="42"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="8"/>
@@ -1294,39 +1333,39 @@
       <c r="Q7" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="R7" s="31"/>
+      <c r="R7" s="43"/>
       <c r="S7" s="4">
         <v>0</v>
       </c>
       <c r="T7" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="U7" s="31"/>
+      <c r="U7" s="43"/>
       <c r="V7" s="4">
         <v>2</v>
       </c>
-      <c r="W7" s="27"/>
-      <c r="X7" s="28"/>
-      <c r="Y7" s="28"/>
-      <c r="Z7" s="28"/>
-      <c r="AA7" s="29"/>
+      <c r="W7" s="40"/>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="41"/>
+      <c r="Z7" s="41"/>
+      <c r="AA7" s="42"/>
     </row>
     <row r="8" spans="1:27">
       <c r="A8" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="31"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="4">
         <v>1</v>
       </c>
       <c r="D8" s="32"/>
-      <c r="E8" s="31"/>
+      <c r="E8" s="43"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="29"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="42"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1335,55 +1374,55 @@
       <c r="Q8" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="R8" s="31"/>
+      <c r="R8" s="43"/>
       <c r="S8" s="4">
         <v>1.4</v>
       </c>
       <c r="T8" s="32"/>
-      <c r="U8" s="31"/>
+      <c r="U8" s="43"/>
       <c r="V8" s="4"/>
-      <c r="W8" s="27"/>
-      <c r="X8" s="28"/>
-      <c r="Y8" s="28"/>
-      <c r="Z8" s="28"/>
-      <c r="AA8" s="29"/>
+      <c r="W8" s="40"/>
+      <c r="X8" s="41"/>
+      <c r="Y8" s="41"/>
+      <c r="Z8" s="41"/>
+      <c r="AA8" s="42"/>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="36"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="2">
         <v>0</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="47"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="29"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="42"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="35" t="s">
+      <c r="Q9" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="R9" s="36"/>
+      <c r="R9" s="47"/>
       <c r="S9" s="2">
         <v>0.4</v>
       </c>
-      <c r="T9" s="35"/>
-      <c r="U9" s="36"/>
+      <c r="T9" s="46"/>
+      <c r="U9" s="47"/>
       <c r="V9" s="2"/>
-      <c r="W9" s="27"/>
-      <c r="X9" s="28"/>
-      <c r="Y9" s="28"/>
-      <c r="Z9" s="28"/>
-      <c r="AA9" s="29"/>
+      <c r="W9" s="40"/>
+      <c r="X9" s="41"/>
+      <c r="Y9" s="41"/>
+      <c r="Z9" s="41"/>
+      <c r="AA9" s="42"/>
     </row>
     <row r="10" spans="1:27" ht="18.75">
       <c r="A10" s="10" t="s">
@@ -1463,115 +1502,115 @@
       <c r="AA12" s="15"/>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="19" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="19" t="s">
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="21"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="18"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-      <c r="Q13" s="16" t="s">
+      <c r="Q13" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="R13" s="17"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="16" t="s">
+      <c r="R13" s="35"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="U13" s="17"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="19" t="s">
+      <c r="U13" s="35"/>
+      <c r="V13" s="36"/>
+      <c r="W13" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="X13" s="20"/>
-      <c r="Y13" s="20"/>
-      <c r="Z13" s="20"/>
-      <c r="AA13" s="21"/>
+      <c r="X13" s="17"/>
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="17"/>
+      <c r="AA13" s="18"/>
     </row>
     <row r="14" spans="1:27">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="23"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="23"/>
+      <c r="E14" s="37"/>
       <c r="F14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="24" t="s">
+      <c r="G14" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="26"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-      <c r="Q14" s="22" t="s">
+      <c r="Q14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="R14" s="23"/>
+      <c r="R14" s="37"/>
       <c r="S14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="T14" s="22" t="s">
+      <c r="T14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="U14" s="23"/>
+      <c r="U14" s="37"/>
       <c r="V14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="W14" s="24" t="s">
+      <c r="W14" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="X14" s="25"/>
-      <c r="Y14" s="25"/>
-      <c r="Z14" s="25"/>
-      <c r="AA14" s="26"/>
+      <c r="X14" s="38"/>
+      <c r="Y14" s="38"/>
+      <c r="Z14" s="38"/>
+      <c r="AA14" s="39"/>
     </row>
     <row r="15" spans="1:27">
       <c r="A15" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="31"/>
+      <c r="B15" s="43"/>
       <c r="C15" s="4">
         <v>0.1</v>
       </c>
       <c r="D15" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="31"/>
+      <c r="E15" s="43"/>
       <c r="F15" s="4">
         <v>0.2</v>
       </c>
-      <c r="G15" s="27"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="29"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="42"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1580,43 +1619,43 @@
       <c r="Q15" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="R15" s="31"/>
+      <c r="R15" s="43"/>
       <c r="S15" s="4">
         <v>0</v>
       </c>
       <c r="T15" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="U15" s="31"/>
+      <c r="U15" s="43"/>
       <c r="V15" s="4">
         <v>0.4</v>
       </c>
-      <c r="W15" s="27"/>
-      <c r="X15" s="28"/>
-      <c r="Y15" s="28"/>
-      <c r="Z15" s="28"/>
-      <c r="AA15" s="29"/>
+      <c r="W15" s="40"/>
+      <c r="X15" s="41"/>
+      <c r="Y15" s="41"/>
+      <c r="Z15" s="41"/>
+      <c r="AA15" s="42"/>
     </row>
     <row r="16" spans="1:27">
       <c r="A16" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="31"/>
+      <c r="B16" s="43"/>
       <c r="C16" s="4">
         <v>0.2</v>
       </c>
       <c r="D16" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="31"/>
+      <c r="E16" s="43"/>
       <c r="F16" s="4">
         <v>0.6</v>
       </c>
-      <c r="G16" s="27"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="29"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="42"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -1625,88 +1664,88 @@
       <c r="Q16" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="R16" s="31"/>
+      <c r="R16" s="43"/>
       <c r="S16" s="4">
         <v>0.2</v>
       </c>
       <c r="T16" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="U16" s="31"/>
+      <c r="U16" s="43"/>
       <c r="V16" s="4">
         <v>1</v>
       </c>
-      <c r="W16" s="27"/>
-      <c r="X16" s="28"/>
-      <c r="Y16" s="28"/>
-      <c r="Z16" s="28"/>
-      <c r="AA16" s="29"/>
+      <c r="W16" s="40"/>
+      <c r="X16" s="41"/>
+      <c r="Y16" s="41"/>
+      <c r="Z16" s="41"/>
+      <c r="AA16" s="42"/>
     </row>
     <row r="17" spans="1:27">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="34"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="3">
         <v>0.5</v>
       </c>
-      <c r="D17" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="34"/>
+      <c r="D17" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="45"/>
       <c r="F17" s="3">
         <v>1.5</v>
       </c>
-      <c r="G17" s="27"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="29"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="42"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
-      <c r="Q17" s="33" t="s">
+      <c r="Q17" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="R17" s="34"/>
+      <c r="R17" s="45"/>
       <c r="S17" s="3">
         <v>0.6</v>
       </c>
-      <c r="T17" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="U17" s="34"/>
+      <c r="T17" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="U17" s="45"/>
       <c r="V17" s="3">
         <v>1.5</v>
       </c>
-      <c r="W17" s="27"/>
-      <c r="X17" s="28"/>
-      <c r="Y17" s="28"/>
-      <c r="Z17" s="28"/>
-      <c r="AA17" s="29"/>
+      <c r="W17" s="40"/>
+      <c r="X17" s="41"/>
+      <c r="Y17" s="41"/>
+      <c r="Z17" s="41"/>
+      <c r="AA17" s="42"/>
     </row>
     <row r="18" spans="1:27">
       <c r="A18" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="31"/>
+      <c r="B18" s="43"/>
       <c r="C18" s="4">
         <v>0.3</v>
       </c>
       <c r="D18" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="31"/>
+      <c r="E18" s="43"/>
       <c r="F18" s="4">
         <v>2</v>
       </c>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="29"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="42"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1715,39 +1754,39 @@
       <c r="Q18" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="R18" s="31"/>
+      <c r="R18" s="43"/>
       <c r="S18" s="4">
         <v>0</v>
       </c>
       <c r="T18" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="U18" s="31"/>
+      <c r="U18" s="43"/>
       <c r="V18" s="4">
         <v>2</v>
       </c>
-      <c r="W18" s="27"/>
-      <c r="X18" s="28"/>
-      <c r="Y18" s="28"/>
-      <c r="Z18" s="28"/>
-      <c r="AA18" s="29"/>
+      <c r="W18" s="40"/>
+      <c r="X18" s="41"/>
+      <c r="Y18" s="41"/>
+      <c r="Z18" s="41"/>
+      <c r="AA18" s="42"/>
     </row>
     <row r="19" spans="1:27">
       <c r="A19" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="31"/>
+      <c r="B19" s="43"/>
       <c r="C19" s="4">
         <v>1</v>
       </c>
       <c r="D19" s="32"/>
-      <c r="E19" s="31"/>
+      <c r="E19" s="43"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="29"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="42"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -1756,55 +1795,55 @@
       <c r="Q19" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="R19" s="31"/>
+      <c r="R19" s="43"/>
       <c r="S19" s="4">
         <v>1.4</v>
       </c>
       <c r="T19" s="32"/>
-      <c r="U19" s="31"/>
+      <c r="U19" s="43"/>
       <c r="V19" s="4"/>
-      <c r="W19" s="27"/>
-      <c r="X19" s="28"/>
-      <c r="Y19" s="28"/>
-      <c r="Z19" s="28"/>
-      <c r="AA19" s="29"/>
+      <c r="W19" s="40"/>
+      <c r="X19" s="41"/>
+      <c r="Y19" s="41"/>
+      <c r="Z19" s="41"/>
+      <c r="AA19" s="42"/>
     </row>
     <row r="20" spans="1:27">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="36"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="2">
         <v>0.7</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="36"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="47"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="29"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="42"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
-      <c r="Q20" s="35" t="s">
+      <c r="Q20" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="R20" s="36"/>
+      <c r="R20" s="47"/>
       <c r="S20" s="2">
         <v>0.4</v>
       </c>
-      <c r="T20" s="35"/>
-      <c r="U20" s="36"/>
+      <c r="T20" s="46"/>
+      <c r="U20" s="47"/>
       <c r="V20" s="2"/>
-      <c r="W20" s="27"/>
-      <c r="X20" s="28"/>
-      <c r="Y20" s="28"/>
-      <c r="Z20" s="28"/>
-      <c r="AA20" s="29"/>
+      <c r="W20" s="40"/>
+      <c r="X20" s="41"/>
+      <c r="Y20" s="41"/>
+      <c r="Z20" s="41"/>
+      <c r="AA20" s="42"/>
     </row>
     <row r="21" spans="1:27" ht="18.75">
       <c r="A21" s="10" t="s">
@@ -1869,215 +1908,363 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
+      <c r="Q23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14"/>
+      <c r="U23" s="14"/>
+      <c r="V23" s="14"/>
+      <c r="W23" s="14"/>
+      <c r="X23" s="14"/>
+      <c r="Y23" s="14"/>
+      <c r="Z23" s="14"/>
+      <c r="AA23" s="15"/>
     </row>
     <row r="24" spans="1:27">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="16" t="s">
+      <c r="B24" s="35"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="16" t="s">
+      <c r="E24" s="35"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="18"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="36"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-    </row>
-    <row r="25" spans="1:27">
-      <c r="A25" s="22" t="s">
+      <c r="Q24" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="R24" s="35"/>
+      <c r="S24" s="36"/>
+      <c r="T24" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="U24" s="35"/>
+      <c r="V24" s="36"/>
+      <c r="W24" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="X24" s="17"/>
+      <c r="Y24" s="17"/>
+      <c r="Z24" s="17"/>
+      <c r="AA24" s="18"/>
+    </row>
+    <row r="25" spans="1:27" ht="15" customHeight="1">
+      <c r="A25" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="23"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="23"/>
+      <c r="E25" s="37"/>
       <c r="F25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="44" t="s">
+      <c r="G25" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="39"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="50"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
+      <c r="Q25" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="R25" s="37"/>
+      <c r="S25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T25" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="U25" s="37"/>
+      <c r="V25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W25" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="X25" s="38"/>
+      <c r="Y25" s="38"/>
+      <c r="Z25" s="38"/>
+      <c r="AA25" s="39"/>
     </row>
     <row r="26" spans="1:27">
       <c r="A26" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="31"/>
+      <c r="B26" s="43"/>
       <c r="C26" s="4">
         <v>0.1</v>
       </c>
       <c r="D26" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="31"/>
+      <c r="E26" s="43"/>
       <c r="F26" s="4">
         <v>0.2</v>
       </c>
-      <c r="G26" s="40"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="42"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="53"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
+      <c r="Q26" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="R26" s="43"/>
+      <c r="S26" s="4">
+        <v>0</v>
+      </c>
+      <c r="T26" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="U26" s="43"/>
+      <c r="V26" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="W26" s="40"/>
+      <c r="X26" s="41"/>
+      <c r="Y26" s="41"/>
+      <c r="Z26" s="41"/>
+      <c r="AA26" s="42"/>
     </row>
     <row r="27" spans="1:27">
       <c r="A27" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="31"/>
+      <c r="B27" s="43"/>
       <c r="C27" s="4">
         <v>0.2</v>
       </c>
       <c r="D27" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="31"/>
+      <c r="E27" s="43"/>
       <c r="F27" s="4">
         <v>0.6</v>
       </c>
-      <c r="G27" s="40"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="42"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="53"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
+      <c r="Q27" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="R27" s="43"/>
+      <c r="S27" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="T27" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="U27" s="43"/>
+      <c r="V27" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="W27" s="40"/>
+      <c r="X27" s="41"/>
+      <c r="Y27" s="41"/>
+      <c r="Z27" s="41"/>
+      <c r="AA27" s="42"/>
     </row>
     <row r="28" spans="1:27">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="34"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="3">
         <v>0.6</v>
       </c>
-      <c r="D28" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" s="34"/>
+      <c r="D28" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="45"/>
       <c r="F28" s="3">
         <v>1.5</v>
       </c>
-      <c r="G28" s="40"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="41"/>
-      <c r="K28" s="42"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="53"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
+      <c r="Q28" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="R28" s="45"/>
+      <c r="S28" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="T28" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="U28" s="45"/>
+      <c r="V28" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="W28" s="40"/>
+      <c r="X28" s="41"/>
+      <c r="Y28" s="41"/>
+      <c r="Z28" s="41"/>
+      <c r="AA28" s="42"/>
     </row>
     <row r="29" spans="1:27">
       <c r="A29" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="31"/>
+      <c r="B29" s="43"/>
       <c r="C29" s="4">
         <v>0</v>
       </c>
       <c r="D29" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="31"/>
+      <c r="E29" s="43"/>
       <c r="F29" s="4">
         <v>2</v>
       </c>
-      <c r="G29" s="40"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="42"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="53"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
+      <c r="Q29" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="R29" s="43"/>
+      <c r="S29" s="4">
+        <v>0</v>
+      </c>
+      <c r="T29" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="U29" s="43"/>
+      <c r="V29" s="4">
+        <v>2</v>
+      </c>
+      <c r="W29" s="40"/>
+      <c r="X29" s="41"/>
+      <c r="Y29" s="41"/>
+      <c r="Z29" s="41"/>
+      <c r="AA29" s="42"/>
     </row>
     <row r="30" spans="1:27">
       <c r="A30" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="31"/>
+      <c r="B30" s="43"/>
       <c r="C30" s="4">
         <v>1.2</v>
       </c>
       <c r="D30" s="32"/>
-      <c r="E30" s="31"/>
+      <c r="E30" s="43"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="42"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="53"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
+      <c r="Q30" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="R30" s="43"/>
+      <c r="S30" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="T30" s="32"/>
+      <c r="U30" s="43"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="40"/>
+      <c r="X30" s="41"/>
+      <c r="Y30" s="41"/>
+      <c r="Z30" s="41"/>
+      <c r="AA30" s="42"/>
     </row>
     <row r="31" spans="1:27">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="36"/>
+      <c r="B31" s="47"/>
       <c r="C31" s="2">
         <v>0.4</v>
       </c>
-      <c r="D31" s="35"/>
-      <c r="E31" s="36"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="47"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="42"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="53"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
+      <c r="Q31" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="R31" s="47"/>
+      <c r="S31" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T31" s="46"/>
+      <c r="U31" s="47"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="40"/>
+      <c r="X31" s="41"/>
+      <c r="Y31" s="41"/>
+      <c r="Z31" s="41"/>
+      <c r="AA31" s="42"/>
     </row>
     <row r="32" spans="1:27" ht="18.75">
       <c r="A32" s="10" t="s">
@@ -2098,9 +2285,21 @@
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-    </row>
-    <row r="33" spans="1:17">
+      <c r="Q32" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+      <c r="W32" s="11"/>
+      <c r="X32" s="11"/>
+      <c r="Y32" s="11"/>
+      <c r="Z32" s="11"/>
+      <c r="AA32" s="12"/>
+    </row>
+    <row r="33" spans="1:27">
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -2111,7 +2310,7 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="1:17" ht="21">
+    <row r="34" spans="1:27" ht="21">
       <c r="A34" s="13" t="s">
         <v>20</v>
       </c>
@@ -2130,193 +2329,345 @@
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-    </row>
-    <row r="35" spans="1:17">
-      <c r="A35" s="16" t="s">
+      <c r="Q34" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
+      <c r="T34" s="14"/>
+      <c r="U34" s="14"/>
+      <c r="V34" s="14"/>
+      <c r="W34" s="14"/>
+      <c r="X34" s="14"/>
+      <c r="Y34" s="14"/>
+      <c r="Z34" s="14"/>
+      <c r="AA34" s="15"/>
+    </row>
+    <row r="35" spans="1:27">
+      <c r="A35" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="16" t="s">
+      <c r="B35" s="35"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="17"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="16" t="s">
+      <c r="E35" s="35"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="18"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="36"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
-    </row>
-    <row r="36" spans="1:17">
-      <c r="A36" s="22" t="s">
+      <c r="Q35" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="R35" s="17"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="U35" s="17"/>
+      <c r="V35" s="18"/>
+      <c r="W35" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="X35" s="17"/>
+      <c r="Y35" s="17"/>
+      <c r="Z35" s="17"/>
+      <c r="AA35" s="18"/>
+    </row>
+    <row r="36" spans="1:27" ht="15" customHeight="1">
+      <c r="A36" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="23"/>
+      <c r="B36" s="37"/>
       <c r="C36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="23"/>
+      <c r="E36" s="37"/>
       <c r="F36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G36" s="44" t="s">
+      <c r="G36" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="H36" s="38"/>
-      <c r="I36" s="38"/>
-      <c r="J36" s="38"/>
-      <c r="K36" s="39"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="50"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
-    </row>
-    <row r="37" spans="1:17">
+      <c r="Q36" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="R36" s="20"/>
+      <c r="S36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T36" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="U36" s="20"/>
+      <c r="V36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W36" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="X36" s="22"/>
+      <c r="Y36" s="22"/>
+      <c r="Z36" s="22"/>
+      <c r="AA36" s="23"/>
+    </row>
+    <row r="37" spans="1:27">
       <c r="A37" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="31"/>
+      <c r="B37" s="43"/>
       <c r="C37" s="4">
         <v>0.1</v>
       </c>
       <c r="D37" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="31"/>
+      <c r="E37" s="43"/>
       <c r="F37" s="4">
         <v>0.2</v>
       </c>
-      <c r="G37" s="40"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
-      <c r="K37" s="42"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="53"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-    </row>
-    <row r="38" spans="1:17">
+      <c r="Q37" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="R37" s="31"/>
+      <c r="S37" s="4">
+        <v>0</v>
+      </c>
+      <c r="T37" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="U37" s="33"/>
+      <c r="V37" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W37" s="24"/>
+      <c r="X37" s="25"/>
+      <c r="Y37" s="25"/>
+      <c r="Z37" s="25"/>
+      <c r="AA37" s="26"/>
+    </row>
+    <row r="38" spans="1:27">
       <c r="A38" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="31"/>
+      <c r="B38" s="43"/>
       <c r="C38" s="4">
         <v>0.2</v>
       </c>
       <c r="D38" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="31"/>
+      <c r="E38" s="43"/>
       <c r="F38" s="4">
         <v>0.6</v>
       </c>
-      <c r="G38" s="40"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
-      <c r="K38" s="42"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="52"/>
+      <c r="I38" s="52"/>
+      <c r="J38" s="52"/>
+      <c r="K38" s="53"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-    </row>
-    <row r="39" spans="1:17">
-      <c r="A39" s="33" t="s">
+      <c r="Q38" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="R38" s="33"/>
+      <c r="S38" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="T38" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="U38" s="33"/>
+      <c r="V38" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="W38" s="24"/>
+      <c r="X38" s="25"/>
+      <c r="Y38" s="25"/>
+      <c r="Z38" s="25"/>
+      <c r="AA38" s="26"/>
+    </row>
+    <row r="39" spans="1:27">
+      <c r="A39" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="34"/>
+      <c r="B39" s="45"/>
       <c r="C39" s="3">
         <v>0.6</v>
       </c>
-      <c r="D39" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E39" s="34"/>
+      <c r="D39" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="45"/>
       <c r="F39" s="3">
         <v>1.5</v>
       </c>
-      <c r="G39" s="40"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="41"/>
-      <c r="J39" s="41"/>
-      <c r="K39" s="42"/>
-    </row>
-    <row r="40" spans="1:17">
+      <c r="G39" s="51"/>
+      <c r="H39" s="52"/>
+      <c r="I39" s="52"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="53"/>
+      <c r="Q39" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="R39" s="33"/>
+      <c r="S39" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="T39" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="U39" s="33"/>
+      <c r="V39" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="W39" s="24"/>
+      <c r="X39" s="25"/>
+      <c r="Y39" s="25"/>
+      <c r="Z39" s="25"/>
+      <c r="AA39" s="26"/>
+    </row>
+    <row r="40" spans="1:27">
       <c r="A40" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="31"/>
+      <c r="B40" s="43"/>
       <c r="C40" s="4">
         <v>0.25</v>
       </c>
       <c r="D40" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="31"/>
+      <c r="E40" s="43"/>
       <c r="F40" s="4">
         <v>2</v>
       </c>
-      <c r="G40" s="40"/>
-      <c r="H40" s="41"/>
-      <c r="I40" s="41"/>
-      <c r="J40" s="41"/>
-      <c r="K40" s="42"/>
-    </row>
-    <row r="41" spans="1:17">
+      <c r="G40" s="51"/>
+      <c r="H40" s="52"/>
+      <c r="I40" s="52"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="53"/>
+      <c r="Q40" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="R40" s="33"/>
+      <c r="S40" s="4">
+        <v>0</v>
+      </c>
+      <c r="T40" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="U40" s="33"/>
+      <c r="V40" s="4">
+        <v>2</v>
+      </c>
+      <c r="W40" s="24"/>
+      <c r="X40" s="25"/>
+      <c r="Y40" s="25"/>
+      <c r="Z40" s="25"/>
+      <c r="AA40" s="26"/>
+    </row>
+    <row r="41" spans="1:27">
       <c r="A41" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="31"/>
+      <c r="B41" s="43"/>
       <c r="C41" s="4">
         <v>1.2</v>
       </c>
       <c r="D41" s="32"/>
-      <c r="E41" s="31"/>
+      <c r="E41" s="43"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="41"/>
-      <c r="I41" s="41"/>
-      <c r="J41" s="41"/>
-      <c r="K41" s="42"/>
-    </row>
-    <row r="42" spans="1:17">
-      <c r="A42" s="35" t="s">
+      <c r="G41" s="51"/>
+      <c r="H41" s="52"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="53"/>
+      <c r="Q41" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="R41" s="33"/>
+      <c r="S41" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="T41" s="32"/>
+      <c r="U41" s="33"/>
+      <c r="V41" s="4"/>
+      <c r="W41" s="24"/>
+      <c r="X41" s="25"/>
+      <c r="Y41" s="25"/>
+      <c r="Z41" s="25"/>
+      <c r="AA41" s="26"/>
+    </row>
+    <row r="42" spans="1:27">
+      <c r="A42" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="36"/>
+      <c r="B42" s="47"/>
       <c r="C42" s="2">
         <v>0.4</v>
       </c>
-      <c r="D42" s="35"/>
-      <c r="E42" s="36"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="47"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="41"/>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
-      <c r="K42" s="42"/>
-    </row>
-    <row r="43" spans="1:17" ht="18.75">
+      <c r="G42" s="51"/>
+      <c r="H42" s="52"/>
+      <c r="I42" s="52"/>
+      <c r="J42" s="52"/>
+      <c r="K42" s="53"/>
+      <c r="Q42" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="R42" s="33"/>
+      <c r="S42" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T42" s="32"/>
+      <c r="U42" s="33"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="27"/>
+      <c r="X42" s="28"/>
+      <c r="Y42" s="28"/>
+      <c r="Z42" s="28"/>
+      <c r="AA42" s="29"/>
+    </row>
+    <row r="43" spans="1:27" ht="18.75">
       <c r="A43" s="10" t="s">
         <v>22</v>
       </c>
@@ -2330,8 +2681,21 @@
       <c r="I43" s="11"/>
       <c r="J43" s="11"/>
       <c r="K43" s="12"/>
-    </row>
-    <row r="45" spans="1:17" ht="21">
+      <c r="Q43" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R43" s="11"/>
+      <c r="S43" s="11"/>
+      <c r="T43" s="11"/>
+      <c r="U43" s="11"/>
+      <c r="V43" s="11"/>
+      <c r="W43" s="11"/>
+      <c r="X43" s="11"/>
+      <c r="Y43" s="11"/>
+      <c r="Z43" s="11"/>
+      <c r="AA43" s="12"/>
+    </row>
+    <row r="45" spans="1:27" ht="21">
       <c r="A45" s="13" t="s">
         <v>23</v>
       </c>
@@ -2345,168 +2709,325 @@
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
       <c r="K45" s="15"/>
-    </row>
-    <row r="46" spans="1:17">
-      <c r="A46" s="16" t="s">
+      <c r="Q45" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
+      <c r="T45" s="14"/>
+      <c r="U45" s="14"/>
+      <c r="V45" s="14"/>
+      <c r="W45" s="14"/>
+      <c r="X45" s="14"/>
+      <c r="Y45" s="14"/>
+      <c r="Z45" s="14"/>
+      <c r="AA45" s="15"/>
+    </row>
+    <row r="46" spans="1:27">
+      <c r="A46" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="17"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="16" t="s">
+      <c r="B46" s="35"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="17"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="16" t="s">
+      <c r="E46" s="35"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="17"/>
-      <c r="K46" s="18"/>
-    </row>
-    <row r="47" spans="1:17">
-      <c r="A47" s="22" t="s">
+      <c r="H46" s="35"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="36"/>
+      <c r="Q46" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="R46" s="35"/>
+      <c r="S46" s="36"/>
+      <c r="T46" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="U46" s="35"/>
+      <c r="V46" s="36"/>
+      <c r="W46" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="X46" s="17"/>
+      <c r="Y46" s="17"/>
+      <c r="Z46" s="17"/>
+      <c r="AA46" s="18"/>
+    </row>
+    <row r="47" spans="1:27">
+      <c r="A47" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="23"/>
+      <c r="B47" s="37"/>
       <c r="C47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D47" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E47" s="23"/>
+      <c r="E47" s="37"/>
       <c r="F47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G47" s="44" t="s">
+      <c r="G47" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="H47" s="38"/>
-      <c r="I47" s="38"/>
-      <c r="J47" s="38"/>
-      <c r="K47" s="39"/>
-    </row>
-    <row r="48" spans="1:17">
+      <c r="H47" s="49"/>
+      <c r="I47" s="49"/>
+      <c r="J47" s="49"/>
+      <c r="K47" s="50"/>
+      <c r="Q47" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="R47" s="37"/>
+      <c r="S47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T47" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="U47" s="37"/>
+      <c r="V47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W47" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="X47" s="38"/>
+      <c r="Y47" s="38"/>
+      <c r="Z47" s="38"/>
+      <c r="AA47" s="39"/>
+    </row>
+    <row r="48" spans="1:27">
       <c r="A48" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B48" s="31"/>
+      <c r="B48" s="43"/>
       <c r="C48" s="4">
         <v>0.1</v>
       </c>
       <c r="D48" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E48" s="31"/>
+      <c r="E48" s="43"/>
       <c r="F48" s="4">
         <v>0.2</v>
       </c>
-      <c r="G48" s="40"/>
-      <c r="H48" s="41"/>
-      <c r="I48" s="41"/>
-      <c r="J48" s="41"/>
-      <c r="K48" s="42"/>
-    </row>
-    <row r="49" spans="1:11">
+      <c r="G48" s="51"/>
+      <c r="H48" s="52"/>
+      <c r="I48" s="52"/>
+      <c r="J48" s="52"/>
+      <c r="K48" s="53"/>
+      <c r="Q48" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="R48" s="43"/>
+      <c r="S48" s="4">
+        <v>0</v>
+      </c>
+      <c r="T48" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="U48" s="43"/>
+      <c r="V48" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W48" s="40"/>
+      <c r="X48" s="41"/>
+      <c r="Y48" s="41"/>
+      <c r="Z48" s="41"/>
+      <c r="AA48" s="42"/>
+    </row>
+    <row r="49" spans="1:27">
       <c r="A49" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B49" s="31"/>
+      <c r="B49" s="43"/>
       <c r="C49" s="4">
         <v>0.2</v>
       </c>
       <c r="D49" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="31"/>
+      <c r="E49" s="43"/>
       <c r="F49" s="4">
         <v>0.6</v>
       </c>
-      <c r="G49" s="40"/>
-      <c r="H49" s="41"/>
-      <c r="I49" s="41"/>
-      <c r="J49" s="41"/>
-      <c r="K49" s="42"/>
-    </row>
-    <row r="50" spans="1:11">
-      <c r="A50" s="33" t="s">
+      <c r="G49" s="51"/>
+      <c r="H49" s="52"/>
+      <c r="I49" s="52"/>
+      <c r="J49" s="52"/>
+      <c r="K49" s="53"/>
+      <c r="Q49" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="R49" s="43"/>
+      <c r="S49" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="T49" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="U49" s="43"/>
+      <c r="V49" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="W49" s="40"/>
+      <c r="X49" s="41"/>
+      <c r="Y49" s="41"/>
+      <c r="Z49" s="41"/>
+      <c r="AA49" s="42"/>
+    </row>
+    <row r="50" spans="1:27">
+      <c r="A50" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="34"/>
+      <c r="B50" s="45"/>
       <c r="C50" s="3">
         <v>0.6</v>
       </c>
-      <c r="D50" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E50" s="34"/>
+      <c r="D50" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="45"/>
       <c r="F50" s="3">
         <v>1.5</v>
       </c>
-      <c r="G50" s="40"/>
-      <c r="H50" s="41"/>
-      <c r="I50" s="41"/>
-      <c r="J50" s="41"/>
-      <c r="K50" s="42"/>
-    </row>
-    <row r="51" spans="1:11">
+      <c r="G50" s="51"/>
+      <c r="H50" s="52"/>
+      <c r="I50" s="52"/>
+      <c r="J50" s="52"/>
+      <c r="K50" s="53"/>
+      <c r="Q50" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="R50" s="45"/>
+      <c r="S50" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="T50" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="U50" s="45"/>
+      <c r="V50" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="W50" s="40"/>
+      <c r="X50" s="41"/>
+      <c r="Y50" s="41"/>
+      <c r="Z50" s="41"/>
+      <c r="AA50" s="42"/>
+    </row>
+    <row r="51" spans="1:27">
       <c r="A51" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="31"/>
+      <c r="B51" s="43"/>
       <c r="C51" s="4">
         <v>0</v>
       </c>
       <c r="D51" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="31"/>
+      <c r="E51" s="43"/>
       <c r="F51" s="4">
         <v>2</v>
       </c>
-      <c r="G51" s="40"/>
-      <c r="H51" s="41"/>
-      <c r="I51" s="41"/>
-      <c r="J51" s="41"/>
-      <c r="K51" s="42"/>
-    </row>
-    <row r="52" spans="1:11">
+      <c r="G51" s="51"/>
+      <c r="H51" s="52"/>
+      <c r="I51" s="52"/>
+      <c r="J51" s="52"/>
+      <c r="K51" s="53"/>
+      <c r="Q51" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="R51" s="43"/>
+      <c r="S51" s="4">
+        <v>0</v>
+      </c>
+      <c r="T51" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="U51" s="43"/>
+      <c r="V51" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="W51" s="40"/>
+      <c r="X51" s="41"/>
+      <c r="Y51" s="41"/>
+      <c r="Z51" s="41"/>
+      <c r="AA51" s="42"/>
+    </row>
+    <row r="52" spans="1:27">
       <c r="A52" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B52" s="31"/>
+      <c r="B52" s="43"/>
       <c r="C52" s="4">
         <v>1.4</v>
       </c>
       <c r="D52" s="32"/>
-      <c r="E52" s="31"/>
+      <c r="E52" s="43"/>
       <c r="F52" s="4"/>
-      <c r="G52" s="40"/>
-      <c r="H52" s="41"/>
-      <c r="I52" s="41"/>
-      <c r="J52" s="41"/>
-      <c r="K52" s="42"/>
-    </row>
-    <row r="53" spans="1:11">
-      <c r="A53" s="35" t="s">
+      <c r="G52" s="51"/>
+      <c r="H52" s="52"/>
+      <c r="I52" s="52"/>
+      <c r="J52" s="52"/>
+      <c r="K52" s="53"/>
+      <c r="Q52" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="R52" s="43"/>
+      <c r="S52" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="T52" s="32"/>
+      <c r="U52" s="43"/>
+      <c r="V52" s="4"/>
+      <c r="W52" s="40"/>
+      <c r="X52" s="41"/>
+      <c r="Y52" s="41"/>
+      <c r="Z52" s="41"/>
+      <c r="AA52" s="42"/>
+    </row>
+    <row r="53" spans="1:27">
+      <c r="A53" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="36"/>
+      <c r="B53" s="47"/>
       <c r="C53" s="2">
         <v>0.4</v>
       </c>
-      <c r="D53" s="35"/>
-      <c r="E53" s="36"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="47"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="40"/>
-      <c r="H53" s="41"/>
-      <c r="I53" s="41"/>
-      <c r="J53" s="41"/>
-      <c r="K53" s="42"/>
-    </row>
-    <row r="54" spans="1:11" ht="18.75">
+      <c r="G53" s="51"/>
+      <c r="H53" s="52"/>
+      <c r="I53" s="52"/>
+      <c r="J53" s="52"/>
+      <c r="K53" s="53"/>
+      <c r="Q53" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="R53" s="47"/>
+      <c r="S53" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T53" s="46"/>
+      <c r="U53" s="47"/>
+      <c r="V53" s="2"/>
+      <c r="W53" s="40"/>
+      <c r="X53" s="41"/>
+      <c r="Y53" s="41"/>
+      <c r="Z53" s="41"/>
+      <c r="AA53" s="42"/>
+    </row>
+    <row r="54" spans="1:27" ht="18.75">
       <c r="A54" s="10" t="s">
         <v>24</v>
       </c>
@@ -2520,8 +3041,21 @@
       <c r="I54" s="11"/>
       <c r="J54" s="11"/>
       <c r="K54" s="12"/>
-    </row>
-    <row r="55" spans="1:11" ht="18.75">
+      <c r="Q54" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R54" s="11"/>
+      <c r="S54" s="11"/>
+      <c r="T54" s="11"/>
+      <c r="U54" s="11"/>
+      <c r="V54" s="11"/>
+      <c r="W54" s="11"/>
+      <c r="X54" s="11"/>
+      <c r="Y54" s="11"/>
+      <c r="Z54" s="11"/>
+      <c r="AA54" s="12"/>
+    </row>
+    <row r="55" spans="1:27" ht="18.75">
       <c r="A55" s="6" t="s">
         <v>29</v>
       </c>
@@ -2536,7 +3070,7 @@
       <c r="J55" s="6"/>
       <c r="K55" s="7"/>
     </row>
-    <row r="57" spans="1:11" ht="21">
+    <row r="57" spans="1:27" ht="21">
       <c r="A57" s="13" t="s">
         <v>25</v>
       </c>
@@ -2551,165 +3085,165 @@
       <c r="J57" s="14"/>
       <c r="K57" s="15"/>
     </row>
-    <row r="58" spans="1:11">
-      <c r="A58" s="16" t="s">
+    <row r="58" spans="1:27">
+      <c r="A58" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B58" s="17"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="16" t="s">
+      <c r="B58" s="35"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E58" s="17"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="16" t="s">
+      <c r="E58" s="35"/>
+      <c r="F58" s="36"/>
+      <c r="G58" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H58" s="17"/>
-      <c r="I58" s="17"/>
-      <c r="J58" s="17"/>
-      <c r="K58" s="18"/>
-    </row>
-    <row r="59" spans="1:11">
-      <c r="A59" s="22" t="s">
+      <c r="H58" s="35"/>
+      <c r="I58" s="35"/>
+      <c r="J58" s="35"/>
+      <c r="K58" s="36"/>
+    </row>
+    <row r="59" spans="1:27">
+      <c r="A59" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="23"/>
+      <c r="B59" s="37"/>
       <c r="C59" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D59" s="22" t="s">
+      <c r="D59" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E59" s="23"/>
+      <c r="E59" s="37"/>
       <c r="F59" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G59" s="44" t="s">
+      <c r="G59" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="H59" s="38"/>
-      <c r="I59" s="38"/>
-      <c r="J59" s="38"/>
-      <c r="K59" s="39"/>
-    </row>
-    <row r="60" spans="1:11">
+      <c r="H59" s="49"/>
+      <c r="I59" s="49"/>
+      <c r="J59" s="49"/>
+      <c r="K59" s="50"/>
+    </row>
+    <row r="60" spans="1:27">
       <c r="A60" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B60" s="31"/>
+      <c r="B60" s="43"/>
       <c r="C60" s="4">
         <v>0.1</v>
       </c>
       <c r="D60" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E60" s="31"/>
+      <c r="E60" s="43"/>
       <c r="F60" s="4">
         <v>0.2</v>
       </c>
-      <c r="G60" s="40"/>
-      <c r="H60" s="41"/>
-      <c r="I60" s="41"/>
-      <c r="J60" s="41"/>
-      <c r="K60" s="42"/>
-    </row>
-    <row r="61" spans="1:11">
+      <c r="G60" s="51"/>
+      <c r="H60" s="52"/>
+      <c r="I60" s="52"/>
+      <c r="J60" s="52"/>
+      <c r="K60" s="53"/>
+    </row>
+    <row r="61" spans="1:27">
       <c r="A61" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B61" s="31"/>
+      <c r="B61" s="43"/>
       <c r="C61" s="4">
         <v>0.2</v>
       </c>
       <c r="D61" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E61" s="31"/>
+      <c r="E61" s="43"/>
       <c r="F61" s="4">
         <v>0.6</v>
       </c>
-      <c r="G61" s="40"/>
-      <c r="H61" s="41"/>
-      <c r="I61" s="41"/>
-      <c r="J61" s="41"/>
-      <c r="K61" s="42"/>
-    </row>
-    <row r="62" spans="1:11">
-      <c r="A62" s="33" t="s">
+      <c r="G61" s="51"/>
+      <c r="H61" s="52"/>
+      <c r="I61" s="52"/>
+      <c r="J61" s="52"/>
+      <c r="K61" s="53"/>
+    </row>
+    <row r="62" spans="1:27">
+      <c r="A62" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B62" s="34"/>
+      <c r="B62" s="45"/>
       <c r="C62" s="3">
         <v>0.7</v>
       </c>
-      <c r="D62" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E62" s="34"/>
+      <c r="D62" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="45"/>
       <c r="F62" s="3">
         <v>1.5</v>
       </c>
-      <c r="G62" s="40"/>
-      <c r="H62" s="41"/>
-      <c r="I62" s="41"/>
-      <c r="J62" s="41"/>
-      <c r="K62" s="42"/>
-    </row>
-    <row r="63" spans="1:11">
+      <c r="G62" s="51"/>
+      <c r="H62" s="52"/>
+      <c r="I62" s="52"/>
+      <c r="J62" s="52"/>
+      <c r="K62" s="53"/>
+    </row>
+    <row r="63" spans="1:27">
       <c r="A63" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B63" s="31"/>
+      <c r="B63" s="43"/>
       <c r="C63" s="4">
         <v>0</v>
       </c>
       <c r="D63" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E63" s="31"/>
+      <c r="E63" s="43"/>
       <c r="F63" s="4">
         <v>2</v>
       </c>
-      <c r="G63" s="40"/>
-      <c r="H63" s="41"/>
-      <c r="I63" s="41"/>
-      <c r="J63" s="41"/>
-      <c r="K63" s="42"/>
-    </row>
-    <row r="64" spans="1:11">
+      <c r="G63" s="51"/>
+      <c r="H63" s="52"/>
+      <c r="I63" s="52"/>
+      <c r="J63" s="52"/>
+      <c r="K63" s="53"/>
+    </row>
+    <row r="64" spans="1:27">
       <c r="A64" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B64" s="31"/>
+      <c r="B64" s="43"/>
       <c r="C64" s="4">
         <v>1.5</v>
       </c>
       <c r="D64" s="32"/>
-      <c r="E64" s="31"/>
+      <c r="E64" s="43"/>
       <c r="F64" s="4"/>
-      <c r="G64" s="40"/>
-      <c r="H64" s="41"/>
-      <c r="I64" s="41"/>
-      <c r="J64" s="41"/>
-      <c r="K64" s="42"/>
+      <c r="G64" s="51"/>
+      <c r="H64" s="52"/>
+      <c r="I64" s="52"/>
+      <c r="J64" s="52"/>
+      <c r="K64" s="53"/>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="35" t="s">
+      <c r="A65" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B65" s="36"/>
+      <c r="B65" s="47"/>
       <c r="C65" s="2">
         <v>0.4</v>
       </c>
-      <c r="D65" s="35"/>
-      <c r="E65" s="36"/>
+      <c r="D65" s="46"/>
+      <c r="E65" s="47"/>
       <c r="F65" s="2"/>
-      <c r="G65" s="40"/>
-      <c r="H65" s="41"/>
-      <c r="I65" s="41"/>
-      <c r="J65" s="41"/>
-      <c r="K65" s="42"/>
+      <c r="G65" s="51"/>
+      <c r="H65" s="52"/>
+      <c r="I65" s="52"/>
+      <c r="J65" s="52"/>
+      <c r="K65" s="53"/>
     </row>
     <row r="66" spans="1:11" ht="18.75">
       <c r="A66" s="10" t="s">
@@ -2742,162 +3276,162 @@
       <c r="K68" s="15"/>
     </row>
     <row r="69" spans="1:11">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B69" s="17"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="16" t="s">
+      <c r="B69" s="35"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E69" s="17"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="16" t="s">
+      <c r="E69" s="35"/>
+      <c r="F69" s="36"/>
+      <c r="G69" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H69" s="17"/>
-      <c r="I69" s="17"/>
-      <c r="J69" s="17"/>
-      <c r="K69" s="18"/>
+      <c r="H69" s="35"/>
+      <c r="I69" s="35"/>
+      <c r="J69" s="35"/>
+      <c r="K69" s="36"/>
     </row>
     <row r="70" spans="1:11">
-      <c r="A70" s="22" t="s">
+      <c r="A70" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B70" s="23"/>
+      <c r="B70" s="37"/>
       <c r="C70" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D70" s="22" t="s">
+      <c r="D70" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="23"/>
+      <c r="E70" s="37"/>
       <c r="F70" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G70" s="44"/>
-      <c r="H70" s="38"/>
-      <c r="I70" s="38"/>
-      <c r="J70" s="38"/>
-      <c r="K70" s="39"/>
+      <c r="G70" s="55"/>
+      <c r="H70" s="49"/>
+      <c r="I70" s="49"/>
+      <c r="J70" s="49"/>
+      <c r="K70" s="50"/>
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B71" s="31"/>
+      <c r="B71" s="43"/>
       <c r="C71" s="4">
         <v>0.1</v>
       </c>
       <c r="D71" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E71" s="31"/>
+      <c r="E71" s="43"/>
       <c r="F71" s="4">
         <v>0.2</v>
       </c>
-      <c r="G71" s="40"/>
-      <c r="H71" s="41"/>
-      <c r="I71" s="41"/>
-      <c r="J71" s="41"/>
-      <c r="K71" s="42"/>
+      <c r="G71" s="51"/>
+      <c r="H71" s="52"/>
+      <c r="I71" s="52"/>
+      <c r="J71" s="52"/>
+      <c r="K71" s="53"/>
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B72" s="31"/>
+      <c r="B72" s="43"/>
       <c r="C72" s="4">
         <v>0.4</v>
       </c>
       <c r="D72" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E72" s="31"/>
+      <c r="E72" s="43"/>
       <c r="F72" s="4">
         <v>0.6</v>
       </c>
-      <c r="G72" s="40"/>
-      <c r="H72" s="41"/>
-      <c r="I72" s="41"/>
-      <c r="J72" s="41"/>
-      <c r="K72" s="42"/>
+      <c r="G72" s="51"/>
+      <c r="H72" s="52"/>
+      <c r="I72" s="52"/>
+      <c r="J72" s="52"/>
+      <c r="K72" s="53"/>
     </row>
     <row r="73" spans="1:11">
-      <c r="A73" s="33" t="s">
+      <c r="A73" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B73" s="34"/>
+      <c r="B73" s="45"/>
       <c r="C73" s="3">
         <v>1</v>
       </c>
-      <c r="D73" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E73" s="34"/>
+      <c r="D73" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="45"/>
       <c r="F73" s="3">
         <v>1.5</v>
       </c>
-      <c r="G73" s="40"/>
-      <c r="H73" s="41"/>
-      <c r="I73" s="41"/>
-      <c r="J73" s="41"/>
-      <c r="K73" s="42"/>
+      <c r="G73" s="51"/>
+      <c r="H73" s="52"/>
+      <c r="I73" s="52"/>
+      <c r="J73" s="52"/>
+      <c r="K73" s="53"/>
     </row>
     <row r="74" spans="1:11">
       <c r="A74" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B74" s="31"/>
+      <c r="B74" s="43"/>
       <c r="C74" s="4">
         <v>0</v>
       </c>
       <c r="D74" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E74" s="31"/>
+      <c r="E74" s="43"/>
       <c r="F74" s="4">
         <v>2</v>
       </c>
-      <c r="G74" s="40"/>
-      <c r="H74" s="41"/>
-      <c r="I74" s="41"/>
-      <c r="J74" s="41"/>
-      <c r="K74" s="42"/>
+      <c r="G74" s="51"/>
+      <c r="H74" s="52"/>
+      <c r="I74" s="52"/>
+      <c r="J74" s="52"/>
+      <c r="K74" s="53"/>
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B75" s="31"/>
+      <c r="B75" s="43"/>
       <c r="C75" s="4">
         <v>1.5</v>
       </c>
       <c r="D75" s="32"/>
-      <c r="E75" s="31"/>
+      <c r="E75" s="43"/>
       <c r="F75" s="4"/>
-      <c r="G75" s="40"/>
-      <c r="H75" s="41"/>
-      <c r="I75" s="41"/>
-      <c r="J75" s="41"/>
-      <c r="K75" s="42"/>
+      <c r="G75" s="51"/>
+      <c r="H75" s="52"/>
+      <c r="I75" s="52"/>
+      <c r="J75" s="52"/>
+      <c r="K75" s="53"/>
     </row>
     <row r="76" spans="1:11">
-      <c r="A76" s="35" t="s">
+      <c r="A76" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B76" s="36"/>
+      <c r="B76" s="47"/>
       <c r="C76" s="2">
         <v>0.5</v>
       </c>
-      <c r="D76" s="35"/>
-      <c r="E76" s="36"/>
+      <c r="D76" s="46"/>
+      <c r="E76" s="47"/>
       <c r="F76" s="2"/>
-      <c r="G76" s="40"/>
-      <c r="H76" s="41"/>
-      <c r="I76" s="41"/>
-      <c r="J76" s="41"/>
-      <c r="K76" s="42"/>
+      <c r="G76" s="51"/>
+      <c r="H76" s="52"/>
+      <c r="I76" s="52"/>
+      <c r="J76" s="52"/>
+      <c r="K76" s="53"/>
     </row>
     <row r="77" spans="1:11" ht="18.75">
       <c r="A77" s="10" t="s">
@@ -2930,164 +3464,164 @@
       <c r="K79" s="15"/>
     </row>
     <row r="80" spans="1:11">
-      <c r="A80" s="16" t="s">
+      <c r="A80" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B80" s="17"/>
-      <c r="C80" s="18"/>
-      <c r="D80" s="16" t="s">
+      <c r="B80" s="35"/>
+      <c r="C80" s="36"/>
+      <c r="D80" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E80" s="17"/>
-      <c r="F80" s="18"/>
-      <c r="G80" s="16" t="s">
+      <c r="E80" s="35"/>
+      <c r="F80" s="36"/>
+      <c r="G80" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H80" s="17"/>
-      <c r="I80" s="17"/>
-      <c r="J80" s="17"/>
-      <c r="K80" s="18"/>
+      <c r="H80" s="35"/>
+      <c r="I80" s="35"/>
+      <c r="J80" s="35"/>
+      <c r="K80" s="36"/>
     </row>
     <row r="81" spans="1:11">
-      <c r="A81" s="22" t="s">
+      <c r="A81" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B81" s="23"/>
+      <c r="B81" s="37"/>
       <c r="C81" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D81" s="22" t="s">
+      <c r="D81" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E81" s="23"/>
+      <c r="E81" s="37"/>
       <c r="F81" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G81" s="44" t="s">
+      <c r="G81" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="H81" s="38"/>
-      <c r="I81" s="38"/>
-      <c r="J81" s="38"/>
-      <c r="K81" s="39"/>
+      <c r="H81" s="49"/>
+      <c r="I81" s="49"/>
+      <c r="J81" s="49"/>
+      <c r="K81" s="50"/>
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B82" s="31"/>
+      <c r="B82" s="43"/>
       <c r="C82" s="4">
         <v>0.1</v>
       </c>
       <c r="D82" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E82" s="31"/>
+      <c r="E82" s="43"/>
       <c r="F82" s="4">
         <v>0.2</v>
       </c>
-      <c r="G82" s="40"/>
-      <c r="H82" s="41"/>
-      <c r="I82" s="41"/>
-      <c r="J82" s="41"/>
-      <c r="K82" s="42"/>
+      <c r="G82" s="51"/>
+      <c r="H82" s="52"/>
+      <c r="I82" s="52"/>
+      <c r="J82" s="52"/>
+      <c r="K82" s="53"/>
     </row>
     <row r="83" spans="1:11">
       <c r="A83" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B83" s="31"/>
+      <c r="B83" s="43"/>
       <c r="C83" s="4">
         <v>0.2</v>
       </c>
       <c r="D83" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E83" s="31"/>
+      <c r="E83" s="43"/>
       <c r="F83" s="4">
         <v>0.6</v>
       </c>
-      <c r="G83" s="40"/>
-      <c r="H83" s="41"/>
-      <c r="I83" s="41"/>
-      <c r="J83" s="41"/>
-      <c r="K83" s="42"/>
+      <c r="G83" s="51"/>
+      <c r="H83" s="52"/>
+      <c r="I83" s="52"/>
+      <c r="J83" s="52"/>
+      <c r="K83" s="53"/>
     </row>
     <row r="84" spans="1:11">
-      <c r="A84" s="33" t="s">
+      <c r="A84" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B84" s="34"/>
+      <c r="B84" s="45"/>
       <c r="C84" s="3">
         <v>0.6</v>
       </c>
-      <c r="D84" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E84" s="34"/>
+      <c r="D84" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="45"/>
       <c r="F84" s="3">
         <v>1.5</v>
       </c>
-      <c r="G84" s="40"/>
-      <c r="H84" s="41"/>
-      <c r="I84" s="41"/>
-      <c r="J84" s="41"/>
-      <c r="K84" s="42"/>
+      <c r="G84" s="51"/>
+      <c r="H84" s="52"/>
+      <c r="I84" s="52"/>
+      <c r="J84" s="52"/>
+      <c r="K84" s="53"/>
     </row>
     <row r="85" spans="1:11">
       <c r="A85" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B85" s="31"/>
+      <c r="B85" s="43"/>
       <c r="C85" s="4">
         <v>0</v>
       </c>
       <c r="D85" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E85" s="31"/>
+      <c r="E85" s="43"/>
       <c r="F85" s="4">
         <v>2</v>
       </c>
-      <c r="G85" s="40"/>
-      <c r="H85" s="41"/>
-      <c r="I85" s="41"/>
-      <c r="J85" s="41"/>
-      <c r="K85" s="42"/>
+      <c r="G85" s="51"/>
+      <c r="H85" s="52"/>
+      <c r="I85" s="52"/>
+      <c r="J85" s="52"/>
+      <c r="K85" s="53"/>
     </row>
     <row r="86" spans="1:11">
       <c r="A86" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B86" s="31"/>
+      <c r="B86" s="43"/>
       <c r="C86" s="4">
         <v>1.4</v>
       </c>
       <c r="D86" s="32"/>
-      <c r="E86" s="31"/>
+      <c r="E86" s="43"/>
       <c r="F86" s="4"/>
-      <c r="G86" s="40"/>
-      <c r="H86" s="41"/>
-      <c r="I86" s="41"/>
-      <c r="J86" s="41"/>
-      <c r="K86" s="42"/>
+      <c r="G86" s="51"/>
+      <c r="H86" s="52"/>
+      <c r="I86" s="52"/>
+      <c r="J86" s="52"/>
+      <c r="K86" s="53"/>
     </row>
     <row r="87" spans="1:11">
-      <c r="A87" s="35" t="s">
+      <c r="A87" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B87" s="36"/>
+      <c r="B87" s="47"/>
       <c r="C87" s="2">
         <v>0.4</v>
       </c>
-      <c r="D87" s="35"/>
-      <c r="E87" s="36"/>
+      <c r="D87" s="46"/>
+      <c r="E87" s="47"/>
       <c r="F87" s="2"/>
-      <c r="G87" s="40"/>
-      <c r="H87" s="41"/>
-      <c r="I87" s="41"/>
-      <c r="J87" s="41"/>
-      <c r="K87" s="42"/>
+      <c r="G87" s="51"/>
+      <c r="H87" s="52"/>
+      <c r="I87" s="52"/>
+      <c r="J87" s="52"/>
+      <c r="K87" s="53"/>
     </row>
     <row r="88" spans="1:11" ht="18.75">
       <c r="A88" s="10" t="s">
@@ -3120,164 +3654,164 @@
       <c r="K90" s="15"/>
     </row>
     <row r="91" spans="1:11">
-      <c r="A91" s="16" t="s">
+      <c r="A91" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B91" s="17"/>
-      <c r="C91" s="18"/>
-      <c r="D91" s="16" t="s">
+      <c r="B91" s="35"/>
+      <c r="C91" s="36"/>
+      <c r="D91" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E91" s="17"/>
-      <c r="F91" s="18"/>
-      <c r="G91" s="16" t="s">
+      <c r="E91" s="35"/>
+      <c r="F91" s="36"/>
+      <c r="G91" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H91" s="17"/>
-      <c r="I91" s="17"/>
-      <c r="J91" s="17"/>
-      <c r="K91" s="18"/>
+      <c r="H91" s="35"/>
+      <c r="I91" s="35"/>
+      <c r="J91" s="35"/>
+      <c r="K91" s="36"/>
     </row>
     <row r="92" spans="1:11">
-      <c r="A92" s="22" t="s">
+      <c r="A92" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B92" s="23"/>
+      <c r="B92" s="37"/>
       <c r="C92" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D92" s="22" t="s">
+      <c r="D92" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E92" s="23"/>
+      <c r="E92" s="37"/>
       <c r="F92" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G92" s="43" t="s">
+      <c r="G92" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="H92" s="38"/>
-      <c r="I92" s="38"/>
-      <c r="J92" s="38"/>
-      <c r="K92" s="39"/>
+      <c r="H92" s="49"/>
+      <c r="I92" s="49"/>
+      <c r="J92" s="49"/>
+      <c r="K92" s="50"/>
     </row>
     <row r="93" spans="1:11">
       <c r="A93" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B93" s="31"/>
+      <c r="B93" s="43"/>
       <c r="C93" s="4">
         <v>0.1</v>
       </c>
       <c r="D93" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E93" s="31"/>
+      <c r="E93" s="43"/>
       <c r="F93" s="4">
         <v>0.2</v>
       </c>
-      <c r="G93" s="40"/>
-      <c r="H93" s="41"/>
-      <c r="I93" s="41"/>
-      <c r="J93" s="41"/>
-      <c r="K93" s="42"/>
+      <c r="G93" s="51"/>
+      <c r="H93" s="52"/>
+      <c r="I93" s="52"/>
+      <c r="J93" s="52"/>
+      <c r="K93" s="53"/>
     </row>
     <row r="94" spans="1:11">
       <c r="A94" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B94" s="31"/>
+      <c r="B94" s="43"/>
       <c r="C94" s="4">
         <v>0.2</v>
       </c>
       <c r="D94" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E94" s="31"/>
+      <c r="E94" s="43"/>
       <c r="F94" s="4">
         <v>0.6</v>
       </c>
-      <c r="G94" s="40"/>
-      <c r="H94" s="41"/>
-      <c r="I94" s="41"/>
-      <c r="J94" s="41"/>
-      <c r="K94" s="42"/>
+      <c r="G94" s="51"/>
+      <c r="H94" s="52"/>
+      <c r="I94" s="52"/>
+      <c r="J94" s="52"/>
+      <c r="K94" s="53"/>
     </row>
     <row r="95" spans="1:11">
-      <c r="A95" s="33" t="s">
+      <c r="A95" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B95" s="34"/>
+      <c r="B95" s="45"/>
       <c r="C95" s="3">
         <v>0.8</v>
       </c>
-      <c r="D95" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E95" s="34"/>
+      <c r="D95" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" s="45"/>
       <c r="F95" s="3">
         <v>1.5</v>
       </c>
-      <c r="G95" s="40"/>
-      <c r="H95" s="41"/>
-      <c r="I95" s="41"/>
-      <c r="J95" s="41"/>
-      <c r="K95" s="42"/>
+      <c r="G95" s="51"/>
+      <c r="H95" s="52"/>
+      <c r="I95" s="52"/>
+      <c r="J95" s="52"/>
+      <c r="K95" s="53"/>
     </row>
     <row r="96" spans="1:11">
       <c r="A96" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B96" s="31"/>
+      <c r="B96" s="43"/>
       <c r="C96" s="4">
         <v>0</v>
       </c>
       <c r="D96" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E96" s="31"/>
+      <c r="E96" s="43"/>
       <c r="F96" s="4">
         <v>2</v>
       </c>
-      <c r="G96" s="40"/>
-      <c r="H96" s="41"/>
-      <c r="I96" s="41"/>
-      <c r="J96" s="41"/>
-      <c r="K96" s="42"/>
+      <c r="G96" s="51"/>
+      <c r="H96" s="52"/>
+      <c r="I96" s="52"/>
+      <c r="J96" s="52"/>
+      <c r="K96" s="53"/>
     </row>
     <row r="97" spans="1:11">
       <c r="A97" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B97" s="31"/>
+      <c r="B97" s="43"/>
       <c r="C97" s="4">
         <v>1.8</v>
       </c>
       <c r="D97" s="32"/>
-      <c r="E97" s="31"/>
+      <c r="E97" s="43"/>
       <c r="F97" s="4"/>
-      <c r="G97" s="40"/>
-      <c r="H97" s="41"/>
-      <c r="I97" s="41"/>
-      <c r="J97" s="41"/>
-      <c r="K97" s="42"/>
+      <c r="G97" s="51"/>
+      <c r="H97" s="52"/>
+      <c r="I97" s="52"/>
+      <c r="J97" s="52"/>
+      <c r="K97" s="53"/>
     </row>
     <row r="98" spans="1:11">
-      <c r="A98" s="35" t="s">
+      <c r="A98" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B98" s="36"/>
+      <c r="B98" s="47"/>
       <c r="C98" s="2">
         <v>0.4</v>
       </c>
-      <c r="D98" s="35"/>
-      <c r="E98" s="36"/>
+      <c r="D98" s="46"/>
+      <c r="E98" s="47"/>
       <c r="F98" s="2"/>
-      <c r="G98" s="40"/>
-      <c r="H98" s="41"/>
-      <c r="I98" s="41"/>
-      <c r="J98" s="41"/>
-      <c r="K98" s="42"/>
+      <c r="G98" s="51"/>
+      <c r="H98" s="52"/>
+      <c r="I98" s="52"/>
+      <c r="J98" s="52"/>
+      <c r="K98" s="53"/>
     </row>
     <row r="99" spans="1:11" ht="18.75">
       <c r="A99" s="10" t="s">
@@ -3310,164 +3844,164 @@
       <c r="K103" s="15"/>
     </row>
     <row r="104" spans="1:11">
-      <c r="A104" s="16" t="s">
+      <c r="A104" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B104" s="17"/>
-      <c r="C104" s="18"/>
-      <c r="D104" s="16" t="s">
+      <c r="B104" s="35"/>
+      <c r="C104" s="36"/>
+      <c r="D104" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E104" s="17"/>
-      <c r="F104" s="18"/>
-      <c r="G104" s="16" t="s">
+      <c r="E104" s="35"/>
+      <c r="F104" s="36"/>
+      <c r="G104" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H104" s="17"/>
-      <c r="I104" s="17"/>
-      <c r="J104" s="17"/>
-      <c r="K104" s="18"/>
+      <c r="H104" s="35"/>
+      <c r="I104" s="35"/>
+      <c r="J104" s="35"/>
+      <c r="K104" s="36"/>
     </row>
     <row r="105" spans="1:11">
-      <c r="A105" s="22" t="s">
+      <c r="A105" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B105" s="23"/>
+      <c r="B105" s="37"/>
       <c r="C105" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D105" s="22" t="s">
+      <c r="D105" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E105" s="23"/>
+      <c r="E105" s="37"/>
       <c r="F105" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G105" s="37" t="s">
+      <c r="G105" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="H105" s="38"/>
-      <c r="I105" s="38"/>
-      <c r="J105" s="38"/>
-      <c r="K105" s="39"/>
+      <c r="H105" s="49"/>
+      <c r="I105" s="49"/>
+      <c r="J105" s="49"/>
+      <c r="K105" s="50"/>
     </row>
     <row r="106" spans="1:11">
       <c r="A106" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B106" s="31"/>
+      <c r="B106" s="43"/>
       <c r="C106" s="4">
         <v>0.1</v>
       </c>
       <c r="D106" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E106" s="31"/>
+      <c r="E106" s="43"/>
       <c r="F106" s="4">
         <v>0.2</v>
       </c>
-      <c r="G106" s="40"/>
-      <c r="H106" s="41"/>
-      <c r="I106" s="41"/>
-      <c r="J106" s="41"/>
-      <c r="K106" s="42"/>
+      <c r="G106" s="51"/>
+      <c r="H106" s="52"/>
+      <c r="I106" s="52"/>
+      <c r="J106" s="52"/>
+      <c r="K106" s="53"/>
     </row>
     <row r="107" spans="1:11">
       <c r="A107" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B107" s="31"/>
+      <c r="B107" s="43"/>
       <c r="C107" s="4">
         <v>0.2</v>
       </c>
       <c r="D107" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E107" s="31"/>
+      <c r="E107" s="43"/>
       <c r="F107" s="4">
         <v>0.6</v>
       </c>
-      <c r="G107" s="40"/>
-      <c r="H107" s="41"/>
-      <c r="I107" s="41"/>
-      <c r="J107" s="41"/>
-      <c r="K107" s="42"/>
+      <c r="G107" s="51"/>
+      <c r="H107" s="52"/>
+      <c r="I107" s="52"/>
+      <c r="J107" s="52"/>
+      <c r="K107" s="53"/>
     </row>
     <row r="108" spans="1:11">
-      <c r="A108" s="33" t="s">
+      <c r="A108" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B108" s="34"/>
+      <c r="B108" s="45"/>
       <c r="C108" s="3">
         <v>0.6</v>
       </c>
-      <c r="D108" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E108" s="34"/>
+      <c r="D108" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="E108" s="45"/>
       <c r="F108" s="3">
         <v>1.5</v>
       </c>
-      <c r="G108" s="40"/>
-      <c r="H108" s="41"/>
-      <c r="I108" s="41"/>
-      <c r="J108" s="41"/>
-      <c r="K108" s="42"/>
+      <c r="G108" s="51"/>
+      <c r="H108" s="52"/>
+      <c r="I108" s="52"/>
+      <c r="J108" s="52"/>
+      <c r="K108" s="53"/>
     </row>
     <row r="109" spans="1:11">
       <c r="A109" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B109" s="31"/>
+      <c r="B109" s="43"/>
       <c r="C109" s="4">
         <v>0</v>
       </c>
       <c r="D109" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E109" s="31"/>
+      <c r="E109" s="43"/>
       <c r="F109" s="4">
         <v>2</v>
       </c>
-      <c r="G109" s="40"/>
-      <c r="H109" s="41"/>
-      <c r="I109" s="41"/>
-      <c r="J109" s="41"/>
-      <c r="K109" s="42"/>
+      <c r="G109" s="51"/>
+      <c r="H109" s="52"/>
+      <c r="I109" s="52"/>
+      <c r="J109" s="52"/>
+      <c r="K109" s="53"/>
     </row>
     <row r="110" spans="1:11">
       <c r="A110" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B110" s="31"/>
+      <c r="B110" s="43"/>
       <c r="C110" s="4">
         <v>2</v>
       </c>
       <c r="D110" s="32"/>
-      <c r="E110" s="31"/>
+      <c r="E110" s="43"/>
       <c r="F110" s="4"/>
-      <c r="G110" s="40"/>
-      <c r="H110" s="41"/>
-      <c r="I110" s="41"/>
-      <c r="J110" s="41"/>
-      <c r="K110" s="42"/>
+      <c r="G110" s="51"/>
+      <c r="H110" s="52"/>
+      <c r="I110" s="52"/>
+      <c r="J110" s="52"/>
+      <c r="K110" s="53"/>
     </row>
     <row r="111" spans="1:11">
-      <c r="A111" s="35" t="s">
+      <c r="A111" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B111" s="36"/>
+      <c r="B111" s="47"/>
       <c r="C111" s="2">
         <v>0.4</v>
       </c>
-      <c r="D111" s="35"/>
-      <c r="E111" s="36"/>
+      <c r="D111" s="46"/>
+      <c r="E111" s="47"/>
       <c r="F111" s="2"/>
-      <c r="G111" s="40"/>
-      <c r="H111" s="41"/>
-      <c r="I111" s="41"/>
-      <c r="J111" s="41"/>
-      <c r="K111" s="42"/>
+      <c r="G111" s="51"/>
+      <c r="H111" s="52"/>
+      <c r="I111" s="52"/>
+      <c r="J111" s="52"/>
+      <c r="K111" s="53"/>
     </row>
     <row r="112" spans="1:11" ht="18.75">
       <c r="A112" s="10" t="s">
@@ -3485,7 +4019,27 @@
       <c r="K112" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="241">
+  <mergeCells count="301">
+    <mergeCell ref="Q54:AA54"/>
+    <mergeCell ref="Q45:AA45"/>
+    <mergeCell ref="Q46:S46"/>
+    <mergeCell ref="T46:V46"/>
+    <mergeCell ref="W46:AA46"/>
+    <mergeCell ref="Q47:R47"/>
+    <mergeCell ref="T47:U47"/>
+    <mergeCell ref="W47:AA53"/>
+    <mergeCell ref="Q48:R48"/>
+    <mergeCell ref="T48:U48"/>
+    <mergeCell ref="Q49:R49"/>
+    <mergeCell ref="T49:U49"/>
+    <mergeCell ref="Q50:R50"/>
+    <mergeCell ref="T50:U50"/>
+    <mergeCell ref="Q51:R51"/>
+    <mergeCell ref="T51:U51"/>
+    <mergeCell ref="Q52:R52"/>
+    <mergeCell ref="T52:U52"/>
+    <mergeCell ref="Q53:R53"/>
+    <mergeCell ref="T53:U53"/>
     <mergeCell ref="Q10:AA10"/>
     <mergeCell ref="N3:P6"/>
     <mergeCell ref="Q1:AA1"/>
@@ -3727,6 +4281,46 @@
     <mergeCell ref="T19:U19"/>
     <mergeCell ref="Q20:R20"/>
     <mergeCell ref="T20:U20"/>
+    <mergeCell ref="Q23:AA23"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="T24:V24"/>
+    <mergeCell ref="W24:AA24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="W25:AA31"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="T27:U27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="T29:U29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="Q43:AA43"/>
+    <mergeCell ref="Q32:AA32"/>
+    <mergeCell ref="Q34:AA34"/>
+    <mergeCell ref="Q35:S35"/>
+    <mergeCell ref="T35:V35"/>
+    <mergeCell ref="W35:AA35"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="T36:U36"/>
+    <mergeCell ref="W36:AA42"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="T37:U37"/>
+    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="T38:U38"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="T39:U39"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="T40:U40"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="T41:U41"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="T42:U42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update with new tests
</commit_message>
<xml_diff>
--- a/Tablut/TestTablut.xlsx
+++ b/Tablut/TestTablut.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milo\Desktop\Tablut\Tablut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70526ABD-F471-413F-8C39-E450316AA003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AEB422-39F4-4C6B-A7F1-082B7EFBB781}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="47">
   <si>
     <t>KingEncirclement</t>
   </si>
@@ -207,6 +207,15 @@
   </si>
   <si>
     <t>La partita è durata quasi 40 minuti, cioè meno del solito</t>
+  </si>
+  <si>
+    <t>Aggiunto l'elemento ZoneWayOut considerando come vie di fuga la croce sul trono</t>
+  </si>
+  <si>
+    <t>ZoneWayOut</t>
+  </si>
+  <si>
+    <t>Aggiunto l'elemento ZoneWayOut considerando come vie di fuga le colonne e righe spostate di uno rispetto alla croce</t>
   </si>
 </sst>
 </file>
@@ -549,6 +558,15 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -561,12 +579,81 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -591,89 +678,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -709,8 +718,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>2134</xdr:rowOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>116434</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -735,6 +744,56 @@
         <a:xfrm>
           <a:off x="8064500" y="11087100"/>
           <a:ext cx="2032000" cy="2059534"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>203201</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>139701</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>558801</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>88901</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Immagine 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32149576-E191-479B-9386-A929E07A5F11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16827501" y="13919201"/>
+          <a:ext cx="1549400" cy="1549400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1045,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{028B81F1-ACA3-4C72-9A53-A89403C903EE}">
   <dimension ref="A1:AA112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="W47" sqref="W47:AA53"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="75" workbookViewId="0">
+      <selection activeCell="AC69" sqref="AC69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1086,245 +1145,245 @@
       <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="34" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="16" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="18"/>
-      <c r="Q2" s="34" t="s">
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="21"/>
+      <c r="Q2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="35"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="34" t="s">
+      <c r="R2" s="17"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="35"/>
-      <c r="V2" s="36"/>
-      <c r="W2" s="16" t="s">
+      <c r="U2" s="17"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="17"/>
-      <c r="AA2" s="18"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="21"/>
     </row>
     <row r="3" spans="1:27" ht="15" customHeight="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="37"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="37"/>
+      <c r="E3" s="23"/>
       <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="39"/>
-      <c r="N3" s="56" t="s">
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="26"/>
+      <c r="N3" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="O3" s="56"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="19" t="s">
+      <c r="O3" s="37"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="37"/>
+      <c r="R3" s="23"/>
       <c r="S3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="T3" s="19" t="s">
+      <c r="T3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="U3" s="37"/>
+      <c r="U3" s="23"/>
       <c r="V3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="W3" s="21" t="s">
+      <c r="W3" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="X3" s="38"/>
-      <c r="Y3" s="38"/>
-      <c r="Z3" s="38"/>
-      <c r="AA3" s="39"/>
+      <c r="X3" s="25"/>
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25"/>
+      <c r="AA3" s="26"/>
     </row>
     <row r="4" spans="1:27">
       <c r="A4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="43"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="4">
         <v>0.1</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="43"/>
+      <c r="E4" s="31"/>
       <c r="F4" s="4">
         <v>0.2</v>
       </c>
-      <c r="G4" s="40"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="42"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="29"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="57"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="38"/>
       <c r="Q4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="R4" s="43"/>
+      <c r="R4" s="31"/>
       <c r="S4" s="4">
         <v>0</v>
       </c>
       <c r="T4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="43"/>
+      <c r="U4" s="31"/>
       <c r="V4" s="4">
         <v>0.2</v>
       </c>
-      <c r="W4" s="40"/>
-      <c r="X4" s="41"/>
-      <c r="Y4" s="41"/>
-      <c r="Z4" s="41"/>
-      <c r="AA4" s="42"/>
+      <c r="W4" s="27"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="28"/>
+      <c r="Z4" s="28"/>
+      <c r="AA4" s="29"/>
     </row>
     <row r="5" spans="1:27">
       <c r="A5" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="43"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="4">
         <v>0.2</v>
       </c>
       <c r="D5" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="43"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="4">
         <v>0.6</v>
       </c>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="42"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="29"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="56"/>
-      <c r="O5" s="56"/>
-      <c r="P5" s="57"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="38"/>
       <c r="Q5" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="R5" s="43"/>
+      <c r="R5" s="31"/>
       <c r="S5" s="4">
         <v>0.2</v>
       </c>
       <c r="T5" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="U5" s="43"/>
+      <c r="U5" s="31"/>
       <c r="V5" s="4">
         <v>0.6</v>
       </c>
-      <c r="W5" s="40"/>
-      <c r="X5" s="41"/>
-      <c r="Y5" s="41"/>
-      <c r="Z5" s="41"/>
-      <c r="AA5" s="42"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="28"/>
+      <c r="Y5" s="28"/>
+      <c r="Z5" s="28"/>
+      <c r="AA5" s="29"/>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="45"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="3">
         <v>0.4</v>
       </c>
-      <c r="D6" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="45"/>
+      <c r="D6" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="34"/>
       <c r="F6" s="3">
         <v>1.5</v>
       </c>
-      <c r="G6" s="40"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="42"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="29"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="56"/>
-      <c r="P6" s="57"/>
-      <c r="Q6" s="44" t="s">
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="R6" s="45"/>
+      <c r="R6" s="34"/>
       <c r="S6" s="3">
         <v>0.6</v>
       </c>
-      <c r="T6" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="U6" s="45"/>
+      <c r="T6" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" s="34"/>
       <c r="V6" s="3">
         <v>1.5</v>
       </c>
-      <c r="W6" s="40"/>
-      <c r="X6" s="41"/>
-      <c r="Y6" s="41"/>
-      <c r="Z6" s="41"/>
-      <c r="AA6" s="42"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="28"/>
+      <c r="Y6" s="28"/>
+      <c r="Z6" s="28"/>
+      <c r="AA6" s="29"/>
     </row>
     <row r="7" spans="1:27">
       <c r="A7" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="43"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="4">
         <v>0.5</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="43"/>
+      <c r="E7" s="31"/>
       <c r="F7" s="4">
         <v>2</v>
       </c>
-      <c r="G7" s="40"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="42"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="29"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="8"/>
@@ -1333,39 +1392,39 @@
       <c r="Q7" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="R7" s="43"/>
+      <c r="R7" s="31"/>
       <c r="S7" s="4">
         <v>0</v>
       </c>
       <c r="T7" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="U7" s="43"/>
+      <c r="U7" s="31"/>
       <c r="V7" s="4">
         <v>2</v>
       </c>
-      <c r="W7" s="40"/>
-      <c r="X7" s="41"/>
-      <c r="Y7" s="41"/>
-      <c r="Z7" s="41"/>
-      <c r="AA7" s="42"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="28"/>
+      <c r="Y7" s="28"/>
+      <c r="Z7" s="28"/>
+      <c r="AA7" s="29"/>
     </row>
     <row r="8" spans="1:27">
       <c r="A8" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="43"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="4">
         <v>1</v>
       </c>
       <c r="D8" s="32"/>
-      <c r="E8" s="43"/>
+      <c r="E8" s="31"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="42"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="29"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1374,55 +1433,55 @@
       <c r="Q8" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="R8" s="43"/>
+      <c r="R8" s="31"/>
       <c r="S8" s="4">
         <v>1.4</v>
       </c>
       <c r="T8" s="32"/>
-      <c r="U8" s="43"/>
+      <c r="U8" s="31"/>
       <c r="V8" s="4"/>
-      <c r="W8" s="40"/>
-      <c r="X8" s="41"/>
-      <c r="Y8" s="41"/>
-      <c r="Z8" s="41"/>
-      <c r="AA8" s="42"/>
+      <c r="W8" s="27"/>
+      <c r="X8" s="28"/>
+      <c r="Y8" s="28"/>
+      <c r="Z8" s="28"/>
+      <c r="AA8" s="29"/>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="47"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="2">
         <v>0</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="47"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="36"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="42"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="29"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="46" t="s">
+      <c r="Q9" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="R9" s="47"/>
+      <c r="R9" s="36"/>
       <c r="S9" s="2">
         <v>0.4</v>
       </c>
-      <c r="T9" s="46"/>
-      <c r="U9" s="47"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="36"/>
       <c r="V9" s="2"/>
-      <c r="W9" s="40"/>
-      <c r="X9" s="41"/>
-      <c r="Y9" s="41"/>
-      <c r="Z9" s="41"/>
-      <c r="AA9" s="42"/>
+      <c r="W9" s="27"/>
+      <c r="X9" s="28"/>
+      <c r="Y9" s="28"/>
+      <c r="Z9" s="28"/>
+      <c r="AA9" s="29"/>
     </row>
     <row r="10" spans="1:27" ht="18.75">
       <c r="A10" s="10" t="s">
@@ -1502,115 +1561,115 @@
       <c r="AA12" s="15"/>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="16" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="16" t="s">
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="18"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="21"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-      <c r="Q13" s="34" t="s">
+      <c r="Q13" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="R13" s="35"/>
-      <c r="S13" s="36"/>
-      <c r="T13" s="34" t="s">
+      <c r="R13" s="17"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="U13" s="35"/>
-      <c r="V13" s="36"/>
-      <c r="W13" s="16" t="s">
+      <c r="U13" s="17"/>
+      <c r="V13" s="18"/>
+      <c r="W13" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="X13" s="17"/>
-      <c r="Y13" s="17"/>
-      <c r="Z13" s="17"/>
-      <c r="AA13" s="18"/>
+      <c r="X13" s="20"/>
+      <c r="Y13" s="20"/>
+      <c r="Z13" s="20"/>
+      <c r="AA13" s="21"/>
     </row>
     <row r="14" spans="1:27">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="37"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="37"/>
+      <c r="E14" s="23"/>
       <c r="F14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="39"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="26"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-      <c r="Q14" s="19" t="s">
+      <c r="Q14" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="R14" s="37"/>
+      <c r="R14" s="23"/>
       <c r="S14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="T14" s="19" t="s">
+      <c r="T14" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="U14" s="37"/>
+      <c r="U14" s="23"/>
       <c r="V14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="W14" s="21" t="s">
+      <c r="W14" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="X14" s="38"/>
-      <c r="Y14" s="38"/>
-      <c r="Z14" s="38"/>
-      <c r="AA14" s="39"/>
+      <c r="X14" s="25"/>
+      <c r="Y14" s="25"/>
+      <c r="Z14" s="25"/>
+      <c r="AA14" s="26"/>
     </row>
     <row r="15" spans="1:27">
       <c r="A15" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="43"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="4">
         <v>0.1</v>
       </c>
       <c r="D15" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="43"/>
+      <c r="E15" s="31"/>
       <c r="F15" s="4">
         <v>0.2</v>
       </c>
-      <c r="G15" s="40"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="42"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="29"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1619,43 +1678,43 @@
       <c r="Q15" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="R15" s="43"/>
+      <c r="R15" s="31"/>
       <c r="S15" s="4">
         <v>0</v>
       </c>
       <c r="T15" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="U15" s="43"/>
+      <c r="U15" s="31"/>
       <c r="V15" s="4">
         <v>0.4</v>
       </c>
-      <c r="W15" s="40"/>
-      <c r="X15" s="41"/>
-      <c r="Y15" s="41"/>
-      <c r="Z15" s="41"/>
-      <c r="AA15" s="42"/>
+      <c r="W15" s="27"/>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="28"/>
+      <c r="Z15" s="28"/>
+      <c r="AA15" s="29"/>
     </row>
     <row r="16" spans="1:27">
       <c r="A16" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="43"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="4">
         <v>0.2</v>
       </c>
       <c r="D16" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="43"/>
+      <c r="E16" s="31"/>
       <c r="F16" s="4">
         <v>0.6</v>
       </c>
-      <c r="G16" s="40"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="42"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="29"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -1664,88 +1723,88 @@
       <c r="Q16" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="R16" s="43"/>
+      <c r="R16" s="31"/>
       <c r="S16" s="4">
         <v>0.2</v>
       </c>
       <c r="T16" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="U16" s="43"/>
+      <c r="U16" s="31"/>
       <c r="V16" s="4">
         <v>1</v>
       </c>
-      <c r="W16" s="40"/>
-      <c r="X16" s="41"/>
-      <c r="Y16" s="41"/>
-      <c r="Z16" s="41"/>
-      <c r="AA16" s="42"/>
+      <c r="W16" s="27"/>
+      <c r="X16" s="28"/>
+      <c r="Y16" s="28"/>
+      <c r="Z16" s="28"/>
+      <c r="AA16" s="29"/>
     </row>
     <row r="17" spans="1:27">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="45"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="3">
         <v>0.5</v>
       </c>
-      <c r="D17" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="45"/>
+      <c r="D17" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="34"/>
       <c r="F17" s="3">
         <v>1.5</v>
       </c>
-      <c r="G17" s="40"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="42"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="29"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
-      <c r="Q17" s="44" t="s">
+      <c r="Q17" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="R17" s="45"/>
+      <c r="R17" s="34"/>
       <c r="S17" s="3">
         <v>0.6</v>
       </c>
-      <c r="T17" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="U17" s="45"/>
+      <c r="T17" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="U17" s="34"/>
       <c r="V17" s="3">
         <v>1.5</v>
       </c>
-      <c r="W17" s="40"/>
-      <c r="X17" s="41"/>
-      <c r="Y17" s="41"/>
-      <c r="Z17" s="41"/>
-      <c r="AA17" s="42"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="28"/>
+      <c r="Y17" s="28"/>
+      <c r="Z17" s="28"/>
+      <c r="AA17" s="29"/>
     </row>
     <row r="18" spans="1:27">
       <c r="A18" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="43"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="4">
         <v>0.3</v>
       </c>
       <c r="D18" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="43"/>
+      <c r="E18" s="31"/>
       <c r="F18" s="4">
         <v>2</v>
       </c>
-      <c r="G18" s="40"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="42"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="29"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1754,39 +1813,39 @@
       <c r="Q18" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="R18" s="43"/>
+      <c r="R18" s="31"/>
       <c r="S18" s="4">
         <v>0</v>
       </c>
       <c r="T18" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="U18" s="43"/>
+      <c r="U18" s="31"/>
       <c r="V18" s="4">
         <v>2</v>
       </c>
-      <c r="W18" s="40"/>
-      <c r="X18" s="41"/>
-      <c r="Y18" s="41"/>
-      <c r="Z18" s="41"/>
-      <c r="AA18" s="42"/>
+      <c r="W18" s="27"/>
+      <c r="X18" s="28"/>
+      <c r="Y18" s="28"/>
+      <c r="Z18" s="28"/>
+      <c r="AA18" s="29"/>
     </row>
     <row r="19" spans="1:27">
       <c r="A19" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="43"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="4">
         <v>1</v>
       </c>
       <c r="D19" s="32"/>
-      <c r="E19" s="43"/>
+      <c r="E19" s="31"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="42"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="29"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -1795,55 +1854,55 @@
       <c r="Q19" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="R19" s="43"/>
+      <c r="R19" s="31"/>
       <c r="S19" s="4">
         <v>1.4</v>
       </c>
       <c r="T19" s="32"/>
-      <c r="U19" s="43"/>
+      <c r="U19" s="31"/>
       <c r="V19" s="4"/>
-      <c r="W19" s="40"/>
-      <c r="X19" s="41"/>
-      <c r="Y19" s="41"/>
-      <c r="Z19" s="41"/>
-      <c r="AA19" s="42"/>
+      <c r="W19" s="27"/>
+      <c r="X19" s="28"/>
+      <c r="Y19" s="28"/>
+      <c r="Z19" s="28"/>
+      <c r="AA19" s="29"/>
     </row>
     <row r="20" spans="1:27">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="47"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="2">
         <v>0.7</v>
       </c>
-      <c r="D20" s="46"/>
-      <c r="E20" s="47"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="36"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="42"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="29"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
-      <c r="Q20" s="46" t="s">
+      <c r="Q20" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="R20" s="47"/>
+      <c r="R20" s="36"/>
       <c r="S20" s="2">
         <v>0.4</v>
       </c>
-      <c r="T20" s="46"/>
-      <c r="U20" s="47"/>
+      <c r="T20" s="35"/>
+      <c r="U20" s="36"/>
       <c r="V20" s="2"/>
-      <c r="W20" s="40"/>
-      <c r="X20" s="41"/>
-      <c r="Y20" s="41"/>
-      <c r="Z20" s="41"/>
-      <c r="AA20" s="42"/>
+      <c r="W20" s="27"/>
+      <c r="X20" s="28"/>
+      <c r="Y20" s="28"/>
+      <c r="Z20" s="28"/>
+      <c r="AA20" s="29"/>
     </row>
     <row r="21" spans="1:27" ht="18.75">
       <c r="A21" s="10" t="s">
@@ -1923,115 +1982,115 @@
       <c r="AA23" s="15"/>
     </row>
     <row r="24" spans="1:27">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="34" t="s">
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="35"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="34" t="s">
+      <c r="E24" s="17"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="36"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="18"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
-      <c r="Q24" s="34" t="s">
+      <c r="Q24" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="R24" s="35"/>
-      <c r="S24" s="36"/>
-      <c r="T24" s="34" t="s">
+      <c r="R24" s="17"/>
+      <c r="S24" s="18"/>
+      <c r="T24" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="U24" s="35"/>
-      <c r="V24" s="36"/>
-      <c r="W24" s="16" t="s">
+      <c r="U24" s="17"/>
+      <c r="V24" s="18"/>
+      <c r="W24" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="X24" s="17"/>
-      <c r="Y24" s="17"/>
-      <c r="Z24" s="17"/>
-      <c r="AA24" s="18"/>
+      <c r="X24" s="20"/>
+      <c r="Y24" s="20"/>
+      <c r="Z24" s="20"/>
+      <c r="AA24" s="21"/>
     </row>
     <row r="25" spans="1:27" ht="15" customHeight="1">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="37"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="37"/>
+      <c r="E25" s="23"/>
       <c r="F25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="55" t="s">
+      <c r="G25" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="50"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="41"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
-      <c r="Q25" s="19" t="s">
+      <c r="Q25" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="R25" s="37"/>
+      <c r="R25" s="23"/>
       <c r="S25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="T25" s="19" t="s">
+      <c r="T25" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="U25" s="37"/>
+      <c r="U25" s="23"/>
       <c r="V25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="W25" s="21" t="s">
+      <c r="W25" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="X25" s="38"/>
-      <c r="Y25" s="38"/>
-      <c r="Z25" s="38"/>
-      <c r="AA25" s="39"/>
+      <c r="X25" s="25"/>
+      <c r="Y25" s="25"/>
+      <c r="Z25" s="25"/>
+      <c r="AA25" s="26"/>
     </row>
     <row r="26" spans="1:27">
       <c r="A26" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="43"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="4">
         <v>0.1</v>
       </c>
       <c r="D26" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="43"/>
+      <c r="E26" s="31"/>
       <c r="F26" s="4">
         <v>0.2</v>
       </c>
-      <c r="G26" s="51"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="53"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="44"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -2040,43 +2099,43 @@
       <c r="Q26" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="R26" s="43"/>
+      <c r="R26" s="31"/>
       <c r="S26" s="4">
         <v>0</v>
       </c>
       <c r="T26" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="U26" s="43"/>
+      <c r="U26" s="31"/>
       <c r="V26" s="4">
         <v>0.4</v>
       </c>
-      <c r="W26" s="40"/>
-      <c r="X26" s="41"/>
-      <c r="Y26" s="41"/>
-      <c r="Z26" s="41"/>
-      <c r="AA26" s="42"/>
+      <c r="W26" s="27"/>
+      <c r="X26" s="28"/>
+      <c r="Y26" s="28"/>
+      <c r="Z26" s="28"/>
+      <c r="AA26" s="29"/>
     </row>
     <row r="27" spans="1:27">
       <c r="A27" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="43"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="4">
         <v>0.2</v>
       </c>
       <c r="D27" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="43"/>
+      <c r="E27" s="31"/>
       <c r="F27" s="4">
         <v>0.6</v>
       </c>
-      <c r="G27" s="51"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="53"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="44"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
@@ -2085,88 +2144,88 @@
       <c r="Q27" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="R27" s="43"/>
+      <c r="R27" s="31"/>
       <c r="S27" s="4">
         <v>0.2</v>
       </c>
       <c r="T27" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="U27" s="43"/>
+      <c r="U27" s="31"/>
       <c r="V27" s="4">
         <v>1.5</v>
       </c>
-      <c r="W27" s="40"/>
-      <c r="X27" s="41"/>
-      <c r="Y27" s="41"/>
-      <c r="Z27" s="41"/>
-      <c r="AA27" s="42"/>
+      <c r="W27" s="27"/>
+      <c r="X27" s="28"/>
+      <c r="Y27" s="28"/>
+      <c r="Z27" s="28"/>
+      <c r="AA27" s="29"/>
     </row>
     <row r="28" spans="1:27">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="45"/>
+      <c r="B28" s="34"/>
       <c r="C28" s="3">
         <v>0.6</v>
       </c>
-      <c r="D28" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" s="45"/>
+      <c r="D28" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="34"/>
       <c r="F28" s="3">
         <v>1.5</v>
       </c>
-      <c r="G28" s="51"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="52"/>
-      <c r="K28" s="53"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="44"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
-      <c r="Q28" s="44" t="s">
+      <c r="Q28" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="R28" s="45"/>
+      <c r="R28" s="34"/>
       <c r="S28" s="3">
         <v>0.6</v>
       </c>
-      <c r="T28" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="U28" s="45"/>
+      <c r="T28" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="U28" s="34"/>
       <c r="V28" s="3">
         <v>1.5</v>
       </c>
-      <c r="W28" s="40"/>
-      <c r="X28" s="41"/>
-      <c r="Y28" s="41"/>
-      <c r="Z28" s="41"/>
-      <c r="AA28" s="42"/>
+      <c r="W28" s="27"/>
+      <c r="X28" s="28"/>
+      <c r="Y28" s="28"/>
+      <c r="Z28" s="28"/>
+      <c r="AA28" s="29"/>
     </row>
     <row r="29" spans="1:27">
       <c r="A29" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="43"/>
+      <c r="B29" s="31"/>
       <c r="C29" s="4">
         <v>0</v>
       </c>
       <c r="D29" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="43"/>
+      <c r="E29" s="31"/>
       <c r="F29" s="4">
         <v>2</v>
       </c>
-      <c r="G29" s="51"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="52"/>
-      <c r="K29" s="53"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="44"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
@@ -2175,39 +2234,39 @@
       <c r="Q29" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="R29" s="43"/>
+      <c r="R29" s="31"/>
       <c r="S29" s="4">
         <v>0</v>
       </c>
       <c r="T29" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="U29" s="43"/>
+      <c r="U29" s="31"/>
       <c r="V29" s="4">
         <v>2</v>
       </c>
-      <c r="W29" s="40"/>
-      <c r="X29" s="41"/>
-      <c r="Y29" s="41"/>
-      <c r="Z29" s="41"/>
-      <c r="AA29" s="42"/>
+      <c r="W29" s="27"/>
+      <c r="X29" s="28"/>
+      <c r="Y29" s="28"/>
+      <c r="Z29" s="28"/>
+      <c r="AA29" s="29"/>
     </row>
     <row r="30" spans="1:27">
       <c r="A30" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="43"/>
+      <c r="B30" s="31"/>
       <c r="C30" s="4">
         <v>1.2</v>
       </c>
       <c r="D30" s="32"/>
-      <c r="E30" s="43"/>
+      <c r="E30" s="31"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
-      <c r="K30" s="53"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="44"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
@@ -2216,55 +2275,55 @@
       <c r="Q30" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="R30" s="43"/>
+      <c r="R30" s="31"/>
       <c r="S30" s="4">
         <v>1.4</v>
       </c>
       <c r="T30" s="32"/>
-      <c r="U30" s="43"/>
+      <c r="U30" s="31"/>
       <c r="V30" s="4"/>
-      <c r="W30" s="40"/>
-      <c r="X30" s="41"/>
-      <c r="Y30" s="41"/>
-      <c r="Z30" s="41"/>
-      <c r="AA30" s="42"/>
+      <c r="W30" s="27"/>
+      <c r="X30" s="28"/>
+      <c r="Y30" s="28"/>
+      <c r="Z30" s="28"/>
+      <c r="AA30" s="29"/>
     </row>
     <row r="31" spans="1:27">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="47"/>
+      <c r="B31" s="36"/>
       <c r="C31" s="2">
         <v>0.4</v>
       </c>
-      <c r="D31" s="46"/>
-      <c r="E31" s="47"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="36"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
-      <c r="K31" s="53"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="44"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
-      <c r="Q31" s="46" t="s">
+      <c r="Q31" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="R31" s="47"/>
+      <c r="R31" s="36"/>
       <c r="S31" s="2">
         <v>0.4</v>
       </c>
-      <c r="T31" s="46"/>
-      <c r="U31" s="47"/>
+      <c r="T31" s="35"/>
+      <c r="U31" s="36"/>
       <c r="V31" s="2"/>
-      <c r="W31" s="40"/>
-      <c r="X31" s="41"/>
-      <c r="Y31" s="41"/>
-      <c r="Z31" s="41"/>
-      <c r="AA31" s="42"/>
+      <c r="W31" s="27"/>
+      <c r="X31" s="28"/>
+      <c r="Y31" s="28"/>
+      <c r="Z31" s="28"/>
+      <c r="AA31" s="29"/>
     </row>
     <row r="32" spans="1:27" ht="18.75">
       <c r="A32" s="10" t="s">
@@ -2344,115 +2403,115 @@
       <c r="AA34" s="15"/>
     </row>
     <row r="35" spans="1:27">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="34" t="s">
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="35"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="34" t="s">
+      <c r="E35" s="17"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H35" s="35"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="36"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="18"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
-      <c r="Q35" s="16" t="s">
+      <c r="Q35" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="R35" s="17"/>
-      <c r="S35" s="18"/>
-      <c r="T35" s="16" t="s">
+      <c r="R35" s="20"/>
+      <c r="S35" s="21"/>
+      <c r="T35" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="U35" s="17"/>
-      <c r="V35" s="18"/>
-      <c r="W35" s="16" t="s">
+      <c r="U35" s="20"/>
+      <c r="V35" s="21"/>
+      <c r="W35" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="X35" s="17"/>
-      <c r="Y35" s="17"/>
-      <c r="Z35" s="17"/>
-      <c r="AA35" s="18"/>
+      <c r="X35" s="20"/>
+      <c r="Y35" s="20"/>
+      <c r="Z35" s="20"/>
+      <c r="AA35" s="21"/>
     </row>
     <row r="36" spans="1:27" ht="15" customHeight="1">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="37"/>
+      <c r="B36" s="23"/>
       <c r="C36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="37"/>
+      <c r="E36" s="23"/>
       <c r="F36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G36" s="55" t="s">
+      <c r="G36" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="H36" s="49"/>
-      <c r="I36" s="49"/>
-      <c r="J36" s="49"/>
-      <c r="K36" s="50"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="41"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
-      <c r="Q36" s="19" t="s">
+      <c r="Q36" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="R36" s="20"/>
+      <c r="R36" s="47"/>
       <c r="S36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="T36" s="19" t="s">
+      <c r="T36" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="U36" s="20"/>
+      <c r="U36" s="47"/>
       <c r="V36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="W36" s="21" t="s">
+      <c r="W36" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="X36" s="22"/>
-      <c r="Y36" s="22"/>
-      <c r="Z36" s="22"/>
-      <c r="AA36" s="23"/>
+      <c r="X36" s="48"/>
+      <c r="Y36" s="48"/>
+      <c r="Z36" s="48"/>
+      <c r="AA36" s="49"/>
     </row>
     <row r="37" spans="1:27">
       <c r="A37" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="43"/>
+      <c r="B37" s="31"/>
       <c r="C37" s="4">
         <v>0.1</v>
       </c>
       <c r="D37" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="43"/>
+      <c r="E37" s="31"/>
       <c r="F37" s="4">
         <v>0.2</v>
       </c>
-      <c r="G37" s="51"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="52"/>
-      <c r="J37" s="52"/>
-      <c r="K37" s="53"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
+      <c r="K37" s="44"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
@@ -2461,43 +2520,43 @@
       <c r="Q37" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="R37" s="31"/>
+      <c r="R37" s="56"/>
       <c r="S37" s="4">
         <v>0</v>
       </c>
       <c r="T37" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="U37" s="33"/>
+      <c r="U37" s="57"/>
       <c r="V37" s="4">
         <v>0.2</v>
       </c>
-      <c r="W37" s="24"/>
-      <c r="X37" s="25"/>
-      <c r="Y37" s="25"/>
-      <c r="Z37" s="25"/>
-      <c r="AA37" s="26"/>
+      <c r="W37" s="50"/>
+      <c r="X37" s="51"/>
+      <c r="Y37" s="51"/>
+      <c r="Z37" s="51"/>
+      <c r="AA37" s="52"/>
     </row>
     <row r="38" spans="1:27">
       <c r="A38" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="43"/>
+      <c r="B38" s="31"/>
       <c r="C38" s="4">
         <v>0.2</v>
       </c>
       <c r="D38" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="43"/>
+      <c r="E38" s="31"/>
       <c r="F38" s="4">
         <v>0.6</v>
       </c>
-      <c r="G38" s="51"/>
-      <c r="H38" s="52"/>
-      <c r="I38" s="52"/>
-      <c r="J38" s="52"/>
-      <c r="K38" s="53"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="43"/>
+      <c r="K38" s="44"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
@@ -2506,166 +2565,166 @@
       <c r="Q38" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="R38" s="33"/>
+      <c r="R38" s="57"/>
       <c r="S38" s="4">
         <v>0.2</v>
       </c>
       <c r="T38" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="U38" s="33"/>
+      <c r="U38" s="57"/>
       <c r="V38" s="4">
         <v>0.6</v>
       </c>
-      <c r="W38" s="24"/>
-      <c r="X38" s="25"/>
-      <c r="Y38" s="25"/>
-      <c r="Z38" s="25"/>
-      <c r="AA38" s="26"/>
+      <c r="W38" s="50"/>
+      <c r="X38" s="51"/>
+      <c r="Y38" s="51"/>
+      <c r="Z38" s="51"/>
+      <c r="AA38" s="52"/>
     </row>
     <row r="39" spans="1:27">
-      <c r="A39" s="44" t="s">
+      <c r="A39" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="45"/>
+      <c r="B39" s="34"/>
       <c r="C39" s="3">
         <v>0.6</v>
       </c>
-      <c r="D39" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="E39" s="45"/>
+      <c r="D39" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="34"/>
       <c r="F39" s="3">
         <v>1.5</v>
       </c>
-      <c r="G39" s="51"/>
-      <c r="H39" s="52"/>
-      <c r="I39" s="52"/>
-      <c r="J39" s="52"/>
-      <c r="K39" s="53"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
+      <c r="K39" s="44"/>
       <c r="Q39" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="R39" s="33"/>
+      <c r="R39" s="57"/>
       <c r="S39" s="3">
         <v>0.6</v>
       </c>
       <c r="T39" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="U39" s="33"/>
+      <c r="U39" s="57"/>
       <c r="V39" s="3">
         <v>1.5</v>
       </c>
-      <c r="W39" s="24"/>
-      <c r="X39" s="25"/>
-      <c r="Y39" s="25"/>
-      <c r="Z39" s="25"/>
-      <c r="AA39" s="26"/>
+      <c r="W39" s="50"/>
+      <c r="X39" s="51"/>
+      <c r="Y39" s="51"/>
+      <c r="Z39" s="51"/>
+      <c r="AA39" s="52"/>
     </row>
     <row r="40" spans="1:27">
       <c r="A40" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="43"/>
+      <c r="B40" s="31"/>
       <c r="C40" s="4">
         <v>0.25</v>
       </c>
       <c r="D40" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="43"/>
+      <c r="E40" s="31"/>
       <c r="F40" s="4">
         <v>2</v>
       </c>
-      <c r="G40" s="51"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="52"/>
-      <c r="J40" s="52"/>
-      <c r="K40" s="53"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="44"/>
       <c r="Q40" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="R40" s="33"/>
+      <c r="R40" s="57"/>
       <c r="S40" s="4">
         <v>0</v>
       </c>
       <c r="T40" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="U40" s="33"/>
+      <c r="U40" s="57"/>
       <c r="V40" s="4">
         <v>2</v>
       </c>
-      <c r="W40" s="24"/>
-      <c r="X40" s="25"/>
-      <c r="Y40" s="25"/>
-      <c r="Z40" s="25"/>
-      <c r="AA40" s="26"/>
+      <c r="W40" s="50"/>
+      <c r="X40" s="51"/>
+      <c r="Y40" s="51"/>
+      <c r="Z40" s="51"/>
+      <c r="AA40" s="52"/>
     </row>
     <row r="41" spans="1:27">
       <c r="A41" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="43"/>
+      <c r="B41" s="31"/>
       <c r="C41" s="4">
         <v>1.2</v>
       </c>
       <c r="D41" s="32"/>
-      <c r="E41" s="43"/>
+      <c r="E41" s="31"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="52"/>
-      <c r="I41" s="52"/>
-      <c r="J41" s="52"/>
-      <c r="K41" s="53"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="44"/>
       <c r="Q41" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="R41" s="33"/>
+      <c r="R41" s="57"/>
       <c r="S41" s="4">
         <v>1.4</v>
       </c>
       <c r="T41" s="32"/>
-      <c r="U41" s="33"/>
+      <c r="U41" s="57"/>
       <c r="V41" s="4"/>
-      <c r="W41" s="24"/>
-      <c r="X41" s="25"/>
-      <c r="Y41" s="25"/>
-      <c r="Z41" s="25"/>
-      <c r="AA41" s="26"/>
+      <c r="W41" s="50"/>
+      <c r="X41" s="51"/>
+      <c r="Y41" s="51"/>
+      <c r="Z41" s="51"/>
+      <c r="AA41" s="52"/>
     </row>
     <row r="42" spans="1:27">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="47"/>
+      <c r="B42" s="36"/>
       <c r="C42" s="2">
         <v>0.4</v>
       </c>
-      <c r="D42" s="46"/>
-      <c r="E42" s="47"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="36"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="52"/>
-      <c r="I42" s="52"/>
-      <c r="J42" s="52"/>
-      <c r="K42" s="53"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
+      <c r="K42" s="44"/>
       <c r="Q42" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="R42" s="33"/>
+      <c r="R42" s="57"/>
       <c r="S42" s="2">
         <v>0.4</v>
       </c>
       <c r="T42" s="32"/>
-      <c r="U42" s="33"/>
+      <c r="U42" s="57"/>
       <c r="V42" s="2"/>
-      <c r="W42" s="27"/>
-      <c r="X42" s="28"/>
-      <c r="Y42" s="28"/>
-      <c r="Z42" s="28"/>
-      <c r="AA42" s="29"/>
+      <c r="W42" s="53"/>
+      <c r="X42" s="54"/>
+      <c r="Y42" s="54"/>
+      <c r="Z42" s="54"/>
+      <c r="AA42" s="55"/>
     </row>
     <row r="43" spans="1:27" ht="18.75">
       <c r="A43" s="10" t="s">
@@ -2724,308 +2783,308 @@
       <c r="AA45" s="15"/>
     </row>
     <row r="46" spans="1:27">
-      <c r="A46" s="34" t="s">
+      <c r="A46" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="35"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="34" t="s">
+      <c r="B46" s="17"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="35"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="34" t="s">
+      <c r="E46" s="17"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H46" s="35"/>
-      <c r="I46" s="35"/>
-      <c r="J46" s="35"/>
-      <c r="K46" s="36"/>
-      <c r="Q46" s="34" t="s">
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="18"/>
+      <c r="Q46" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="R46" s="35"/>
-      <c r="S46" s="36"/>
-      <c r="T46" s="34" t="s">
+      <c r="R46" s="17"/>
+      <c r="S46" s="18"/>
+      <c r="T46" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="U46" s="35"/>
-      <c r="V46" s="36"/>
-      <c r="W46" s="16" t="s">
+      <c r="U46" s="17"/>
+      <c r="V46" s="18"/>
+      <c r="W46" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="X46" s="17"/>
-      <c r="Y46" s="17"/>
-      <c r="Z46" s="17"/>
-      <c r="AA46" s="18"/>
+      <c r="X46" s="20"/>
+      <c r="Y46" s="20"/>
+      <c r="Z46" s="20"/>
+      <c r="AA46" s="21"/>
     </row>
     <row r="47" spans="1:27">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="37"/>
+      <c r="B47" s="23"/>
       <c r="C47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="19" t="s">
+      <c r="D47" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E47" s="37"/>
+      <c r="E47" s="23"/>
       <c r="F47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G47" s="55" t="s">
+      <c r="G47" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="H47" s="49"/>
-      <c r="I47" s="49"/>
-      <c r="J47" s="49"/>
-      <c r="K47" s="50"/>
-      <c r="Q47" s="19" t="s">
+      <c r="H47" s="40"/>
+      <c r="I47" s="40"/>
+      <c r="J47" s="40"/>
+      <c r="K47" s="41"/>
+      <c r="Q47" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="R47" s="37"/>
+      <c r="R47" s="23"/>
       <c r="S47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="T47" s="19" t="s">
+      <c r="T47" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="U47" s="37"/>
+      <c r="U47" s="23"/>
       <c r="V47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="W47" s="21" t="s">
+      <c r="W47" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="X47" s="38"/>
-      <c r="Y47" s="38"/>
-      <c r="Z47" s="38"/>
-      <c r="AA47" s="39"/>
+      <c r="X47" s="25"/>
+      <c r="Y47" s="25"/>
+      <c r="Z47" s="25"/>
+      <c r="AA47" s="26"/>
     </row>
     <row r="48" spans="1:27">
       <c r="A48" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B48" s="43"/>
+      <c r="B48" s="31"/>
       <c r="C48" s="4">
         <v>0.1</v>
       </c>
       <c r="D48" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E48" s="43"/>
+      <c r="E48" s="31"/>
       <c r="F48" s="4">
         <v>0.2</v>
       </c>
-      <c r="G48" s="51"/>
-      <c r="H48" s="52"/>
-      <c r="I48" s="52"/>
-      <c r="J48" s="52"/>
-      <c r="K48" s="53"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="44"/>
       <c r="Q48" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="R48" s="43"/>
+      <c r="R48" s="31"/>
       <c r="S48" s="4">
         <v>0</v>
       </c>
       <c r="T48" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="U48" s="43"/>
+      <c r="U48" s="31"/>
       <c r="V48" s="4">
         <v>0.2</v>
       </c>
-      <c r="W48" s="40"/>
-      <c r="X48" s="41"/>
-      <c r="Y48" s="41"/>
-      <c r="Z48" s="41"/>
-      <c r="AA48" s="42"/>
+      <c r="W48" s="27"/>
+      <c r="X48" s="28"/>
+      <c r="Y48" s="28"/>
+      <c r="Z48" s="28"/>
+      <c r="AA48" s="29"/>
     </row>
     <row r="49" spans="1:27">
       <c r="A49" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B49" s="43"/>
+      <c r="B49" s="31"/>
       <c r="C49" s="4">
         <v>0.2</v>
       </c>
       <c r="D49" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="43"/>
+      <c r="E49" s="31"/>
       <c r="F49" s="4">
         <v>0.6</v>
       </c>
-      <c r="G49" s="51"/>
-      <c r="H49" s="52"/>
-      <c r="I49" s="52"/>
-      <c r="J49" s="52"/>
-      <c r="K49" s="53"/>
+      <c r="G49" s="42"/>
+      <c r="H49" s="43"/>
+      <c r="I49" s="43"/>
+      <c r="J49" s="43"/>
+      <c r="K49" s="44"/>
       <c r="Q49" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="R49" s="43"/>
+      <c r="R49" s="31"/>
       <c r="S49" s="4">
         <v>0.2</v>
       </c>
       <c r="T49" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="U49" s="43"/>
+      <c r="U49" s="31"/>
       <c r="V49" s="4">
         <v>0.6</v>
       </c>
-      <c r="W49" s="40"/>
-      <c r="X49" s="41"/>
-      <c r="Y49" s="41"/>
-      <c r="Z49" s="41"/>
-      <c r="AA49" s="42"/>
+      <c r="W49" s="27"/>
+      <c r="X49" s="28"/>
+      <c r="Y49" s="28"/>
+      <c r="Z49" s="28"/>
+      <c r="AA49" s="29"/>
     </row>
     <row r="50" spans="1:27">
-      <c r="A50" s="44" t="s">
+      <c r="A50" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="45"/>
+      <c r="B50" s="34"/>
       <c r="C50" s="3">
         <v>0.6</v>
       </c>
-      <c r="D50" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="E50" s="45"/>
+      <c r="D50" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="34"/>
       <c r="F50" s="3">
         <v>1.5</v>
       </c>
-      <c r="G50" s="51"/>
-      <c r="H50" s="52"/>
-      <c r="I50" s="52"/>
-      <c r="J50" s="52"/>
-      <c r="K50" s="53"/>
-      <c r="Q50" s="44" t="s">
+      <c r="G50" s="42"/>
+      <c r="H50" s="43"/>
+      <c r="I50" s="43"/>
+      <c r="J50" s="43"/>
+      <c r="K50" s="44"/>
+      <c r="Q50" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="R50" s="45"/>
+      <c r="R50" s="34"/>
       <c r="S50" s="3">
         <v>0.6</v>
       </c>
-      <c r="T50" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="U50" s="45"/>
+      <c r="T50" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="U50" s="34"/>
       <c r="V50" s="3">
         <v>0.8</v>
       </c>
-      <c r="W50" s="40"/>
-      <c r="X50" s="41"/>
-      <c r="Y50" s="41"/>
-      <c r="Z50" s="41"/>
-      <c r="AA50" s="42"/>
+      <c r="W50" s="27"/>
+      <c r="X50" s="28"/>
+      <c r="Y50" s="28"/>
+      <c r="Z50" s="28"/>
+      <c r="AA50" s="29"/>
     </row>
     <row r="51" spans="1:27">
       <c r="A51" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="43"/>
+      <c r="B51" s="31"/>
       <c r="C51" s="4">
         <v>0</v>
       </c>
       <c r="D51" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="43"/>
+      <c r="E51" s="31"/>
       <c r="F51" s="4">
         <v>2</v>
       </c>
-      <c r="G51" s="51"/>
-      <c r="H51" s="52"/>
-      <c r="I51" s="52"/>
-      <c r="J51" s="52"/>
-      <c r="K51" s="53"/>
+      <c r="G51" s="42"/>
+      <c r="H51" s="43"/>
+      <c r="I51" s="43"/>
+      <c r="J51" s="43"/>
+      <c r="K51" s="44"/>
       <c r="Q51" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="R51" s="43"/>
+      <c r="R51" s="31"/>
       <c r="S51" s="4">
         <v>0</v>
       </c>
       <c r="T51" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="U51" s="43"/>
+      <c r="U51" s="31"/>
       <c r="V51" s="4">
         <v>1.4</v>
       </c>
-      <c r="W51" s="40"/>
-      <c r="X51" s="41"/>
-      <c r="Y51" s="41"/>
-      <c r="Z51" s="41"/>
-      <c r="AA51" s="42"/>
+      <c r="W51" s="27"/>
+      <c r="X51" s="28"/>
+      <c r="Y51" s="28"/>
+      <c r="Z51" s="28"/>
+      <c r="AA51" s="29"/>
     </row>
     <row r="52" spans="1:27">
       <c r="A52" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B52" s="43"/>
+      <c r="B52" s="31"/>
       <c r="C52" s="4">
         <v>1.4</v>
       </c>
       <c r="D52" s="32"/>
-      <c r="E52" s="43"/>
+      <c r="E52" s="31"/>
       <c r="F52" s="4"/>
-      <c r="G52" s="51"/>
-      <c r="H52" s="52"/>
-      <c r="I52" s="52"/>
-      <c r="J52" s="52"/>
-      <c r="K52" s="53"/>
+      <c r="G52" s="42"/>
+      <c r="H52" s="43"/>
+      <c r="I52" s="43"/>
+      <c r="J52" s="43"/>
+      <c r="K52" s="44"/>
       <c r="Q52" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="R52" s="43"/>
+      <c r="R52" s="31"/>
       <c r="S52" s="4">
         <v>1.4</v>
       </c>
       <c r="T52" s="32"/>
-      <c r="U52" s="43"/>
+      <c r="U52" s="31"/>
       <c r="V52" s="4"/>
-      <c r="W52" s="40"/>
-      <c r="X52" s="41"/>
-      <c r="Y52" s="41"/>
-      <c r="Z52" s="41"/>
-      <c r="AA52" s="42"/>
+      <c r="W52" s="27"/>
+      <c r="X52" s="28"/>
+      <c r="Y52" s="28"/>
+      <c r="Z52" s="28"/>
+      <c r="AA52" s="29"/>
     </row>
     <row r="53" spans="1:27">
-      <c r="A53" s="46" t="s">
+      <c r="A53" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="47"/>
+      <c r="B53" s="36"/>
       <c r="C53" s="2">
         <v>0.4</v>
       </c>
-      <c r="D53" s="46"/>
-      <c r="E53" s="47"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="36"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="51"/>
-      <c r="H53" s="52"/>
-      <c r="I53" s="52"/>
-      <c r="J53" s="52"/>
-      <c r="K53" s="53"/>
-      <c r="Q53" s="46" t="s">
+      <c r="G53" s="42"/>
+      <c r="H53" s="43"/>
+      <c r="I53" s="43"/>
+      <c r="J53" s="43"/>
+      <c r="K53" s="44"/>
+      <c r="Q53" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="R53" s="47"/>
+      <c r="R53" s="36"/>
       <c r="S53" s="2">
         <v>0.4</v>
       </c>
-      <c r="T53" s="46"/>
-      <c r="U53" s="47"/>
+      <c r="T53" s="35"/>
+      <c r="U53" s="36"/>
       <c r="V53" s="2"/>
-      <c r="W53" s="40"/>
-      <c r="X53" s="41"/>
-      <c r="Y53" s="41"/>
-      <c r="Z53" s="41"/>
-      <c r="AA53" s="42"/>
+      <c r="W53" s="27"/>
+      <c r="X53" s="28"/>
+      <c r="Y53" s="28"/>
+      <c r="Z53" s="28"/>
+      <c r="AA53" s="29"/>
     </row>
     <row r="54" spans="1:27" ht="18.75">
       <c r="A54" s="10" t="s">
@@ -3070,6 +3129,21 @@
       <c r="J55" s="6"/>
       <c r="K55" s="7"/>
     </row>
+    <row r="56" spans="1:27" ht="21">
+      <c r="Q56" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="R56" s="14"/>
+      <c r="S56" s="14"/>
+      <c r="T56" s="14"/>
+      <c r="U56" s="14"/>
+      <c r="V56" s="14"/>
+      <c r="W56" s="14"/>
+      <c r="X56" s="14"/>
+      <c r="Y56" s="14"/>
+      <c r="Z56" s="14"/>
+      <c r="AA56" s="15"/>
+    </row>
     <row r="57" spans="1:27" ht="21">
       <c r="A57" s="13" t="s">
         <v>25</v>
@@ -3084,168 +3158,329 @@
       <c r="I57" s="14"/>
       <c r="J57" s="14"/>
       <c r="K57" s="15"/>
+      <c r="Q57" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="R57" s="17"/>
+      <c r="S57" s="18"/>
+      <c r="T57" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="U57" s="17"/>
+      <c r="V57" s="18"/>
+      <c r="W57" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="X57" s="20"/>
+      <c r="Y57" s="20"/>
+      <c r="Z57" s="20"/>
+      <c r="AA57" s="21"/>
     </row>
     <row r="58" spans="1:27">
-      <c r="A58" s="34" t="s">
+      <c r="A58" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B58" s="35"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="34" t="s">
+      <c r="B58" s="17"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E58" s="35"/>
-      <c r="F58" s="36"/>
-      <c r="G58" s="34" t="s">
+      <c r="E58" s="17"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H58" s="35"/>
-      <c r="I58" s="35"/>
-      <c r="J58" s="35"/>
-      <c r="K58" s="36"/>
-    </row>
-    <row r="59" spans="1:27">
-      <c r="A59" s="19" t="s">
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17"/>
+      <c r="K58" s="18"/>
+      <c r="Q58" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="37"/>
+      <c r="R58" s="23"/>
+      <c r="S58" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T58" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="U58" s="23"/>
+      <c r="V58" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W58" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="X58" s="25"/>
+      <c r="Y58" s="25"/>
+      <c r="Z58" s="25"/>
+      <c r="AA58" s="26"/>
+    </row>
+    <row r="59" spans="1:27" ht="15" customHeight="1">
+      <c r="A59" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" s="23"/>
       <c r="C59" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D59" s="19" t="s">
+      <c r="D59" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E59" s="37"/>
+      <c r="E59" s="23"/>
       <c r="F59" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G59" s="55" t="s">
+      <c r="G59" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="H59" s="49"/>
-      <c r="I59" s="49"/>
-      <c r="J59" s="49"/>
-      <c r="K59" s="50"/>
+      <c r="H59" s="40"/>
+      <c r="I59" s="40"/>
+      <c r="J59" s="40"/>
+      <c r="K59" s="41"/>
+      <c r="Q59" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="R59" s="31"/>
+      <c r="S59" s="4">
+        <v>0</v>
+      </c>
+      <c r="T59" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="U59" s="31"/>
+      <c r="V59" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W59" s="27"/>
+      <c r="X59" s="28"/>
+      <c r="Y59" s="28"/>
+      <c r="Z59" s="28"/>
+      <c r="AA59" s="29"/>
     </row>
     <row r="60" spans="1:27">
       <c r="A60" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B60" s="43"/>
+      <c r="B60" s="31"/>
       <c r="C60" s="4">
         <v>0.1</v>
       </c>
       <c r="D60" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E60" s="43"/>
+      <c r="E60" s="31"/>
       <c r="F60" s="4">
         <v>0.2</v>
       </c>
-      <c r="G60" s="51"/>
-      <c r="H60" s="52"/>
-      <c r="I60" s="52"/>
-      <c r="J60" s="52"/>
-      <c r="K60" s="53"/>
+      <c r="G60" s="42"/>
+      <c r="H60" s="43"/>
+      <c r="I60" s="43"/>
+      <c r="J60" s="43"/>
+      <c r="K60" s="44"/>
+      <c r="Q60" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="R60" s="31"/>
+      <c r="S60" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="T60" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="U60" s="31"/>
+      <c r="V60" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="W60" s="27"/>
+      <c r="X60" s="28"/>
+      <c r="Y60" s="28"/>
+      <c r="Z60" s="28"/>
+      <c r="AA60" s="29"/>
     </row>
     <row r="61" spans="1:27">
       <c r="A61" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B61" s="43"/>
+      <c r="B61" s="31"/>
       <c r="C61" s="4">
         <v>0.2</v>
       </c>
       <c r="D61" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E61" s="43"/>
+      <c r="E61" s="31"/>
       <c r="F61" s="4">
         <v>0.6</v>
       </c>
-      <c r="G61" s="51"/>
-      <c r="H61" s="52"/>
-      <c r="I61" s="52"/>
-      <c r="J61" s="52"/>
-      <c r="K61" s="53"/>
+      <c r="G61" s="42"/>
+      <c r="H61" s="43"/>
+      <c r="I61" s="43"/>
+      <c r="J61" s="43"/>
+      <c r="K61" s="44"/>
+      <c r="Q61" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="R61" s="34"/>
+      <c r="S61" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="T61" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="U61" s="34"/>
+      <c r="V61" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="W61" s="27"/>
+      <c r="X61" s="28"/>
+      <c r="Y61" s="28"/>
+      <c r="Z61" s="28"/>
+      <c r="AA61" s="29"/>
     </row>
     <row r="62" spans="1:27">
-      <c r="A62" s="44" t="s">
+      <c r="A62" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B62" s="45"/>
+      <c r="B62" s="34"/>
       <c r="C62" s="3">
         <v>0.7</v>
       </c>
-      <c r="D62" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="E62" s="45"/>
+      <c r="D62" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="34"/>
       <c r="F62" s="3">
         <v>1.5</v>
       </c>
-      <c r="G62" s="51"/>
-      <c r="H62" s="52"/>
-      <c r="I62" s="52"/>
-      <c r="J62" s="52"/>
-      <c r="K62" s="53"/>
+      <c r="G62" s="42"/>
+      <c r="H62" s="43"/>
+      <c r="I62" s="43"/>
+      <c r="J62" s="43"/>
+      <c r="K62" s="44"/>
+      <c r="Q62" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="R62" s="31"/>
+      <c r="S62" s="4">
+        <v>0</v>
+      </c>
+      <c r="T62" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="U62" s="31"/>
+      <c r="V62" s="4">
+        <v>2</v>
+      </c>
+      <c r="W62" s="27"/>
+      <c r="X62" s="28"/>
+      <c r="Y62" s="28"/>
+      <c r="Z62" s="28"/>
+      <c r="AA62" s="29"/>
     </row>
     <row r="63" spans="1:27">
       <c r="A63" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B63" s="43"/>
+      <c r="B63" s="31"/>
       <c r="C63" s="4">
         <v>0</v>
       </c>
       <c r="D63" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E63" s="43"/>
+      <c r="E63" s="31"/>
       <c r="F63" s="4">
         <v>2</v>
       </c>
-      <c r="G63" s="51"/>
-      <c r="H63" s="52"/>
-      <c r="I63" s="52"/>
-      <c r="J63" s="52"/>
-      <c r="K63" s="53"/>
+      <c r="G63" s="42"/>
+      <c r="H63" s="43"/>
+      <c r="I63" s="43"/>
+      <c r="J63" s="43"/>
+      <c r="K63" s="44"/>
+      <c r="Q63" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="R63" s="31"/>
+      <c r="S63" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="T63" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="U63" s="31"/>
+      <c r="V63" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="W63" s="27"/>
+      <c r="X63" s="28"/>
+      <c r="Y63" s="28"/>
+      <c r="Z63" s="28"/>
+      <c r="AA63" s="29"/>
     </row>
     <row r="64" spans="1:27">
       <c r="A64" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B64" s="43"/>
+      <c r="B64" s="31"/>
       <c r="C64" s="4">
         <v>1.5</v>
       </c>
       <c r="D64" s="32"/>
-      <c r="E64" s="43"/>
+      <c r="E64" s="31"/>
       <c r="F64" s="4"/>
-      <c r="G64" s="51"/>
-      <c r="H64" s="52"/>
-      <c r="I64" s="52"/>
-      <c r="J64" s="52"/>
-      <c r="K64" s="53"/>
-    </row>
-    <row r="65" spans="1:11">
-      <c r="A65" s="46" t="s">
+      <c r="G64" s="42"/>
+      <c r="H64" s="43"/>
+      <c r="I64" s="43"/>
+      <c r="J64" s="43"/>
+      <c r="K64" s="44"/>
+      <c r="Q64" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B65" s="47"/>
+      <c r="R64" s="36"/>
+      <c r="S64" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T64" s="35"/>
+      <c r="U64" s="36"/>
+      <c r="V64" s="2"/>
+      <c r="W64" s="27"/>
+      <c r="X64" s="28"/>
+      <c r="Y64" s="28"/>
+      <c r="Z64" s="28"/>
+      <c r="AA64" s="29"/>
+    </row>
+    <row r="65" spans="1:27" ht="18.75">
+      <c r="A65" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" s="36"/>
       <c r="C65" s="2">
         <v>0.4</v>
       </c>
-      <c r="D65" s="46"/>
-      <c r="E65" s="47"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="36"/>
       <c r="F65" s="2"/>
-      <c r="G65" s="51"/>
-      <c r="H65" s="52"/>
-      <c r="I65" s="52"/>
-      <c r="J65" s="52"/>
-      <c r="K65" s="53"/>
-    </row>
-    <row r="66" spans="1:11" ht="18.75">
+      <c r="G65" s="42"/>
+      <c r="H65" s="43"/>
+      <c r="I65" s="43"/>
+      <c r="J65" s="43"/>
+      <c r="K65" s="44"/>
+      <c r="Q65" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R65" s="11"/>
+      <c r="S65" s="11"/>
+      <c r="T65" s="11"/>
+      <c r="U65" s="11"/>
+      <c r="V65" s="11"/>
+      <c r="W65" s="11"/>
+      <c r="X65" s="11"/>
+      <c r="Y65" s="11"/>
+      <c r="Z65" s="11"/>
+      <c r="AA65" s="12"/>
+    </row>
+    <row r="66" spans="1:27" ht="18.75">
       <c r="A66" s="10" t="s">
         <v>27</v>
       </c>
@@ -3260,7 +3495,22 @@
       <c r="J66" s="11"/>
       <c r="K66" s="12"/>
     </row>
-    <row r="68" spans="1:11" ht="21">
+    <row r="67" spans="1:27" ht="21">
+      <c r="Q67" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="R67" s="14"/>
+      <c r="S67" s="14"/>
+      <c r="T67" s="14"/>
+      <c r="U67" s="14"/>
+      <c r="V67" s="14"/>
+      <c r="W67" s="14"/>
+      <c r="X67" s="14"/>
+      <c r="Y67" s="14"/>
+      <c r="Z67" s="14"/>
+      <c r="AA67" s="15"/>
+    </row>
+    <row r="68" spans="1:27" ht="21">
       <c r="A68" s="13" t="s">
         <v>28</v>
       </c>
@@ -3274,166 +3524,327 @@
       <c r="I68" s="14"/>
       <c r="J68" s="14"/>
       <c r="K68" s="15"/>
-    </row>
-    <row r="69" spans="1:11">
-      <c r="A69" s="34" t="s">
+      <c r="Q68" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B69" s="35"/>
-      <c r="C69" s="36"/>
-      <c r="D69" s="34" t="s">
+      <c r="R68" s="17"/>
+      <c r="S68" s="18"/>
+      <c r="T68" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E69" s="35"/>
-      <c r="F69" s="36"/>
-      <c r="G69" s="34" t="s">
+      <c r="U68" s="17"/>
+      <c r="V68" s="18"/>
+      <c r="W68" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H69" s="35"/>
-      <c r="I69" s="35"/>
-      <c r="J69" s="35"/>
-      <c r="K69" s="36"/>
-    </row>
-    <row r="70" spans="1:11">
-      <c r="A70" s="19" t="s">
+      <c r="X68" s="20"/>
+      <c r="Y68" s="20"/>
+      <c r="Z68" s="20"/>
+      <c r="AA68" s="21"/>
+    </row>
+    <row r="69" spans="1:27">
+      <c r="A69" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69" s="17"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E69" s="17"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H69" s="17"/>
+      <c r="I69" s="17"/>
+      <c r="J69" s="17"/>
+      <c r="K69" s="18"/>
+      <c r="Q69" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B70" s="37"/>
+      <c r="R69" s="23"/>
+      <c r="S69" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T69" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="U69" s="23"/>
+      <c r="V69" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W69" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="X69" s="25"/>
+      <c r="Y69" s="25"/>
+      <c r="Z69" s="25"/>
+      <c r="AA69" s="26"/>
+    </row>
+    <row r="70" spans="1:27">
+      <c r="A70" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" s="23"/>
       <c r="C70" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D70" s="19" t="s">
+      <c r="D70" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="37"/>
+      <c r="E70" s="23"/>
       <c r="F70" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G70" s="55"/>
-      <c r="H70" s="49"/>
-      <c r="I70" s="49"/>
-      <c r="J70" s="49"/>
-      <c r="K70" s="50"/>
-    </row>
-    <row r="71" spans="1:11">
+      <c r="G70" s="39"/>
+      <c r="H70" s="40"/>
+      <c r="I70" s="40"/>
+      <c r="J70" s="40"/>
+      <c r="K70" s="41"/>
+      <c r="Q70" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="R70" s="31"/>
+      <c r="S70" s="4">
+        <v>0</v>
+      </c>
+      <c r="T70" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="U70" s="31"/>
+      <c r="V70" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W70" s="27"/>
+      <c r="X70" s="28"/>
+      <c r="Y70" s="28"/>
+      <c r="Z70" s="28"/>
+      <c r="AA70" s="29"/>
+    </row>
+    <row r="71" spans="1:27">
       <c r="A71" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B71" s="43"/>
+      <c r="B71" s="31"/>
       <c r="C71" s="4">
         <v>0.1</v>
       </c>
       <c r="D71" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E71" s="43"/>
+      <c r="E71" s="31"/>
       <c r="F71" s="4">
         <v>0.2</v>
       </c>
-      <c r="G71" s="51"/>
-      <c r="H71" s="52"/>
-      <c r="I71" s="52"/>
-      <c r="J71" s="52"/>
-      <c r="K71" s="53"/>
-    </row>
-    <row r="72" spans="1:11">
+      <c r="G71" s="42"/>
+      <c r="H71" s="43"/>
+      <c r="I71" s="43"/>
+      <c r="J71" s="43"/>
+      <c r="K71" s="44"/>
+      <c r="Q71" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="R71" s="31"/>
+      <c r="S71" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="T71" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="U71" s="31"/>
+      <c r="V71" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="W71" s="27"/>
+      <c r="X71" s="28"/>
+      <c r="Y71" s="28"/>
+      <c r="Z71" s="28"/>
+      <c r="AA71" s="29"/>
+    </row>
+    <row r="72" spans="1:27">
       <c r="A72" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B72" s="43"/>
+      <c r="B72" s="31"/>
       <c r="C72" s="4">
         <v>0.4</v>
       </c>
       <c r="D72" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E72" s="43"/>
+      <c r="E72" s="31"/>
       <c r="F72" s="4">
         <v>0.6</v>
       </c>
-      <c r="G72" s="51"/>
-      <c r="H72" s="52"/>
-      <c r="I72" s="52"/>
-      <c r="J72" s="52"/>
-      <c r="K72" s="53"/>
-    </row>
-    <row r="73" spans="1:11">
-      <c r="A73" s="44" t="s">
+      <c r="G72" s="42"/>
+      <c r="H72" s="43"/>
+      <c r="I72" s="43"/>
+      <c r="J72" s="43"/>
+      <c r="K72" s="44"/>
+      <c r="Q72" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B73" s="45"/>
+      <c r="R72" s="34"/>
+      <c r="S72" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="T72" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="U72" s="34"/>
+      <c r="V72" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="W72" s="27"/>
+      <c r="X72" s="28"/>
+      <c r="Y72" s="28"/>
+      <c r="Z72" s="28"/>
+      <c r="AA72" s="29"/>
+    </row>
+    <row r="73" spans="1:27">
+      <c r="A73" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="34"/>
       <c r="C73" s="3">
         <v>1</v>
       </c>
-      <c r="D73" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="E73" s="45"/>
+      <c r="D73" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="34"/>
       <c r="F73" s="3">
         <v>1.5</v>
       </c>
-      <c r="G73" s="51"/>
-      <c r="H73" s="52"/>
-      <c r="I73" s="52"/>
-      <c r="J73" s="52"/>
-      <c r="K73" s="53"/>
-    </row>
-    <row r="74" spans="1:11">
+      <c r="G73" s="42"/>
+      <c r="H73" s="43"/>
+      <c r="I73" s="43"/>
+      <c r="J73" s="43"/>
+      <c r="K73" s="44"/>
+      <c r="Q73" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="R73" s="31"/>
+      <c r="S73" s="4">
+        <v>0</v>
+      </c>
+      <c r="T73" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="U73" s="31"/>
+      <c r="V73" s="4">
+        <v>2</v>
+      </c>
+      <c r="W73" s="27"/>
+      <c r="X73" s="28"/>
+      <c r="Y73" s="28"/>
+      <c r="Z73" s="28"/>
+      <c r="AA73" s="29"/>
+    </row>
+    <row r="74" spans="1:27">
       <c r="A74" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B74" s="43"/>
+      <c r="B74" s="31"/>
       <c r="C74" s="4">
         <v>0</v>
       </c>
       <c r="D74" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E74" s="43"/>
+      <c r="E74" s="31"/>
       <c r="F74" s="4">
         <v>2</v>
       </c>
-      <c r="G74" s="51"/>
-      <c r="H74" s="52"/>
-      <c r="I74" s="52"/>
-      <c r="J74" s="52"/>
-      <c r="K74" s="53"/>
-    </row>
-    <row r="75" spans="1:11">
+      <c r="G74" s="42"/>
+      <c r="H74" s="43"/>
+      <c r="I74" s="43"/>
+      <c r="J74" s="43"/>
+      <c r="K74" s="44"/>
+      <c r="Q74" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="R74" s="31"/>
+      <c r="S74" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="T74" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="U74" s="31"/>
+      <c r="V74" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="W74" s="27"/>
+      <c r="X74" s="28"/>
+      <c r="Y74" s="28"/>
+      <c r="Z74" s="28"/>
+      <c r="AA74" s="29"/>
+    </row>
+    <row r="75" spans="1:27">
       <c r="A75" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B75" s="43"/>
+      <c r="B75" s="31"/>
       <c r="C75" s="4">
         <v>1.5</v>
       </c>
       <c r="D75" s="32"/>
-      <c r="E75" s="43"/>
+      <c r="E75" s="31"/>
       <c r="F75" s="4"/>
-      <c r="G75" s="51"/>
-      <c r="H75" s="52"/>
-      <c r="I75" s="52"/>
-      <c r="J75" s="52"/>
-      <c r="K75" s="53"/>
-    </row>
-    <row r="76" spans="1:11">
-      <c r="A76" s="46" t="s">
+      <c r="G75" s="42"/>
+      <c r="H75" s="43"/>
+      <c r="I75" s="43"/>
+      <c r="J75" s="43"/>
+      <c r="K75" s="44"/>
+      <c r="Q75" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B76" s="47"/>
+      <c r="R75" s="36"/>
+      <c r="S75" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T75" s="35"/>
+      <c r="U75" s="36"/>
+      <c r="V75" s="2"/>
+      <c r="W75" s="27"/>
+      <c r="X75" s="28"/>
+      <c r="Y75" s="28"/>
+      <c r="Z75" s="28"/>
+      <c r="AA75" s="29"/>
+    </row>
+    <row r="76" spans="1:27" ht="18.75">
+      <c r="A76" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" s="36"/>
       <c r="C76" s="2">
         <v>0.5</v>
       </c>
-      <c r="D76" s="46"/>
-      <c r="E76" s="47"/>
+      <c r="D76" s="35"/>
+      <c r="E76" s="36"/>
       <c r="F76" s="2"/>
-      <c r="G76" s="51"/>
-      <c r="H76" s="52"/>
-      <c r="I76" s="52"/>
-      <c r="J76" s="52"/>
-      <c r="K76" s="53"/>
-    </row>
-    <row r="77" spans="1:11" ht="18.75">
+      <c r="G76" s="42"/>
+      <c r="H76" s="43"/>
+      <c r="I76" s="43"/>
+      <c r="J76" s="43"/>
+      <c r="K76" s="44"/>
+      <c r="Q76" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="R76" s="11"/>
+      <c r="S76" s="11"/>
+      <c r="T76" s="11"/>
+      <c r="U76" s="11"/>
+      <c r="V76" s="11"/>
+      <c r="W76" s="11"/>
+      <c r="X76" s="11"/>
+      <c r="Y76" s="11"/>
+      <c r="Z76" s="11"/>
+      <c r="AA76" s="12"/>
+    </row>
+    <row r="77" spans="1:27" ht="18.75">
       <c r="A77" s="10" t="s">
         <v>10</v>
       </c>
@@ -3448,7 +3859,7 @@
       <c r="J77" s="11"/>
       <c r="K77" s="12"/>
     </row>
-    <row r="79" spans="1:11" ht="21">
+    <row r="79" spans="1:27" ht="21">
       <c r="A79" s="13" t="s">
         <v>30</v>
       </c>
@@ -3463,165 +3874,165 @@
       <c r="J79" s="14"/>
       <c r="K79" s="15"/>
     </row>
-    <row r="80" spans="1:11">
-      <c r="A80" s="34" t="s">
+    <row r="80" spans="1:27">
+      <c r="A80" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B80" s="35"/>
-      <c r="C80" s="36"/>
-      <c r="D80" s="34" t="s">
+      <c r="B80" s="17"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E80" s="35"/>
-      <c r="F80" s="36"/>
-      <c r="G80" s="34" t="s">
+      <c r="E80" s="17"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H80" s="35"/>
-      <c r="I80" s="35"/>
-      <c r="J80" s="35"/>
-      <c r="K80" s="36"/>
+      <c r="H80" s="17"/>
+      <c r="I80" s="17"/>
+      <c r="J80" s="17"/>
+      <c r="K80" s="18"/>
     </row>
     <row r="81" spans="1:11">
-      <c r="A81" s="19" t="s">
+      <c r="A81" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B81" s="37"/>
+      <c r="B81" s="23"/>
       <c r="C81" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D81" s="19" t="s">
+      <c r="D81" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E81" s="37"/>
+      <c r="E81" s="23"/>
       <c r="F81" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G81" s="55" t="s">
+      <c r="G81" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="H81" s="49"/>
-      <c r="I81" s="49"/>
-      <c r="J81" s="49"/>
-      <c r="K81" s="50"/>
+      <c r="H81" s="40"/>
+      <c r="I81" s="40"/>
+      <c r="J81" s="40"/>
+      <c r="K81" s="41"/>
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B82" s="43"/>
+      <c r="B82" s="31"/>
       <c r="C82" s="4">
         <v>0.1</v>
       </c>
       <c r="D82" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E82" s="43"/>
+      <c r="E82" s="31"/>
       <c r="F82" s="4">
         <v>0.2</v>
       </c>
-      <c r="G82" s="51"/>
-      <c r="H82" s="52"/>
-      <c r="I82" s="52"/>
-      <c r="J82" s="52"/>
-      <c r="K82" s="53"/>
+      <c r="G82" s="42"/>
+      <c r="H82" s="43"/>
+      <c r="I82" s="43"/>
+      <c r="J82" s="43"/>
+      <c r="K82" s="44"/>
     </row>
     <row r="83" spans="1:11">
       <c r="A83" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B83" s="43"/>
+      <c r="B83" s="31"/>
       <c r="C83" s="4">
         <v>0.2</v>
       </c>
       <c r="D83" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E83" s="43"/>
+      <c r="E83" s="31"/>
       <c r="F83" s="4">
         <v>0.6</v>
       </c>
-      <c r="G83" s="51"/>
-      <c r="H83" s="52"/>
-      <c r="I83" s="52"/>
-      <c r="J83" s="52"/>
-      <c r="K83" s="53"/>
+      <c r="G83" s="42"/>
+      <c r="H83" s="43"/>
+      <c r="I83" s="43"/>
+      <c r="J83" s="43"/>
+      <c r="K83" s="44"/>
     </row>
     <row r="84" spans="1:11">
-      <c r="A84" s="44" t="s">
+      <c r="A84" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B84" s="45"/>
+      <c r="B84" s="34"/>
       <c r="C84" s="3">
         <v>0.6</v>
       </c>
-      <c r="D84" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="E84" s="45"/>
+      <c r="D84" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="34"/>
       <c r="F84" s="3">
         <v>1.5</v>
       </c>
-      <c r="G84" s="51"/>
-      <c r="H84" s="52"/>
-      <c r="I84" s="52"/>
-      <c r="J84" s="52"/>
-      <c r="K84" s="53"/>
+      <c r="G84" s="42"/>
+      <c r="H84" s="43"/>
+      <c r="I84" s="43"/>
+      <c r="J84" s="43"/>
+      <c r="K84" s="44"/>
     </row>
     <row r="85" spans="1:11">
       <c r="A85" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B85" s="43"/>
+      <c r="B85" s="31"/>
       <c r="C85" s="4">
         <v>0</v>
       </c>
       <c r="D85" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E85" s="43"/>
+      <c r="E85" s="31"/>
       <c r="F85" s="4">
         <v>2</v>
       </c>
-      <c r="G85" s="51"/>
-      <c r="H85" s="52"/>
-      <c r="I85" s="52"/>
-      <c r="J85" s="52"/>
-      <c r="K85" s="53"/>
+      <c r="G85" s="42"/>
+      <c r="H85" s="43"/>
+      <c r="I85" s="43"/>
+      <c r="J85" s="43"/>
+      <c r="K85" s="44"/>
     </row>
     <row r="86" spans="1:11">
       <c r="A86" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B86" s="43"/>
+      <c r="B86" s="31"/>
       <c r="C86" s="4">
         <v>1.4</v>
       </c>
       <c r="D86" s="32"/>
-      <c r="E86" s="43"/>
+      <c r="E86" s="31"/>
       <c r="F86" s="4"/>
-      <c r="G86" s="51"/>
-      <c r="H86" s="52"/>
-      <c r="I86" s="52"/>
-      <c r="J86" s="52"/>
-      <c r="K86" s="53"/>
+      <c r="G86" s="42"/>
+      <c r="H86" s="43"/>
+      <c r="I86" s="43"/>
+      <c r="J86" s="43"/>
+      <c r="K86" s="44"/>
     </row>
     <row r="87" spans="1:11">
-      <c r="A87" s="46" t="s">
+      <c r="A87" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B87" s="47"/>
+      <c r="B87" s="36"/>
       <c r="C87" s="2">
         <v>0.4</v>
       </c>
-      <c r="D87" s="46"/>
-      <c r="E87" s="47"/>
+      <c r="D87" s="35"/>
+      <c r="E87" s="36"/>
       <c r="F87" s="2"/>
-      <c r="G87" s="51"/>
-      <c r="H87" s="52"/>
-      <c r="I87" s="52"/>
-      <c r="J87" s="52"/>
-      <c r="K87" s="53"/>
+      <c r="G87" s="42"/>
+      <c r="H87" s="43"/>
+      <c r="I87" s="43"/>
+      <c r="J87" s="43"/>
+      <c r="K87" s="44"/>
     </row>
     <row r="88" spans="1:11" ht="18.75">
       <c r="A88" s="10" t="s">
@@ -3654,164 +4065,164 @@
       <c r="K90" s="15"/>
     </row>
     <row r="91" spans="1:11">
-      <c r="A91" s="34" t="s">
+      <c r="A91" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B91" s="35"/>
-      <c r="C91" s="36"/>
-      <c r="D91" s="34" t="s">
+      <c r="B91" s="17"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E91" s="35"/>
-      <c r="F91" s="36"/>
-      <c r="G91" s="34" t="s">
+      <c r="E91" s="17"/>
+      <c r="F91" s="18"/>
+      <c r="G91" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H91" s="35"/>
-      <c r="I91" s="35"/>
-      <c r="J91" s="35"/>
-      <c r="K91" s="36"/>
+      <c r="H91" s="17"/>
+      <c r="I91" s="17"/>
+      <c r="J91" s="17"/>
+      <c r="K91" s="18"/>
     </row>
     <row r="92" spans="1:11">
-      <c r="A92" s="19" t="s">
+      <c r="A92" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B92" s="37"/>
+      <c r="B92" s="23"/>
       <c r="C92" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D92" s="19" t="s">
+      <c r="D92" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E92" s="37"/>
+      <c r="E92" s="23"/>
       <c r="F92" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G92" s="54" t="s">
+      <c r="G92" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="H92" s="49"/>
-      <c r="I92" s="49"/>
-      <c r="J92" s="49"/>
-      <c r="K92" s="50"/>
+      <c r="H92" s="40"/>
+      <c r="I92" s="40"/>
+      <c r="J92" s="40"/>
+      <c r="K92" s="41"/>
     </row>
     <row r="93" spans="1:11">
       <c r="A93" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B93" s="43"/>
+      <c r="B93" s="31"/>
       <c r="C93" s="4">
         <v>0.1</v>
       </c>
       <c r="D93" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E93" s="43"/>
+      <c r="E93" s="31"/>
       <c r="F93" s="4">
         <v>0.2</v>
       </c>
-      <c r="G93" s="51"/>
-      <c r="H93" s="52"/>
-      <c r="I93" s="52"/>
-      <c r="J93" s="52"/>
-      <c r="K93" s="53"/>
+      <c r="G93" s="42"/>
+      <c r="H93" s="43"/>
+      <c r="I93" s="43"/>
+      <c r="J93" s="43"/>
+      <c r="K93" s="44"/>
     </row>
     <row r="94" spans="1:11">
       <c r="A94" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B94" s="43"/>
+      <c r="B94" s="31"/>
       <c r="C94" s="4">
         <v>0.2</v>
       </c>
       <c r="D94" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E94" s="43"/>
+      <c r="E94" s="31"/>
       <c r="F94" s="4">
         <v>0.6</v>
       </c>
-      <c r="G94" s="51"/>
-      <c r="H94" s="52"/>
-      <c r="I94" s="52"/>
-      <c r="J94" s="52"/>
-      <c r="K94" s="53"/>
+      <c r="G94" s="42"/>
+      <c r="H94" s="43"/>
+      <c r="I94" s="43"/>
+      <c r="J94" s="43"/>
+      <c r="K94" s="44"/>
     </row>
     <row r="95" spans="1:11">
-      <c r="A95" s="44" t="s">
+      <c r="A95" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B95" s="45"/>
+      <c r="B95" s="34"/>
       <c r="C95" s="3">
         <v>0.8</v>
       </c>
-      <c r="D95" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="E95" s="45"/>
+      <c r="D95" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" s="34"/>
       <c r="F95" s="3">
         <v>1.5</v>
       </c>
-      <c r="G95" s="51"/>
-      <c r="H95" s="52"/>
-      <c r="I95" s="52"/>
-      <c r="J95" s="52"/>
-      <c r="K95" s="53"/>
+      <c r="G95" s="42"/>
+      <c r="H95" s="43"/>
+      <c r="I95" s="43"/>
+      <c r="J95" s="43"/>
+      <c r="K95" s="44"/>
     </row>
     <row r="96" spans="1:11">
       <c r="A96" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B96" s="43"/>
+      <c r="B96" s="31"/>
       <c r="C96" s="4">
         <v>0</v>
       </c>
       <c r="D96" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E96" s="43"/>
+      <c r="E96" s="31"/>
       <c r="F96" s="4">
         <v>2</v>
       </c>
-      <c r="G96" s="51"/>
-      <c r="H96" s="52"/>
-      <c r="I96" s="52"/>
-      <c r="J96" s="52"/>
-      <c r="K96" s="53"/>
+      <c r="G96" s="42"/>
+      <c r="H96" s="43"/>
+      <c r="I96" s="43"/>
+      <c r="J96" s="43"/>
+      <c r="K96" s="44"/>
     </row>
     <row r="97" spans="1:11">
       <c r="A97" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B97" s="43"/>
+      <c r="B97" s="31"/>
       <c r="C97" s="4">
         <v>1.8</v>
       </c>
       <c r="D97" s="32"/>
-      <c r="E97" s="43"/>
+      <c r="E97" s="31"/>
       <c r="F97" s="4"/>
-      <c r="G97" s="51"/>
-      <c r="H97" s="52"/>
-      <c r="I97" s="52"/>
-      <c r="J97" s="52"/>
-      <c r="K97" s="53"/>
+      <c r="G97" s="42"/>
+      <c r="H97" s="43"/>
+      <c r="I97" s="43"/>
+      <c r="J97" s="43"/>
+      <c r="K97" s="44"/>
     </row>
     <row r="98" spans="1:11">
-      <c r="A98" s="46" t="s">
+      <c r="A98" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B98" s="47"/>
+      <c r="B98" s="36"/>
       <c r="C98" s="2">
         <v>0.4</v>
       </c>
-      <c r="D98" s="46"/>
-      <c r="E98" s="47"/>
+      <c r="D98" s="35"/>
+      <c r="E98" s="36"/>
       <c r="F98" s="2"/>
-      <c r="G98" s="51"/>
-      <c r="H98" s="52"/>
-      <c r="I98" s="52"/>
-      <c r="J98" s="52"/>
-      <c r="K98" s="53"/>
+      <c r="G98" s="42"/>
+      <c r="H98" s="43"/>
+      <c r="I98" s="43"/>
+      <c r="J98" s="43"/>
+      <c r="K98" s="44"/>
     </row>
     <row r="99" spans="1:11" ht="18.75">
       <c r="A99" s="10" t="s">
@@ -3844,164 +4255,164 @@
       <c r="K103" s="15"/>
     </row>
     <row r="104" spans="1:11">
-      <c r="A104" s="34" t="s">
+      <c r="A104" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B104" s="35"/>
-      <c r="C104" s="36"/>
-      <c r="D104" s="34" t="s">
+      <c r="B104" s="17"/>
+      <c r="C104" s="18"/>
+      <c r="D104" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E104" s="35"/>
-      <c r="F104" s="36"/>
-      <c r="G104" s="34" t="s">
+      <c r="E104" s="17"/>
+      <c r="F104" s="18"/>
+      <c r="G104" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H104" s="35"/>
-      <c r="I104" s="35"/>
-      <c r="J104" s="35"/>
-      <c r="K104" s="36"/>
+      <c r="H104" s="17"/>
+      <c r="I104" s="17"/>
+      <c r="J104" s="17"/>
+      <c r="K104" s="18"/>
     </row>
     <row r="105" spans="1:11">
-      <c r="A105" s="19" t="s">
+      <c r="A105" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B105" s="37"/>
+      <c r="B105" s="23"/>
       <c r="C105" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D105" s="19" t="s">
+      <c r="D105" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E105" s="37"/>
+      <c r="E105" s="23"/>
       <c r="F105" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G105" s="48" t="s">
+      <c r="G105" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="H105" s="49"/>
-      <c r="I105" s="49"/>
-      <c r="J105" s="49"/>
-      <c r="K105" s="50"/>
+      <c r="H105" s="40"/>
+      <c r="I105" s="40"/>
+      <c r="J105" s="40"/>
+      <c r="K105" s="41"/>
     </row>
     <row r="106" spans="1:11">
       <c r="A106" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B106" s="43"/>
+      <c r="B106" s="31"/>
       <c r="C106" s="4">
         <v>0.1</v>
       </c>
       <c r="D106" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E106" s="43"/>
+      <c r="E106" s="31"/>
       <c r="F106" s="4">
         <v>0.2</v>
       </c>
-      <c r="G106" s="51"/>
-      <c r="H106" s="52"/>
-      <c r="I106" s="52"/>
-      <c r="J106" s="52"/>
-      <c r="K106" s="53"/>
+      <c r="G106" s="42"/>
+      <c r="H106" s="43"/>
+      <c r="I106" s="43"/>
+      <c r="J106" s="43"/>
+      <c r="K106" s="44"/>
     </row>
     <row r="107" spans="1:11">
       <c r="A107" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B107" s="43"/>
+      <c r="B107" s="31"/>
       <c r="C107" s="4">
         <v>0.2</v>
       </c>
       <c r="D107" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E107" s="43"/>
+      <c r="E107" s="31"/>
       <c r="F107" s="4">
         <v>0.6</v>
       </c>
-      <c r="G107" s="51"/>
-      <c r="H107" s="52"/>
-      <c r="I107" s="52"/>
-      <c r="J107" s="52"/>
-      <c r="K107" s="53"/>
+      <c r="G107" s="42"/>
+      <c r="H107" s="43"/>
+      <c r="I107" s="43"/>
+      <c r="J107" s="43"/>
+      <c r="K107" s="44"/>
     </row>
     <row r="108" spans="1:11">
-      <c r="A108" s="44" t="s">
+      <c r="A108" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B108" s="45"/>
+      <c r="B108" s="34"/>
       <c r="C108" s="3">
         <v>0.6</v>
       </c>
-      <c r="D108" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="E108" s="45"/>
+      <c r="D108" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E108" s="34"/>
       <c r="F108" s="3">
         <v>1.5</v>
       </c>
-      <c r="G108" s="51"/>
-      <c r="H108" s="52"/>
-      <c r="I108" s="52"/>
-      <c r="J108" s="52"/>
-      <c r="K108" s="53"/>
+      <c r="G108" s="42"/>
+      <c r="H108" s="43"/>
+      <c r="I108" s="43"/>
+      <c r="J108" s="43"/>
+      <c r="K108" s="44"/>
     </row>
     <row r="109" spans="1:11">
       <c r="A109" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B109" s="43"/>
+      <c r="B109" s="31"/>
       <c r="C109" s="4">
         <v>0</v>
       </c>
       <c r="D109" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="E109" s="43"/>
+      <c r="E109" s="31"/>
       <c r="F109" s="4">
         <v>2</v>
       </c>
-      <c r="G109" s="51"/>
-      <c r="H109" s="52"/>
-      <c r="I109" s="52"/>
-      <c r="J109" s="52"/>
-      <c r="K109" s="53"/>
+      <c r="G109" s="42"/>
+      <c r="H109" s="43"/>
+      <c r="I109" s="43"/>
+      <c r="J109" s="43"/>
+      <c r="K109" s="44"/>
     </row>
     <row r="110" spans="1:11">
       <c r="A110" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B110" s="43"/>
+      <c r="B110" s="31"/>
       <c r="C110" s="4">
         <v>2</v>
       </c>
       <c r="D110" s="32"/>
-      <c r="E110" s="43"/>
+      <c r="E110" s="31"/>
       <c r="F110" s="4"/>
-      <c r="G110" s="51"/>
-      <c r="H110" s="52"/>
-      <c r="I110" s="52"/>
-      <c r="J110" s="52"/>
-      <c r="K110" s="53"/>
+      <c r="G110" s="42"/>
+      <c r="H110" s="43"/>
+      <c r="I110" s="43"/>
+      <c r="J110" s="43"/>
+      <c r="K110" s="44"/>
     </row>
     <row r="111" spans="1:11">
-      <c r="A111" s="46" t="s">
+      <c r="A111" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B111" s="47"/>
+      <c r="B111" s="36"/>
       <c r="C111" s="2">
         <v>0.4</v>
       </c>
-      <c r="D111" s="46"/>
-      <c r="E111" s="47"/>
+      <c r="D111" s="35"/>
+      <c r="E111" s="36"/>
       <c r="F111" s="2"/>
-      <c r="G111" s="51"/>
-      <c r="H111" s="52"/>
-      <c r="I111" s="52"/>
-      <c r="J111" s="52"/>
-      <c r="K111" s="53"/>
+      <c r="G111" s="42"/>
+      <c r="H111" s="43"/>
+      <c r="I111" s="43"/>
+      <c r="J111" s="43"/>
+      <c r="K111" s="44"/>
     </row>
     <row r="112" spans="1:11" ht="18.75">
       <c r="A112" s="10" t="s">
@@ -4019,126 +4430,205 @@
       <c r="K112" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="301">
-    <mergeCell ref="Q54:AA54"/>
-    <mergeCell ref="Q45:AA45"/>
-    <mergeCell ref="Q46:S46"/>
-    <mergeCell ref="T46:V46"/>
-    <mergeCell ref="W46:AA46"/>
-    <mergeCell ref="Q47:R47"/>
-    <mergeCell ref="T47:U47"/>
-    <mergeCell ref="W47:AA53"/>
-    <mergeCell ref="Q48:R48"/>
-    <mergeCell ref="T48:U48"/>
-    <mergeCell ref="Q49:R49"/>
-    <mergeCell ref="T49:U49"/>
-    <mergeCell ref="Q50:R50"/>
-    <mergeCell ref="T50:U50"/>
-    <mergeCell ref="Q51:R51"/>
-    <mergeCell ref="T51:U51"/>
-    <mergeCell ref="Q52:R52"/>
-    <mergeCell ref="T52:U52"/>
-    <mergeCell ref="Q53:R53"/>
-    <mergeCell ref="T53:U53"/>
-    <mergeCell ref="Q10:AA10"/>
-    <mergeCell ref="N3:P6"/>
-    <mergeCell ref="Q1:AA1"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="W2:AA2"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="W3:AA9"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="T9:U9"/>
-    <mergeCell ref="A77:K77"/>
-    <mergeCell ref="A68:K68"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="G69:K69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="G70:K76"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="A54:K54"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="G46:K46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="G47:K53"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A45:K45"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="G36:K42"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A32:K32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K20"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:E16"/>
+  <mergeCells count="341">
+    <mergeCell ref="Q76:AA76"/>
+    <mergeCell ref="Q67:AA67"/>
+    <mergeCell ref="Q68:S68"/>
+    <mergeCell ref="T68:V68"/>
+    <mergeCell ref="W68:AA68"/>
+    <mergeCell ref="Q69:R69"/>
+    <mergeCell ref="T69:U69"/>
+    <mergeCell ref="W69:AA75"/>
+    <mergeCell ref="Q70:R70"/>
+    <mergeCell ref="T70:U70"/>
+    <mergeCell ref="Q71:R71"/>
+    <mergeCell ref="T71:U71"/>
+    <mergeCell ref="Q72:R72"/>
+    <mergeCell ref="T72:U72"/>
+    <mergeCell ref="Q73:R73"/>
+    <mergeCell ref="T73:U73"/>
+    <mergeCell ref="Q74:R74"/>
+    <mergeCell ref="T74:U74"/>
+    <mergeCell ref="Q75:R75"/>
+    <mergeCell ref="T75:U75"/>
+    <mergeCell ref="Q56:AA56"/>
+    <mergeCell ref="Q57:S57"/>
+    <mergeCell ref="T57:V57"/>
+    <mergeCell ref="W57:AA57"/>
+    <mergeCell ref="Q58:R58"/>
+    <mergeCell ref="T58:U58"/>
+    <mergeCell ref="W58:AA64"/>
+    <mergeCell ref="Q65:AA65"/>
+    <mergeCell ref="Q59:R59"/>
+    <mergeCell ref="T59:U59"/>
+    <mergeCell ref="Q60:R60"/>
+    <mergeCell ref="T60:U60"/>
+    <mergeCell ref="Q61:R61"/>
+    <mergeCell ref="T61:U61"/>
+    <mergeCell ref="Q62:R62"/>
+    <mergeCell ref="T62:U62"/>
+    <mergeCell ref="Q63:R63"/>
+    <mergeCell ref="T63:U63"/>
+    <mergeCell ref="Q64:R64"/>
+    <mergeCell ref="T64:U64"/>
+    <mergeCell ref="Q43:AA43"/>
+    <mergeCell ref="Q32:AA32"/>
+    <mergeCell ref="Q34:AA34"/>
+    <mergeCell ref="Q35:S35"/>
+    <mergeCell ref="T35:V35"/>
+    <mergeCell ref="W35:AA35"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="T36:U36"/>
+    <mergeCell ref="W36:AA42"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="T37:U37"/>
+    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="T38:U38"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="T39:U39"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="T40:U40"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="T41:U41"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="Q23:AA23"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="T24:V24"/>
+    <mergeCell ref="W24:AA24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="W25:AA31"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="T27:U27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="T29:U29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="Q21:AA21"/>
+    <mergeCell ref="Q12:AA12"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="T13:V13"/>
+    <mergeCell ref="W13:AA13"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="W14:AA20"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="T19:U19"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="T20:U20"/>
+    <mergeCell ref="A112:K112"/>
+    <mergeCell ref="A103:K103"/>
+    <mergeCell ref="A104:C104"/>
+    <mergeCell ref="D104:F104"/>
+    <mergeCell ref="G104:K104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="G105:K111"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="A99:K99"/>
+    <mergeCell ref="A90:K90"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="G91:K91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="G92:K98"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="A88:K88"/>
+    <mergeCell ref="A79:K79"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="G80:K80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="G81:K87"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="G58:K58"/>
+    <mergeCell ref="G59:K65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="A66:K66"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="G3:K9"/>
@@ -4163,164 +4653,125 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A57:K57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="G58:K58"/>
-    <mergeCell ref="G59:K65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="A66:K66"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A88:K88"/>
-    <mergeCell ref="A79:K79"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="G80:K80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="G81:K87"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="A99:K99"/>
-    <mergeCell ref="A90:K90"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="G91:K91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="G92:K98"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="A112:K112"/>
-    <mergeCell ref="A103:K103"/>
-    <mergeCell ref="A104:C104"/>
-    <mergeCell ref="D104:F104"/>
-    <mergeCell ref="G104:K104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="G105:K111"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="Q21:AA21"/>
-    <mergeCell ref="Q12:AA12"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="T13:V13"/>
-    <mergeCell ref="W13:AA13"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="W14:AA20"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="T15:U15"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="T19:U19"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="T20:U20"/>
-    <mergeCell ref="Q23:AA23"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="T24:V24"/>
-    <mergeCell ref="W24:AA24"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="W25:AA31"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="T26:U26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="T27:U27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="T28:U28"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="T29:U29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="T31:U31"/>
-    <mergeCell ref="Q43:AA43"/>
-    <mergeCell ref="Q32:AA32"/>
-    <mergeCell ref="Q34:AA34"/>
-    <mergeCell ref="Q35:S35"/>
-    <mergeCell ref="T35:V35"/>
-    <mergeCell ref="W35:AA35"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="T36:U36"/>
-    <mergeCell ref="W36:AA42"/>
-    <mergeCell ref="Q37:R37"/>
-    <mergeCell ref="T37:U37"/>
-    <mergeCell ref="Q38:R38"/>
-    <mergeCell ref="T38:U38"/>
-    <mergeCell ref="Q39:R39"/>
-    <mergeCell ref="T39:U39"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="T40:U40"/>
-    <mergeCell ref="Q41:R41"/>
-    <mergeCell ref="T41:U41"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="A32:K32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K20"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A45:K45"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:K42"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A54:K54"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="G46:K46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="G47:K53"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="A77:K77"/>
+    <mergeCell ref="A68:K68"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="G69:K69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="G70:K76"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="Q10:AA10"/>
+    <mergeCell ref="N3:P6"/>
+    <mergeCell ref="Q1:AA1"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="W2:AA2"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="W3:AA9"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="Q54:AA54"/>
+    <mergeCell ref="Q45:AA45"/>
+    <mergeCell ref="Q46:S46"/>
+    <mergeCell ref="T46:V46"/>
+    <mergeCell ref="W46:AA46"/>
+    <mergeCell ref="Q47:R47"/>
+    <mergeCell ref="T47:U47"/>
+    <mergeCell ref="W47:AA53"/>
+    <mergeCell ref="Q48:R48"/>
+    <mergeCell ref="T48:U48"/>
+    <mergeCell ref="Q49:R49"/>
+    <mergeCell ref="T49:U49"/>
+    <mergeCell ref="Q50:R50"/>
+    <mergeCell ref="T50:U50"/>
+    <mergeCell ref="Q51:R51"/>
+    <mergeCell ref="T51:U51"/>
+    <mergeCell ref="Q52:R52"/>
+    <mergeCell ref="T52:U52"/>
+    <mergeCell ref="Q53:R53"/>
+    <mergeCell ref="T53:U53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update with test#8 in the right side
</commit_message>
<xml_diff>
--- a/Tablut/TestTablut.xlsx
+++ b/Tablut/TestTablut.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milo\Desktop\Tablut\Tablut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AEB422-39F4-4C6B-A7F1-082B7EFBB781}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7920C55B-A0AC-4983-8951-6E10CEB62991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C6A09FCF-4833-4CE2-B5C6-F2E39DCF96CA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="49">
   <si>
     <t>KingEncirclement</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>Aggiunto l'elemento ZoneWayOut considerando come vie di fuga le colonne e righe spostate di uno rispetto alla croce</t>
+  </si>
+  <si>
+    <t>Come il precedente ma con l'aggiunta dei check sulla croce del trono</t>
+  </si>
+  <si>
+    <t>TEST #8</t>
   </si>
 </sst>
 </file>
@@ -621,68 +627,68 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1105,7 +1111,7 @@
   <dimension ref="A1:AA112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" zoomScale="75" workbookViewId="0">
-      <selection activeCell="AC69" sqref="AC69"/>
+      <selection activeCell="X90" sqref="X90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1202,11 +1208,11 @@
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
       <c r="K3" s="26"/>
-      <c r="N3" s="37" t="s">
+      <c r="N3" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="O3" s="37"/>
-      <c r="P3" s="38"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="57"/>
       <c r="Q3" s="22" t="s">
         <v>6</v>
       </c>
@@ -1251,9 +1257,9 @@
       <c r="K4" s="29"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="38"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="57"/>
       <c r="Q4" s="30" t="s">
         <v>0</v>
       </c>
@@ -1296,9 +1302,9 @@
       <c r="K5" s="29"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="38"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="56"/>
+      <c r="P5" s="57"/>
       <c r="Q5" s="32" t="s">
         <v>1</v>
       </c>
@@ -1341,9 +1347,9 @@
       <c r="K6" s="29"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="38"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="57"/>
       <c r="Q6" s="33" t="s">
         <v>2</v>
       </c>
@@ -2037,13 +2043,13 @@
       <c r="F25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="39" t="s">
+      <c r="G25" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="41"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="50"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -2086,11 +2092,11 @@
       <c r="F26" s="4">
         <v>0.2</v>
       </c>
-      <c r="G26" s="42"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="44"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="53"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -2131,11 +2137,11 @@
       <c r="F27" s="4">
         <v>0.6</v>
       </c>
-      <c r="G27" s="42"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="44"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="53"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
@@ -2176,11 +2182,11 @@
       <c r="F28" s="3">
         <v>1.5</v>
       </c>
-      <c r="G28" s="42"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="44"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="53"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
@@ -2221,11 +2227,11 @@
       <c r="F29" s="4">
         <v>2</v>
       </c>
-      <c r="G29" s="42"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="44"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="53"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
@@ -2262,11 +2268,11 @@
       <c r="D30" s="32"/>
       <c r="E30" s="31"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="44"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="53"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
@@ -2299,11 +2305,11 @@
       <c r="D31" s="35"/>
       <c r="E31" s="36"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="44"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="53"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
@@ -2458,13 +2464,13 @@
       <c r="F36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G36" s="39" t="s">
+      <c r="G36" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
-      <c r="K36" s="41"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="50"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
@@ -2473,24 +2479,24 @@
       <c r="Q36" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="R36" s="47"/>
+      <c r="R36" s="37"/>
       <c r="S36" s="5" t="s">
         <v>5</v>
       </c>
       <c r="T36" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="U36" s="47"/>
+      <c r="U36" s="37"/>
       <c r="V36" s="5" t="s">
         <v>5</v>
       </c>
       <c r="W36" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="X36" s="48"/>
-      <c r="Y36" s="48"/>
-      <c r="Z36" s="48"/>
-      <c r="AA36" s="49"/>
+      <c r="X36" s="38"/>
+      <c r="Y36" s="38"/>
+      <c r="Z36" s="38"/>
+      <c r="AA36" s="39"/>
     </row>
     <row r="37" spans="1:27">
       <c r="A37" s="30" t="s">
@@ -2507,11 +2513,11 @@
       <c r="F37" s="4">
         <v>0.2</v>
       </c>
-      <c r="G37" s="42"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="44"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="53"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
@@ -2520,22 +2526,22 @@
       <c r="Q37" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="R37" s="56"/>
+      <c r="R37" s="46"/>
       <c r="S37" s="4">
         <v>0</v>
       </c>
       <c r="T37" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="U37" s="57"/>
+      <c r="U37" s="47"/>
       <c r="V37" s="4">
         <v>0.2</v>
       </c>
-      <c r="W37" s="50"/>
-      <c r="X37" s="51"/>
-      <c r="Y37" s="51"/>
-      <c r="Z37" s="51"/>
-      <c r="AA37" s="52"/>
+      <c r="W37" s="40"/>
+      <c r="X37" s="41"/>
+      <c r="Y37" s="41"/>
+      <c r="Z37" s="41"/>
+      <c r="AA37" s="42"/>
     </row>
     <row r="38" spans="1:27">
       <c r="A38" s="32" t="s">
@@ -2552,11 +2558,11 @@
       <c r="F38" s="4">
         <v>0.6</v>
       </c>
-      <c r="G38" s="42"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-      <c r="J38" s="43"/>
-      <c r="K38" s="44"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="52"/>
+      <c r="I38" s="52"/>
+      <c r="J38" s="52"/>
+      <c r="K38" s="53"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
@@ -2565,22 +2571,22 @@
       <c r="Q38" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="R38" s="57"/>
+      <c r="R38" s="47"/>
       <c r="S38" s="4">
         <v>0.2</v>
       </c>
       <c r="T38" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="U38" s="57"/>
+      <c r="U38" s="47"/>
       <c r="V38" s="4">
         <v>0.6</v>
       </c>
-      <c r="W38" s="50"/>
-      <c r="X38" s="51"/>
-      <c r="Y38" s="51"/>
-      <c r="Z38" s="51"/>
-      <c r="AA38" s="52"/>
+      <c r="W38" s="40"/>
+      <c r="X38" s="41"/>
+      <c r="Y38" s="41"/>
+      <c r="Z38" s="41"/>
+      <c r="AA38" s="42"/>
     </row>
     <row r="39" spans="1:27">
       <c r="A39" s="33" t="s">
@@ -2597,30 +2603,30 @@
       <c r="F39" s="3">
         <v>1.5</v>
       </c>
-      <c r="G39" s="42"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
-      <c r="K39" s="44"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="52"/>
+      <c r="I39" s="52"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="53"/>
       <c r="Q39" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="R39" s="57"/>
+      <c r="R39" s="47"/>
       <c r="S39" s="3">
         <v>0.6</v>
       </c>
       <c r="T39" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="U39" s="57"/>
+      <c r="U39" s="47"/>
       <c r="V39" s="3">
         <v>1.5</v>
       </c>
-      <c r="W39" s="50"/>
-      <c r="X39" s="51"/>
-      <c r="Y39" s="51"/>
-      <c r="Z39" s="51"/>
-      <c r="AA39" s="52"/>
+      <c r="W39" s="40"/>
+      <c r="X39" s="41"/>
+      <c r="Y39" s="41"/>
+      <c r="Z39" s="41"/>
+      <c r="AA39" s="42"/>
     </row>
     <row r="40" spans="1:27">
       <c r="A40" s="32" t="s">
@@ -2637,30 +2643,30 @@
       <c r="F40" s="4">
         <v>2</v>
       </c>
-      <c r="G40" s="42"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="43"/>
-      <c r="J40" s="43"/>
-      <c r="K40" s="44"/>
+      <c r="G40" s="51"/>
+      <c r="H40" s="52"/>
+      <c r="I40" s="52"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="53"/>
       <c r="Q40" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="R40" s="57"/>
+      <c r="R40" s="47"/>
       <c r="S40" s="4">
         <v>0</v>
       </c>
       <c r="T40" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="U40" s="57"/>
+      <c r="U40" s="47"/>
       <c r="V40" s="4">
         <v>2</v>
       </c>
-      <c r="W40" s="50"/>
-      <c r="X40" s="51"/>
-      <c r="Y40" s="51"/>
-      <c r="Z40" s="51"/>
-      <c r="AA40" s="52"/>
+      <c r="W40" s="40"/>
+      <c r="X40" s="41"/>
+      <c r="Y40" s="41"/>
+      <c r="Z40" s="41"/>
+      <c r="AA40" s="42"/>
     </row>
     <row r="41" spans="1:27">
       <c r="A41" s="32" t="s">
@@ -2673,26 +2679,26 @@
       <c r="D41" s="32"/>
       <c r="E41" s="31"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="43"/>
-      <c r="J41" s="43"/>
-      <c r="K41" s="44"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="52"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="53"/>
       <c r="Q41" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="R41" s="57"/>
+      <c r="R41" s="47"/>
       <c r="S41" s="4">
         <v>1.4</v>
       </c>
       <c r="T41" s="32"/>
-      <c r="U41" s="57"/>
+      <c r="U41" s="47"/>
       <c r="V41" s="4"/>
-      <c r="W41" s="50"/>
-      <c r="X41" s="51"/>
-      <c r="Y41" s="51"/>
-      <c r="Z41" s="51"/>
-      <c r="AA41" s="52"/>
+      <c r="W41" s="40"/>
+      <c r="X41" s="41"/>
+      <c r="Y41" s="41"/>
+      <c r="Z41" s="41"/>
+      <c r="AA41" s="42"/>
     </row>
     <row r="42" spans="1:27">
       <c r="A42" s="35" t="s">
@@ -2705,26 +2711,26 @@
       <c r="D42" s="35"/>
       <c r="E42" s="36"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="43"/>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
-      <c r="K42" s="44"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="52"/>
+      <c r="I42" s="52"/>
+      <c r="J42" s="52"/>
+      <c r="K42" s="53"/>
       <c r="Q42" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="R42" s="57"/>
+      <c r="R42" s="47"/>
       <c r="S42" s="2">
         <v>0.4</v>
       </c>
       <c r="T42" s="32"/>
-      <c r="U42" s="57"/>
+      <c r="U42" s="47"/>
       <c r="V42" s="2"/>
-      <c r="W42" s="53"/>
-      <c r="X42" s="54"/>
-      <c r="Y42" s="54"/>
-      <c r="Z42" s="54"/>
-      <c r="AA42" s="55"/>
+      <c r="W42" s="43"/>
+      <c r="X42" s="44"/>
+      <c r="Y42" s="44"/>
+      <c r="Z42" s="44"/>
+      <c r="AA42" s="45"/>
     </row>
     <row r="43" spans="1:27" ht="18.75">
       <c r="A43" s="10" t="s">
@@ -2833,13 +2839,13 @@
       <c r="F47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G47" s="39" t="s">
+      <c r="G47" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="H47" s="40"/>
-      <c r="I47" s="40"/>
-      <c r="J47" s="40"/>
-      <c r="K47" s="41"/>
+      <c r="H47" s="49"/>
+      <c r="I47" s="49"/>
+      <c r="J47" s="49"/>
+      <c r="K47" s="50"/>
       <c r="Q47" s="22" t="s">
         <v>6</v>
       </c>
@@ -2877,11 +2883,11 @@
       <c r="F48" s="4">
         <v>0.2</v>
       </c>
-      <c r="G48" s="42"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="43"/>
-      <c r="J48" s="43"/>
-      <c r="K48" s="44"/>
+      <c r="G48" s="51"/>
+      <c r="H48" s="52"/>
+      <c r="I48" s="52"/>
+      <c r="J48" s="52"/>
+      <c r="K48" s="53"/>
       <c r="Q48" s="30" t="s">
         <v>0</v>
       </c>
@@ -2917,11 +2923,11 @@
       <c r="F49" s="4">
         <v>0.6</v>
       </c>
-      <c r="G49" s="42"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
-      <c r="J49" s="43"/>
-      <c r="K49" s="44"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="52"/>
+      <c r="I49" s="52"/>
+      <c r="J49" s="52"/>
+      <c r="K49" s="53"/>
       <c r="Q49" s="32" t="s">
         <v>1</v>
       </c>
@@ -2957,11 +2963,11 @@
       <c r="F50" s="3">
         <v>1.5</v>
       </c>
-      <c r="G50" s="42"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="43"/>
-      <c r="J50" s="43"/>
-      <c r="K50" s="44"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="52"/>
+      <c r="I50" s="52"/>
+      <c r="J50" s="52"/>
+      <c r="K50" s="53"/>
       <c r="Q50" s="33" t="s">
         <v>2</v>
       </c>
@@ -2997,11 +3003,11 @@
       <c r="F51" s="4">
         <v>2</v>
       </c>
-      <c r="G51" s="42"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="43"/>
-      <c r="J51" s="43"/>
-      <c r="K51" s="44"/>
+      <c r="G51" s="51"/>
+      <c r="H51" s="52"/>
+      <c r="I51" s="52"/>
+      <c r="J51" s="52"/>
+      <c r="K51" s="53"/>
       <c r="Q51" s="32" t="s">
         <v>3</v>
       </c>
@@ -3033,11 +3039,11 @@
       <c r="D52" s="32"/>
       <c r="E52" s="31"/>
       <c r="F52" s="4"/>
-      <c r="G52" s="42"/>
-      <c r="H52" s="43"/>
-      <c r="I52" s="43"/>
-      <c r="J52" s="43"/>
-      <c r="K52" s="44"/>
+      <c r="G52" s="51"/>
+      <c r="H52" s="52"/>
+      <c r="I52" s="52"/>
+      <c r="J52" s="52"/>
+      <c r="K52" s="53"/>
       <c r="Q52" s="32" t="s">
         <v>4</v>
       </c>
@@ -3065,11 +3071,11 @@
       <c r="D53" s="35"/>
       <c r="E53" s="36"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="42"/>
-      <c r="H53" s="43"/>
-      <c r="I53" s="43"/>
-      <c r="J53" s="43"/>
-      <c r="K53" s="44"/>
+      <c r="G53" s="51"/>
+      <c r="H53" s="52"/>
+      <c r="I53" s="52"/>
+      <c r="J53" s="52"/>
+      <c r="K53" s="53"/>
       <c r="Q53" s="35" t="s">
         <v>7</v>
       </c>
@@ -3231,13 +3237,13 @@
       <c r="F59" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G59" s="39" t="s">
+      <c r="G59" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="H59" s="40"/>
-      <c r="I59" s="40"/>
-      <c r="J59" s="40"/>
-      <c r="K59" s="41"/>
+      <c r="H59" s="49"/>
+      <c r="I59" s="49"/>
+      <c r="J59" s="49"/>
+      <c r="K59" s="50"/>
       <c r="Q59" s="30" t="s">
         <v>0</v>
       </c>
@@ -3273,11 +3279,11 @@
       <c r="F60" s="4">
         <v>0.2</v>
       </c>
-      <c r="G60" s="42"/>
-      <c r="H60" s="43"/>
-      <c r="I60" s="43"/>
-      <c r="J60" s="43"/>
-      <c r="K60" s="44"/>
+      <c r="G60" s="51"/>
+      <c r="H60" s="52"/>
+      <c r="I60" s="52"/>
+      <c r="J60" s="52"/>
+      <c r="K60" s="53"/>
       <c r="Q60" s="32" t="s">
         <v>1</v>
       </c>
@@ -3313,11 +3319,11 @@
       <c r="F61" s="4">
         <v>0.6</v>
       </c>
-      <c r="G61" s="42"/>
-      <c r="H61" s="43"/>
-      <c r="I61" s="43"/>
-      <c r="J61" s="43"/>
-      <c r="K61" s="44"/>
+      <c r="G61" s="51"/>
+      <c r="H61" s="52"/>
+      <c r="I61" s="52"/>
+      <c r="J61" s="52"/>
+      <c r="K61" s="53"/>
       <c r="Q61" s="33" t="s">
         <v>2</v>
       </c>
@@ -3353,11 +3359,11 @@
       <c r="F62" s="3">
         <v>1.5</v>
       </c>
-      <c r="G62" s="42"/>
-      <c r="H62" s="43"/>
-      <c r="I62" s="43"/>
-      <c r="J62" s="43"/>
-      <c r="K62" s="44"/>
+      <c r="G62" s="51"/>
+      <c r="H62" s="52"/>
+      <c r="I62" s="52"/>
+      <c r="J62" s="52"/>
+      <c r="K62" s="53"/>
       <c r="Q62" s="32" t="s">
         <v>3</v>
       </c>
@@ -3393,11 +3399,11 @@
       <c r="F63" s="4">
         <v>2</v>
       </c>
-      <c r="G63" s="42"/>
-      <c r="H63" s="43"/>
-      <c r="I63" s="43"/>
-      <c r="J63" s="43"/>
-      <c r="K63" s="44"/>
+      <c r="G63" s="51"/>
+      <c r="H63" s="52"/>
+      <c r="I63" s="52"/>
+      <c r="J63" s="52"/>
+      <c r="K63" s="53"/>
       <c r="Q63" s="32" t="s">
         <v>4</v>
       </c>
@@ -3429,11 +3435,11 @@
       <c r="D64" s="32"/>
       <c r="E64" s="31"/>
       <c r="F64" s="4"/>
-      <c r="G64" s="42"/>
-      <c r="H64" s="43"/>
-      <c r="I64" s="43"/>
-      <c r="J64" s="43"/>
-      <c r="K64" s="44"/>
+      <c r="G64" s="51"/>
+      <c r="H64" s="52"/>
+      <c r="I64" s="52"/>
+      <c r="J64" s="52"/>
+      <c r="K64" s="53"/>
       <c r="Q64" s="35" t="s">
         <v>7</v>
       </c>
@@ -3461,11 +3467,11 @@
       <c r="D65" s="35"/>
       <c r="E65" s="36"/>
       <c r="F65" s="2"/>
-      <c r="G65" s="42"/>
-      <c r="H65" s="43"/>
-      <c r="I65" s="43"/>
-      <c r="J65" s="43"/>
-      <c r="K65" s="44"/>
+      <c r="G65" s="51"/>
+      <c r="H65" s="52"/>
+      <c r="I65" s="52"/>
+      <c r="J65" s="52"/>
+      <c r="K65" s="53"/>
       <c r="Q65" s="10" t="s">
         <v>38</v>
       </c>
@@ -3597,11 +3603,11 @@
       <c r="F70" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G70" s="39"/>
-      <c r="H70" s="40"/>
-      <c r="I70" s="40"/>
-      <c r="J70" s="40"/>
-      <c r="K70" s="41"/>
+      <c r="G70" s="55"/>
+      <c r="H70" s="49"/>
+      <c r="I70" s="49"/>
+      <c r="J70" s="49"/>
+      <c r="K70" s="50"/>
       <c r="Q70" s="30" t="s">
         <v>0</v>
       </c>
@@ -3637,11 +3643,11 @@
       <c r="F71" s="4">
         <v>0.2</v>
       </c>
-      <c r="G71" s="42"/>
-      <c r="H71" s="43"/>
-      <c r="I71" s="43"/>
-      <c r="J71" s="43"/>
-      <c r="K71" s="44"/>
+      <c r="G71" s="51"/>
+      <c r="H71" s="52"/>
+      <c r="I71" s="52"/>
+      <c r="J71" s="52"/>
+      <c r="K71" s="53"/>
       <c r="Q71" s="32" t="s">
         <v>1</v>
       </c>
@@ -3677,11 +3683,11 @@
       <c r="F72" s="4">
         <v>0.6</v>
       </c>
-      <c r="G72" s="42"/>
-      <c r="H72" s="43"/>
-      <c r="I72" s="43"/>
-      <c r="J72" s="43"/>
-      <c r="K72" s="44"/>
+      <c r="G72" s="51"/>
+      <c r="H72" s="52"/>
+      <c r="I72" s="52"/>
+      <c r="J72" s="52"/>
+      <c r="K72" s="53"/>
       <c r="Q72" s="33" t="s">
         <v>2</v>
       </c>
@@ -3717,11 +3723,11 @@
       <c r="F73" s="3">
         <v>1.5</v>
       </c>
-      <c r="G73" s="42"/>
-      <c r="H73" s="43"/>
-      <c r="I73" s="43"/>
-      <c r="J73" s="43"/>
-      <c r="K73" s="44"/>
+      <c r="G73" s="51"/>
+      <c r="H73" s="52"/>
+      <c r="I73" s="52"/>
+      <c r="J73" s="52"/>
+      <c r="K73" s="53"/>
       <c r="Q73" s="32" t="s">
         <v>3</v>
       </c>
@@ -3757,11 +3763,11 @@
       <c r="F74" s="4">
         <v>2</v>
       </c>
-      <c r="G74" s="42"/>
-      <c r="H74" s="43"/>
-      <c r="I74" s="43"/>
-      <c r="J74" s="43"/>
-      <c r="K74" s="44"/>
+      <c r="G74" s="51"/>
+      <c r="H74" s="52"/>
+      <c r="I74" s="52"/>
+      <c r="J74" s="52"/>
+      <c r="K74" s="53"/>
       <c r="Q74" s="32" t="s">
         <v>4</v>
       </c>
@@ -3793,11 +3799,11 @@
       <c r="D75" s="32"/>
       <c r="E75" s="31"/>
       <c r="F75" s="4"/>
-      <c r="G75" s="42"/>
-      <c r="H75" s="43"/>
-      <c r="I75" s="43"/>
-      <c r="J75" s="43"/>
-      <c r="K75" s="44"/>
+      <c r="G75" s="51"/>
+      <c r="H75" s="52"/>
+      <c r="I75" s="52"/>
+      <c r="J75" s="52"/>
+      <c r="K75" s="53"/>
       <c r="Q75" s="35" t="s">
         <v>7</v>
       </c>
@@ -3825,11 +3831,11 @@
       <c r="D76" s="35"/>
       <c r="E76" s="36"/>
       <c r="F76" s="2"/>
-      <c r="G76" s="42"/>
-      <c r="H76" s="43"/>
-      <c r="I76" s="43"/>
-      <c r="J76" s="43"/>
-      <c r="K76" s="44"/>
+      <c r="G76" s="51"/>
+      <c r="H76" s="52"/>
+      <c r="I76" s="52"/>
+      <c r="J76" s="52"/>
+      <c r="K76" s="53"/>
       <c r="Q76" s="10" t="s">
         <v>27</v>
       </c>
@@ -3859,6 +3865,21 @@
       <c r="J77" s="11"/>
       <c r="K77" s="12"/>
     </row>
+    <row r="78" spans="1:27" ht="21">
+      <c r="Q78" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="R78" s="14"/>
+      <c r="S78" s="14"/>
+      <c r="T78" s="14"/>
+      <c r="U78" s="14"/>
+      <c r="V78" s="14"/>
+      <c r="W78" s="14"/>
+      <c r="X78" s="14"/>
+      <c r="Y78" s="14"/>
+      <c r="Z78" s="14"/>
+      <c r="AA78" s="15"/>
+    </row>
     <row r="79" spans="1:27" ht="21">
       <c r="A79" s="13" t="s">
         <v>30</v>
@@ -3873,6 +3894,23 @@
       <c r="I79" s="14"/>
       <c r="J79" s="14"/>
       <c r="K79" s="15"/>
+      <c r="Q79" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="R79" s="17"/>
+      <c r="S79" s="18"/>
+      <c r="T79" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="U79" s="17"/>
+      <c r="V79" s="18"/>
+      <c r="W79" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="X79" s="20"/>
+      <c r="Y79" s="20"/>
+      <c r="Z79" s="20"/>
+      <c r="AA79" s="21"/>
     </row>
     <row r="80" spans="1:27">
       <c r="A80" s="16" t="s">
@@ -3892,8 +3930,29 @@
       <c r="I80" s="17"/>
       <c r="J80" s="17"/>
       <c r="K80" s="18"/>
-    </row>
-    <row r="81" spans="1:11">
+      <c r="Q80" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="R80" s="23"/>
+      <c r="S80" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T80" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="U80" s="23"/>
+      <c r="V80" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="W80" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="X80" s="25"/>
+      <c r="Y80" s="25"/>
+      <c r="Z80" s="25"/>
+      <c r="AA80" s="26"/>
+    </row>
+    <row r="81" spans="1:27">
       <c r="A81" s="22" t="s">
         <v>6</v>
       </c>
@@ -3908,15 +3967,34 @@
       <c r="F81" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G81" s="39" t="s">
+      <c r="G81" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="H81" s="40"/>
-      <c r="I81" s="40"/>
-      <c r="J81" s="40"/>
-      <c r="K81" s="41"/>
-    </row>
-    <row r="82" spans="1:11">
+      <c r="H81" s="49"/>
+      <c r="I81" s="49"/>
+      <c r="J81" s="49"/>
+      <c r="K81" s="50"/>
+      <c r="Q81" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="R81" s="31"/>
+      <c r="S81" s="4">
+        <v>0</v>
+      </c>
+      <c r="T81" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="U81" s="31"/>
+      <c r="V81" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W81" s="27"/>
+      <c r="X81" s="28"/>
+      <c r="Y81" s="28"/>
+      <c r="Z81" s="28"/>
+      <c r="AA81" s="29"/>
+    </row>
+    <row r="82" spans="1:27">
       <c r="A82" s="30" t="s">
         <v>0</v>
       </c>
@@ -3931,13 +4009,32 @@
       <c r="F82" s="4">
         <v>0.2</v>
       </c>
-      <c r="G82" s="42"/>
-      <c r="H82" s="43"/>
-      <c r="I82" s="43"/>
-      <c r="J82" s="43"/>
-      <c r="K82" s="44"/>
-    </row>
-    <row r="83" spans="1:11">
+      <c r="G82" s="51"/>
+      <c r="H82" s="52"/>
+      <c r="I82" s="52"/>
+      <c r="J82" s="52"/>
+      <c r="K82" s="53"/>
+      <c r="Q82" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="R82" s="31"/>
+      <c r="S82" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="T82" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="U82" s="31"/>
+      <c r="V82" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="W82" s="27"/>
+      <c r="X82" s="28"/>
+      <c r="Y82" s="28"/>
+      <c r="Z82" s="28"/>
+      <c r="AA82" s="29"/>
+    </row>
+    <row r="83" spans="1:27">
       <c r="A83" s="32" t="s">
         <v>1</v>
       </c>
@@ -3952,13 +4049,32 @@
       <c r="F83" s="4">
         <v>0.6</v>
       </c>
-      <c r="G83" s="42"/>
-      <c r="H83" s="43"/>
-      <c r="I83" s="43"/>
-      <c r="J83" s="43"/>
-      <c r="K83" s="44"/>
-    </row>
-    <row r="84" spans="1:11">
+      <c r="G83" s="51"/>
+      <c r="H83" s="52"/>
+      <c r="I83" s="52"/>
+      <c r="J83" s="52"/>
+      <c r="K83" s="53"/>
+      <c r="Q83" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="R83" s="34"/>
+      <c r="S83" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="T83" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="U83" s="34"/>
+      <c r="V83" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="W83" s="27"/>
+      <c r="X83" s="28"/>
+      <c r="Y83" s="28"/>
+      <c r="Z83" s="28"/>
+      <c r="AA83" s="29"/>
+    </row>
+    <row r="84" spans="1:27">
       <c r="A84" s="33" t="s">
         <v>2</v>
       </c>
@@ -3973,13 +4089,32 @@
       <c r="F84" s="3">
         <v>1.5</v>
       </c>
-      <c r="G84" s="42"/>
-      <c r="H84" s="43"/>
-      <c r="I84" s="43"/>
-      <c r="J84" s="43"/>
-      <c r="K84" s="44"/>
-    </row>
-    <row r="85" spans="1:11">
+      <c r="G84" s="51"/>
+      <c r="H84" s="52"/>
+      <c r="I84" s="52"/>
+      <c r="J84" s="52"/>
+      <c r="K84" s="53"/>
+      <c r="Q84" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="R84" s="31"/>
+      <c r="S84" s="4">
+        <v>0</v>
+      </c>
+      <c r="T84" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="U84" s="31"/>
+      <c r="V84" s="4">
+        <v>2</v>
+      </c>
+      <c r="W84" s="27"/>
+      <c r="X84" s="28"/>
+      <c r="Y84" s="28"/>
+      <c r="Z84" s="28"/>
+      <c r="AA84" s="29"/>
+    </row>
+    <row r="85" spans="1:27">
       <c r="A85" s="32" t="s">
         <v>3</v>
       </c>
@@ -3994,13 +4129,32 @@
       <c r="F85" s="4">
         <v>2</v>
       </c>
-      <c r="G85" s="42"/>
-      <c r="H85" s="43"/>
-      <c r="I85" s="43"/>
-      <c r="J85" s="43"/>
-      <c r="K85" s="44"/>
-    </row>
-    <row r="86" spans="1:11">
+      <c r="G85" s="51"/>
+      <c r="H85" s="52"/>
+      <c r="I85" s="52"/>
+      <c r="J85" s="52"/>
+      <c r="K85" s="53"/>
+      <c r="Q85" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="R85" s="31"/>
+      <c r="S85" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="T85" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="U85" s="31"/>
+      <c r="V85" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="W85" s="27"/>
+      <c r="X85" s="28"/>
+      <c r="Y85" s="28"/>
+      <c r="Z85" s="28"/>
+      <c r="AA85" s="29"/>
+    </row>
+    <row r="86" spans="1:27">
       <c r="A86" s="32" t="s">
         <v>4</v>
       </c>
@@ -4011,13 +4165,28 @@
       <c r="D86" s="32"/>
       <c r="E86" s="31"/>
       <c r="F86" s="4"/>
-      <c r="G86" s="42"/>
-      <c r="H86" s="43"/>
-      <c r="I86" s="43"/>
-      <c r="J86" s="43"/>
-      <c r="K86" s="44"/>
-    </row>
-    <row r="87" spans="1:11">
+      <c r="G86" s="51"/>
+      <c r="H86" s="52"/>
+      <c r="I86" s="52"/>
+      <c r="J86" s="52"/>
+      <c r="K86" s="53"/>
+      <c r="Q86" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="R86" s="36"/>
+      <c r="S86" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="T86" s="35"/>
+      <c r="U86" s="36"/>
+      <c r="V86" s="2"/>
+      <c r="W86" s="27"/>
+      <c r="X86" s="28"/>
+      <c r="Y86" s="28"/>
+      <c r="Z86" s="28"/>
+      <c r="AA86" s="29"/>
+    </row>
+    <row r="87" spans="1:27" ht="18.75">
       <c r="A87" s="35" t="s">
         <v>7</v>
       </c>
@@ -4028,13 +4197,26 @@
       <c r="D87" s="35"/>
       <c r="E87" s="36"/>
       <c r="F87" s="2"/>
-      <c r="G87" s="42"/>
-      <c r="H87" s="43"/>
-      <c r="I87" s="43"/>
-      <c r="J87" s="43"/>
-      <c r="K87" s="44"/>
-    </row>
-    <row r="88" spans="1:11" ht="18.75">
+      <c r="G87" s="51"/>
+      <c r="H87" s="52"/>
+      <c r="I87" s="52"/>
+      <c r="J87" s="52"/>
+      <c r="K87" s="53"/>
+      <c r="Q87" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="R87" s="11"/>
+      <c r="S87" s="11"/>
+      <c r="T87" s="11"/>
+      <c r="U87" s="11"/>
+      <c r="V87" s="11"/>
+      <c r="W87" s="11"/>
+      <c r="X87" s="11"/>
+      <c r="Y87" s="11"/>
+      <c r="Z87" s="11"/>
+      <c r="AA87" s="12"/>
+    </row>
+    <row r="88" spans="1:27" ht="18.75">
       <c r="A88" s="10" t="s">
         <v>32</v>
       </c>
@@ -4049,7 +4231,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="12"/>
     </row>
-    <row r="90" spans="1:11" ht="21">
+    <row r="90" spans="1:27" ht="21">
       <c r="A90" s="13" t="s">
         <v>34</v>
       </c>
@@ -4064,7 +4246,7 @@
       <c r="J90" s="14"/>
       <c r="K90" s="15"/>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:27">
       <c r="A91" s="16" t="s">
         <v>11</v>
       </c>
@@ -4083,7 +4265,7 @@
       <c r="J91" s="17"/>
       <c r="K91" s="18"/>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:27">
       <c r="A92" s="22" t="s">
         <v>6</v>
       </c>
@@ -4098,15 +4280,15 @@
       <c r="F92" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G92" s="45" t="s">
+      <c r="G92" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="H92" s="40"/>
-      <c r="I92" s="40"/>
-      <c r="J92" s="40"/>
-      <c r="K92" s="41"/>
-    </row>
-    <row r="93" spans="1:11">
+      <c r="H92" s="49"/>
+      <c r="I92" s="49"/>
+      <c r="J92" s="49"/>
+      <c r="K92" s="50"/>
+    </row>
+    <row r="93" spans="1:27">
       <c r="A93" s="30" t="s">
         <v>0</v>
       </c>
@@ -4121,13 +4303,13 @@
       <c r="F93" s="4">
         <v>0.2</v>
       </c>
-      <c r="G93" s="42"/>
-      <c r="H93" s="43"/>
-      <c r="I93" s="43"/>
-      <c r="J93" s="43"/>
-      <c r="K93" s="44"/>
-    </row>
-    <row r="94" spans="1:11">
+      <c r="G93" s="51"/>
+      <c r="H93" s="52"/>
+      <c r="I93" s="52"/>
+      <c r="J93" s="52"/>
+      <c r="K93" s="53"/>
+    </row>
+    <row r="94" spans="1:27">
       <c r="A94" s="32" t="s">
         <v>1</v>
       </c>
@@ -4142,13 +4324,13 @@
       <c r="F94" s="4">
         <v>0.6</v>
       </c>
-      <c r="G94" s="42"/>
-      <c r="H94" s="43"/>
-      <c r="I94" s="43"/>
-      <c r="J94" s="43"/>
-      <c r="K94" s="44"/>
-    </row>
-    <row r="95" spans="1:11">
+      <c r="G94" s="51"/>
+      <c r="H94" s="52"/>
+      <c r="I94" s="52"/>
+      <c r="J94" s="52"/>
+      <c r="K94" s="53"/>
+    </row>
+    <row r="95" spans="1:27">
       <c r="A95" s="33" t="s">
         <v>2</v>
       </c>
@@ -4163,13 +4345,13 @@
       <c r="F95" s="3">
         <v>1.5</v>
       </c>
-      <c r="G95" s="42"/>
-      <c r="H95" s="43"/>
-      <c r="I95" s="43"/>
-      <c r="J95" s="43"/>
-      <c r="K95" s="44"/>
-    </row>
-    <row r="96" spans="1:11">
+      <c r="G95" s="51"/>
+      <c r="H95" s="52"/>
+      <c r="I95" s="52"/>
+      <c r="J95" s="52"/>
+      <c r="K95" s="53"/>
+    </row>
+    <row r="96" spans="1:27">
       <c r="A96" s="32" t="s">
         <v>3</v>
       </c>
@@ -4184,11 +4366,11 @@
       <c r="F96" s="4">
         <v>2</v>
       </c>
-      <c r="G96" s="42"/>
-      <c r="H96" s="43"/>
-      <c r="I96" s="43"/>
-      <c r="J96" s="43"/>
-      <c r="K96" s="44"/>
+      <c r="G96" s="51"/>
+      <c r="H96" s="52"/>
+      <c r="I96" s="52"/>
+      <c r="J96" s="52"/>
+      <c r="K96" s="53"/>
     </row>
     <row r="97" spans="1:11">
       <c r="A97" s="32" t="s">
@@ -4201,11 +4383,11 @@
       <c r="D97" s="32"/>
       <c r="E97" s="31"/>
       <c r="F97" s="4"/>
-      <c r="G97" s="42"/>
-      <c r="H97" s="43"/>
-      <c r="I97" s="43"/>
-      <c r="J97" s="43"/>
-      <c r="K97" s="44"/>
+      <c r="G97" s="51"/>
+      <c r="H97" s="52"/>
+      <c r="I97" s="52"/>
+      <c r="J97" s="52"/>
+      <c r="K97" s="53"/>
     </row>
     <row r="98" spans="1:11">
       <c r="A98" s="35" t="s">
@@ -4218,11 +4400,11 @@
       <c r="D98" s="35"/>
       <c r="E98" s="36"/>
       <c r="F98" s="2"/>
-      <c r="G98" s="42"/>
-      <c r="H98" s="43"/>
-      <c r="I98" s="43"/>
-      <c r="J98" s="43"/>
-      <c r="K98" s="44"/>
+      <c r="G98" s="51"/>
+      <c r="H98" s="52"/>
+      <c r="I98" s="52"/>
+      <c r="J98" s="52"/>
+      <c r="K98" s="53"/>
     </row>
     <row r="99" spans="1:11" ht="18.75">
       <c r="A99" s="10" t="s">
@@ -4288,13 +4470,13 @@
       <c r="F105" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G105" s="46" t="s">
+      <c r="G105" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="H105" s="40"/>
-      <c r="I105" s="40"/>
-      <c r="J105" s="40"/>
-      <c r="K105" s="41"/>
+      <c r="H105" s="49"/>
+      <c r="I105" s="49"/>
+      <c r="J105" s="49"/>
+      <c r="K105" s="50"/>
     </row>
     <row r="106" spans="1:11">
       <c r="A106" s="30" t="s">
@@ -4311,11 +4493,11 @@
       <c r="F106" s="4">
         <v>0.2</v>
       </c>
-      <c r="G106" s="42"/>
-      <c r="H106" s="43"/>
-      <c r="I106" s="43"/>
-      <c r="J106" s="43"/>
-      <c r="K106" s="44"/>
+      <c r="G106" s="51"/>
+      <c r="H106" s="52"/>
+      <c r="I106" s="52"/>
+      <c r="J106" s="52"/>
+      <c r="K106" s="53"/>
     </row>
     <row r="107" spans="1:11">
       <c r="A107" s="32" t="s">
@@ -4332,11 +4514,11 @@
       <c r="F107" s="4">
         <v>0.6</v>
       </c>
-      <c r="G107" s="42"/>
-      <c r="H107" s="43"/>
-      <c r="I107" s="43"/>
-      <c r="J107" s="43"/>
-      <c r="K107" s="44"/>
+      <c r="G107" s="51"/>
+      <c r="H107" s="52"/>
+      <c r="I107" s="52"/>
+      <c r="J107" s="52"/>
+      <c r="K107" s="53"/>
     </row>
     <row r="108" spans="1:11">
       <c r="A108" s="33" t="s">
@@ -4353,11 +4535,11 @@
       <c r="F108" s="3">
         <v>1.5</v>
       </c>
-      <c r="G108" s="42"/>
-      <c r="H108" s="43"/>
-      <c r="I108" s="43"/>
-      <c r="J108" s="43"/>
-      <c r="K108" s="44"/>
+      <c r="G108" s="51"/>
+      <c r="H108" s="52"/>
+      <c r="I108" s="52"/>
+      <c r="J108" s="52"/>
+      <c r="K108" s="53"/>
     </row>
     <row r="109" spans="1:11">
       <c r="A109" s="32" t="s">
@@ -4374,11 +4556,11 @@
       <c r="F109" s="4">
         <v>2</v>
       </c>
-      <c r="G109" s="42"/>
-      <c r="H109" s="43"/>
-      <c r="I109" s="43"/>
-      <c r="J109" s="43"/>
-      <c r="K109" s="44"/>
+      <c r="G109" s="51"/>
+      <c r="H109" s="52"/>
+      <c r="I109" s="52"/>
+      <c r="J109" s="52"/>
+      <c r="K109" s="53"/>
     </row>
     <row r="110" spans="1:11">
       <c r="A110" s="32" t="s">
@@ -4391,11 +4573,11 @@
       <c r="D110" s="32"/>
       <c r="E110" s="31"/>
       <c r="F110" s="4"/>
-      <c r="G110" s="42"/>
-      <c r="H110" s="43"/>
-      <c r="I110" s="43"/>
-      <c r="J110" s="43"/>
-      <c r="K110" s="44"/>
+      <c r="G110" s="51"/>
+      <c r="H110" s="52"/>
+      <c r="I110" s="52"/>
+      <c r="J110" s="52"/>
+      <c r="K110" s="53"/>
     </row>
     <row r="111" spans="1:11">
       <c r="A111" s="35" t="s">
@@ -4408,11 +4590,11 @@
       <c r="D111" s="35"/>
       <c r="E111" s="36"/>
       <c r="F111" s="2"/>
-      <c r="G111" s="42"/>
-      <c r="H111" s="43"/>
-      <c r="I111" s="43"/>
-      <c r="J111" s="43"/>
-      <c r="K111" s="44"/>
+      <c r="G111" s="51"/>
+      <c r="H111" s="52"/>
+      <c r="I111" s="52"/>
+      <c r="J111" s="52"/>
+      <c r="K111" s="53"/>
     </row>
     <row r="112" spans="1:11" ht="18.75">
       <c r="A112" s="10" t="s">
@@ -4430,205 +4612,146 @@
       <c r="K112" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="341">
-    <mergeCell ref="Q76:AA76"/>
-    <mergeCell ref="Q67:AA67"/>
-    <mergeCell ref="Q68:S68"/>
-    <mergeCell ref="T68:V68"/>
-    <mergeCell ref="W68:AA68"/>
-    <mergeCell ref="Q69:R69"/>
-    <mergeCell ref="T69:U69"/>
-    <mergeCell ref="W69:AA75"/>
-    <mergeCell ref="Q70:R70"/>
-    <mergeCell ref="T70:U70"/>
-    <mergeCell ref="Q71:R71"/>
-    <mergeCell ref="T71:U71"/>
-    <mergeCell ref="Q72:R72"/>
-    <mergeCell ref="T72:U72"/>
-    <mergeCell ref="Q73:R73"/>
-    <mergeCell ref="T73:U73"/>
-    <mergeCell ref="Q74:R74"/>
-    <mergeCell ref="T74:U74"/>
-    <mergeCell ref="Q75:R75"/>
-    <mergeCell ref="T75:U75"/>
-    <mergeCell ref="Q56:AA56"/>
-    <mergeCell ref="Q57:S57"/>
-    <mergeCell ref="T57:V57"/>
-    <mergeCell ref="W57:AA57"/>
-    <mergeCell ref="Q58:R58"/>
-    <mergeCell ref="T58:U58"/>
-    <mergeCell ref="W58:AA64"/>
-    <mergeCell ref="Q65:AA65"/>
-    <mergeCell ref="Q59:R59"/>
-    <mergeCell ref="T59:U59"/>
-    <mergeCell ref="Q60:R60"/>
-    <mergeCell ref="T60:U60"/>
-    <mergeCell ref="Q61:R61"/>
-    <mergeCell ref="T61:U61"/>
-    <mergeCell ref="Q62:R62"/>
-    <mergeCell ref="T62:U62"/>
-    <mergeCell ref="Q63:R63"/>
-    <mergeCell ref="T63:U63"/>
-    <mergeCell ref="Q64:R64"/>
-    <mergeCell ref="T64:U64"/>
-    <mergeCell ref="Q43:AA43"/>
-    <mergeCell ref="Q32:AA32"/>
-    <mergeCell ref="Q34:AA34"/>
-    <mergeCell ref="Q35:S35"/>
-    <mergeCell ref="T35:V35"/>
-    <mergeCell ref="W35:AA35"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="T36:U36"/>
-    <mergeCell ref="W36:AA42"/>
-    <mergeCell ref="Q37:R37"/>
-    <mergeCell ref="T37:U37"/>
-    <mergeCell ref="Q38:R38"/>
-    <mergeCell ref="T38:U38"/>
-    <mergeCell ref="Q39:R39"/>
-    <mergeCell ref="T39:U39"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="T40:U40"/>
-    <mergeCell ref="Q41:R41"/>
-    <mergeCell ref="T41:U41"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="Q23:AA23"/>
-    <mergeCell ref="Q24:S24"/>
-    <mergeCell ref="T24:V24"/>
-    <mergeCell ref="W24:AA24"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="W25:AA31"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="T26:U26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="T27:U27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="T28:U28"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="T29:U29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="T31:U31"/>
-    <mergeCell ref="Q21:AA21"/>
-    <mergeCell ref="Q12:AA12"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="T13:V13"/>
-    <mergeCell ref="W13:AA13"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="W14:AA20"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="T15:U15"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="T19:U19"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="T20:U20"/>
-    <mergeCell ref="A112:K112"/>
-    <mergeCell ref="A103:K103"/>
-    <mergeCell ref="A104:C104"/>
-    <mergeCell ref="D104:F104"/>
-    <mergeCell ref="G104:K104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="G105:K111"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="A99:K99"/>
-    <mergeCell ref="A90:K90"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="G91:K91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="G92:K98"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="A88:K88"/>
-    <mergeCell ref="A79:K79"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="G80:K80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="G81:K87"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="A57:K57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="G58:K58"/>
-    <mergeCell ref="G59:K65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="A66:K66"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
+  <mergeCells count="361">
+    <mergeCell ref="Q87:AA87"/>
+    <mergeCell ref="Q78:AA78"/>
+    <mergeCell ref="Q79:S79"/>
+    <mergeCell ref="T79:V79"/>
+    <mergeCell ref="W79:AA79"/>
+    <mergeCell ref="Q80:R80"/>
+    <mergeCell ref="T80:U80"/>
+    <mergeCell ref="W80:AA86"/>
+    <mergeCell ref="Q81:R81"/>
+    <mergeCell ref="T81:U81"/>
+    <mergeCell ref="Q82:R82"/>
+    <mergeCell ref="T82:U82"/>
+    <mergeCell ref="Q83:R83"/>
+    <mergeCell ref="T83:U83"/>
+    <mergeCell ref="Q84:R84"/>
+    <mergeCell ref="T84:U84"/>
+    <mergeCell ref="Q85:R85"/>
+    <mergeCell ref="T85:U85"/>
+    <mergeCell ref="Q86:R86"/>
+    <mergeCell ref="T86:U86"/>
+    <mergeCell ref="Q54:AA54"/>
+    <mergeCell ref="Q45:AA45"/>
+    <mergeCell ref="Q46:S46"/>
+    <mergeCell ref="T46:V46"/>
+    <mergeCell ref="W46:AA46"/>
+    <mergeCell ref="Q47:R47"/>
+    <mergeCell ref="T47:U47"/>
+    <mergeCell ref="W47:AA53"/>
+    <mergeCell ref="Q48:R48"/>
+    <mergeCell ref="T48:U48"/>
+    <mergeCell ref="Q49:R49"/>
+    <mergeCell ref="T49:U49"/>
+    <mergeCell ref="Q50:R50"/>
+    <mergeCell ref="T50:U50"/>
+    <mergeCell ref="Q51:R51"/>
+    <mergeCell ref="T51:U51"/>
+    <mergeCell ref="Q52:R52"/>
+    <mergeCell ref="T52:U52"/>
+    <mergeCell ref="Q53:R53"/>
+    <mergeCell ref="T53:U53"/>
+    <mergeCell ref="Q10:AA10"/>
+    <mergeCell ref="N3:P6"/>
+    <mergeCell ref="Q1:AA1"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="W2:AA2"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="W3:AA9"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="A77:K77"/>
+    <mergeCell ref="A68:K68"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="G69:K69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="G70:K76"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="A54:K54"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="G46:K46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="G47:K53"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A45:K45"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:K42"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A32:K32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K20"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:E16"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="G3:K9"/>
@@ -4653,125 +4776,204 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A32:K32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K20"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A45:K45"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="G36:K42"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A54:K54"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="G46:K46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="G47:K53"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="A77:K77"/>
-    <mergeCell ref="A68:K68"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="G69:K69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="G70:K76"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="Q10:AA10"/>
-    <mergeCell ref="N3:P6"/>
-    <mergeCell ref="Q1:AA1"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="W2:AA2"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="W3:AA9"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="T9:U9"/>
-    <mergeCell ref="Q54:AA54"/>
-    <mergeCell ref="Q45:AA45"/>
-    <mergeCell ref="Q46:S46"/>
-    <mergeCell ref="T46:V46"/>
-    <mergeCell ref="W46:AA46"/>
-    <mergeCell ref="Q47:R47"/>
-    <mergeCell ref="T47:U47"/>
-    <mergeCell ref="W47:AA53"/>
-    <mergeCell ref="Q48:R48"/>
-    <mergeCell ref="T48:U48"/>
-    <mergeCell ref="Q49:R49"/>
-    <mergeCell ref="T49:U49"/>
-    <mergeCell ref="Q50:R50"/>
-    <mergeCell ref="T50:U50"/>
-    <mergeCell ref="Q51:R51"/>
-    <mergeCell ref="T51:U51"/>
-    <mergeCell ref="Q52:R52"/>
-    <mergeCell ref="T52:U52"/>
-    <mergeCell ref="Q53:R53"/>
-    <mergeCell ref="T53:U53"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="G58:K58"/>
+    <mergeCell ref="G59:K65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="A66:K66"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A88:K88"/>
+    <mergeCell ref="A79:K79"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="G80:K80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="G81:K87"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="A99:K99"/>
+    <mergeCell ref="A90:K90"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="G91:K91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="G92:K98"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="A112:K112"/>
+    <mergeCell ref="A103:K103"/>
+    <mergeCell ref="A104:C104"/>
+    <mergeCell ref="D104:F104"/>
+    <mergeCell ref="G104:K104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="G105:K111"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="Q21:AA21"/>
+    <mergeCell ref="Q12:AA12"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="T13:V13"/>
+    <mergeCell ref="W13:AA13"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="W14:AA20"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="T19:U19"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="T20:U20"/>
+    <mergeCell ref="Q23:AA23"/>
+    <mergeCell ref="Q24:S24"/>
+    <mergeCell ref="T24:V24"/>
+    <mergeCell ref="W24:AA24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="W25:AA31"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="T27:U27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="T28:U28"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="T29:U29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="Q43:AA43"/>
+    <mergeCell ref="Q32:AA32"/>
+    <mergeCell ref="Q34:AA34"/>
+    <mergeCell ref="Q35:S35"/>
+    <mergeCell ref="T35:V35"/>
+    <mergeCell ref="W35:AA35"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="T36:U36"/>
+    <mergeCell ref="W36:AA42"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="T37:U37"/>
+    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="T38:U38"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="T39:U39"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="T40:U40"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="T41:U41"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="Q56:AA56"/>
+    <mergeCell ref="Q57:S57"/>
+    <mergeCell ref="T57:V57"/>
+    <mergeCell ref="W57:AA57"/>
+    <mergeCell ref="Q58:R58"/>
+    <mergeCell ref="T58:U58"/>
+    <mergeCell ref="W58:AA64"/>
+    <mergeCell ref="Q65:AA65"/>
+    <mergeCell ref="Q59:R59"/>
+    <mergeCell ref="T59:U59"/>
+    <mergeCell ref="Q60:R60"/>
+    <mergeCell ref="T60:U60"/>
+    <mergeCell ref="Q61:R61"/>
+    <mergeCell ref="T61:U61"/>
+    <mergeCell ref="Q62:R62"/>
+    <mergeCell ref="T62:U62"/>
+    <mergeCell ref="Q63:R63"/>
+    <mergeCell ref="T63:U63"/>
+    <mergeCell ref="Q64:R64"/>
+    <mergeCell ref="T64:U64"/>
+    <mergeCell ref="Q76:AA76"/>
+    <mergeCell ref="Q67:AA67"/>
+    <mergeCell ref="Q68:S68"/>
+    <mergeCell ref="T68:V68"/>
+    <mergeCell ref="W68:AA68"/>
+    <mergeCell ref="Q69:R69"/>
+    <mergeCell ref="T69:U69"/>
+    <mergeCell ref="W69:AA75"/>
+    <mergeCell ref="Q70:R70"/>
+    <mergeCell ref="T70:U70"/>
+    <mergeCell ref="Q71:R71"/>
+    <mergeCell ref="T71:U71"/>
+    <mergeCell ref="Q72:R72"/>
+    <mergeCell ref="T72:U72"/>
+    <mergeCell ref="Q73:R73"/>
+    <mergeCell ref="T73:U73"/>
+    <mergeCell ref="Q74:R74"/>
+    <mergeCell ref="T74:U74"/>
+    <mergeCell ref="Q75:R75"/>
+    <mergeCell ref="T75:U75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>